<commit_message>
check-in: 20200419 zhongshuwangge update
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="7596"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7590"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="60">
   <si>
     <t>交易品种：</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -252,18 +252,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>0.974/0.990</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>pending</t>
+    <t>0.974/0.981</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0_);\(0\)"/>
   </numFmts>
@@ -377,7 +373,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -665,22 +661,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="B43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" customWidth="1"/>
-    <col min="2" max="2" width="25.109375" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" customWidth="1"/>
+    <col min="1" max="1" width="17.75" customWidth="1"/>
+    <col min="2" max="2" width="25.125" customWidth="1"/>
+    <col min="3" max="3" width="23.125" customWidth="1"/>
+    <col min="4" max="4" width="21.5" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="21.77734375" customWidth="1"/>
-    <col min="7" max="8" width="19.44140625" customWidth="1"/>
+    <col min="6" max="6" width="21.75" customWidth="1"/>
+    <col min="7" max="8" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="25.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:18" ht="25.5" x14ac:dyDescent="0.3">
       <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
@@ -694,7 +690,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
         <v>29</v>
       </c>
@@ -702,7 +698,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
         <v>10</v>
       </c>
@@ -710,7 +706,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
         <v>11</v>
       </c>
@@ -718,7 +714,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -748,7 +744,7 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
@@ -772,7 +768,7 @@
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
@@ -798,7 +794,7 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A11" s="7" t="s">
         <v>0</v>
       </c>
@@ -806,13 +802,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A12" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="8"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A13" s="7" t="s">
         <v>17</v>
       </c>
@@ -820,7 +816,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
@@ -850,7 +846,7 @@
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
         <v>40</v>
       </c>
@@ -874,7 +870,7 @@
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A16" s="4" t="s">
         <v>39</v>
       </c>
@@ -902,7 +898,7 @@
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A19" s="7" t="s">
         <v>0</v>
       </c>
@@ -910,13 +906,13 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A20" s="7" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="8"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A21" s="7" t="s">
         <v>21</v>
       </c>
@@ -924,7 +920,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>6</v>
       </c>
@@ -950,7 +946,7 @@
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A23" s="2" t="s">
         <v>41</v>
       </c>
@@ -974,7 +970,7 @@
       <c r="Q23" s="2"/>
       <c r="R23" s="2"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A24" s="4" t="s">
         <v>8</v>
       </c>
@@ -998,7 +994,7 @@
       <c r="Q24" s="4"/>
       <c r="R24" s="4"/>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A27" s="7" t="s">
         <v>0</v>
       </c>
@@ -1006,13 +1002,13 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A28" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B28" s="8"/>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A29" s="7" t="s">
         <v>17</v>
       </c>
@@ -1020,7 +1016,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
         <v>6</v>
       </c>
@@ -1050,7 +1046,7 @@
       <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A31" s="2" t="s">
         <v>42</v>
       </c>
@@ -1076,7 +1072,7 @@
       <c r="Q31" s="2"/>
       <c r="R31" s="2"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A32" s="4" t="s">
         <v>8</v>
       </c>
@@ -1102,7 +1098,7 @@
       <c r="Q32" s="4"/>
       <c r="R32" s="4"/>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A35" s="7" t="s">
         <v>0</v>
       </c>
@@ -1110,7 +1106,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A36" s="7" t="s">
         <v>16</v>
       </c>
@@ -1118,7 +1114,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A37" s="7" t="s">
         <v>17</v>
       </c>
@@ -1126,7 +1122,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
         <v>6</v>
       </c>
@@ -1156,7 +1152,7 @@
       <c r="Q38" s="1"/>
       <c r="R38" s="1"/>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A39" s="2" t="s">
         <v>43</v>
       </c>
@@ -1182,7 +1178,7 @@
       <c r="Q39" s="2"/>
       <c r="R39" s="2"/>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A40" s="4" t="s">
         <v>8</v>
       </c>
@@ -1208,7 +1204,7 @@
       <c r="Q40" s="4"/>
       <c r="R40" s="4"/>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A42" s="7" t="s">
         <v>0</v>
       </c>
@@ -1216,13 +1212,13 @@
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A43" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B43" s="8"/>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A44" s="7" t="s">
         <v>17</v>
       </c>
@@ -1230,7 +1226,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A45" s="1" t="s">
         <v>6</v>
       </c>
@@ -1260,7 +1256,7 @@
       <c r="Q45" s="1"/>
       <c r="R45" s="1"/>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A46" s="2" t="s">
         <v>44</v>
       </c>
@@ -1284,7 +1280,7 @@
       <c r="Q46" s="2"/>
       <c r="R46" s="2"/>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A47" s="4" t="s">
         <v>8</v>
       </c>
@@ -1310,7 +1306,7 @@
       <c r="Q47" s="4"/>
       <c r="R47" s="4"/>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A50" s="7" t="s">
         <v>0</v>
       </c>
@@ -1318,7 +1314,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A51" s="7" t="s">
         <v>16</v>
       </c>
@@ -1326,7 +1322,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A52" s="7" t="s">
         <v>17</v>
       </c>
@@ -1334,7 +1330,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A53" s="1" t="s">
         <v>6</v>
       </c>
@@ -1364,7 +1360,7 @@
       <c r="Q53" s="1"/>
       <c r="R53" s="1"/>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A54" s="2" t="s">
         <v>45</v>
       </c>
@@ -1390,16 +1386,14 @@
       <c r="Q54" s="2"/>
       <c r="R54" s="2"/>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A55" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B55" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C55" s="5" t="s">
-        <v>60</v>
-      </c>
+      <c r="C55" s="5"/>
       <c r="D55" s="5"/>
       <c r="E55" s="5"/>
       <c r="F55" s="5"/>
@@ -1416,7 +1410,7 @@
       <c r="Q55" s="4"/>
       <c r="R55" s="4"/>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A58" s="7" t="s">
         <v>0</v>
       </c>
@@ -1424,13 +1418,13 @@
         <v>35</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A59" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B59" s="8"/>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A60" s="7" t="s">
         <v>17</v>
       </c>
@@ -1438,7 +1432,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A61" s="1" t="s">
         <v>6</v>
       </c>
@@ -1468,7 +1462,7 @@
       <c r="Q61" s="1"/>
       <c r="R61" s="1"/>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A62" s="2" t="s">
         <v>46</v>
       </c>
@@ -1494,7 +1488,7 @@
       <c r="Q62" s="2"/>
       <c r="R62" s="2"/>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A63" s="4" t="s">
         <v>8</v>
       </c>
@@ -1520,7 +1514,7 @@
       <c r="Q63" s="4"/>
       <c r="R63" s="4"/>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A66" s="7" t="s">
         <v>0</v>
       </c>
@@ -1528,7 +1522,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A67" s="7" t="s">
         <v>16</v>
       </c>
@@ -1536,7 +1530,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A68" s="7" t="s">
         <v>17</v>
       </c>
@@ -1544,7 +1538,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A69" s="1" t="s">
         <v>6</v>
       </c>
@@ -1574,7 +1568,7 @@
       <c r="Q69" s="1"/>
       <c r="R69" s="1"/>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A70" s="2" t="s">
         <v>45</v>
       </c>
@@ -1598,7 +1592,7 @@
       <c r="Q70" s="2"/>
       <c r="R70" s="2"/>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A71" s="4" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
check-in: 20200420 zhongshuwangge update
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="62">
   <si>
     <t>交易品种：</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -253,6 +253,10 @@
   </si>
   <si>
     <t>0.974/0.990</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pending</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -666,7 +670,7 @@
   <dimension ref="A1:R71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -755,7 +759,9 @@
       <c r="B7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="9"/>
+      <c r="C7" s="9">
+        <v>1</v>
+      </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -981,7 +987,9 @@
       <c r="B24" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="10"/>
+      <c r="C24" s="10">
+        <v>1</v>
+      </c>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
@@ -1291,8 +1299,8 @@
       <c r="B47" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C47" s="10">
-        <v>1</v>
+      <c r="C47" s="10" t="s">
+        <v>61</v>
       </c>
       <c r="D47" s="5"/>
       <c r="E47" s="5"/>

</xml_diff>

<commit_message>
check-in: 20240422 zhongshu_wangge.xlsx update
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="7596"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7590"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="65">
   <si>
     <t>交易品种：</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -264,14 +264,22 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>pending</t>
+    <t>众兴转债（128026）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100.28/101.87</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>93.503/99.117</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0_);\(0\)"/>
   </numFmts>
@@ -393,7 +401,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -679,24 +687,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R71"/>
+  <dimension ref="A1:R77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView tabSelected="1" topLeftCell="B49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F64" sqref="F64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" customWidth="1"/>
-    <col min="2" max="2" width="25.109375" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" customWidth="1"/>
+    <col min="1" max="1" width="17.75" customWidth="1"/>
+    <col min="2" max="2" width="25.125" customWidth="1"/>
+    <col min="3" max="3" width="23.125" customWidth="1"/>
+    <col min="4" max="4" width="21.5" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="21.77734375" customWidth="1"/>
-    <col min="7" max="8" width="19.44140625" customWidth="1"/>
+    <col min="6" max="6" width="21.75" customWidth="1"/>
+    <col min="7" max="8" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="25.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:18" ht="25.5" x14ac:dyDescent="0.3">
       <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
@@ -710,7 +718,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
         <v>29</v>
       </c>
@@ -718,7 +726,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
         <v>10</v>
       </c>
@@ -726,7 +734,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
         <v>11</v>
       </c>
@@ -734,7 +742,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -764,7 +772,7 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
@@ -790,7 +798,7 @@
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
@@ -816,7 +824,7 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A11" s="7" t="s">
         <v>0</v>
       </c>
@@ -824,13 +832,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A12" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="8"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A13" s="7" t="s">
         <v>17</v>
       </c>
@@ -838,7 +846,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
@@ -868,7 +876,7 @@
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
         <v>40</v>
       </c>
@@ -892,7 +900,7 @@
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A16" s="4" t="s">
         <v>39</v>
       </c>
@@ -920,7 +928,7 @@
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A19" s="7" t="s">
         <v>0</v>
       </c>
@@ -928,13 +936,13 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A20" s="7" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="8"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A21" s="7" t="s">
         <v>21</v>
       </c>
@@ -942,7 +950,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>6</v>
       </c>
@@ -968,7 +976,7 @@
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A23" s="2" t="s">
         <v>41</v>
       </c>
@@ -992,7 +1000,7 @@
       <c r="Q23" s="2"/>
       <c r="R23" s="2"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A24" s="4" t="s">
         <v>8</v>
       </c>
@@ -1018,7 +1026,7 @@
       <c r="Q24" s="4"/>
       <c r="R24" s="4"/>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A27" s="7" t="s">
         <v>0</v>
       </c>
@@ -1026,13 +1034,13 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A28" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B28" s="8"/>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A29" s="7" t="s">
         <v>17</v>
       </c>
@@ -1040,7 +1048,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
         <v>6</v>
       </c>
@@ -1070,7 +1078,7 @@
       <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A31" s="2" t="s">
         <v>42</v>
       </c>
@@ -1096,7 +1104,7 @@
       <c r="Q31" s="2"/>
       <c r="R31" s="2"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A32" s="4" t="s">
         <v>8</v>
       </c>
@@ -1122,7 +1130,7 @@
       <c r="Q32" s="4"/>
       <c r="R32" s="4"/>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A35" s="7" t="s">
         <v>0</v>
       </c>
@@ -1130,7 +1138,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A36" s="7" t="s">
         <v>16</v>
       </c>
@@ -1138,7 +1146,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A37" s="7" t="s">
         <v>17</v>
       </c>
@@ -1146,7 +1154,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
         <v>6</v>
       </c>
@@ -1176,7 +1184,7 @@
       <c r="Q38" s="1"/>
       <c r="R38" s="1"/>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A39" s="2" t="s">
         <v>43</v>
       </c>
@@ -1202,7 +1210,7 @@
       <c r="Q39" s="2"/>
       <c r="R39" s="2"/>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A40" s="4" t="s">
         <v>8</v>
       </c>
@@ -1228,7 +1236,7 @@
       <c r="Q40" s="4"/>
       <c r="R40" s="4"/>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A42" s="7" t="s">
         <v>0</v>
       </c>
@@ -1236,13 +1244,13 @@
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A43" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B43" s="8"/>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A44" s="7" t="s">
         <v>17</v>
       </c>
@@ -1250,7 +1258,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A45" s="1" t="s">
         <v>6</v>
       </c>
@@ -1280,14 +1288,16 @@
       <c r="Q45" s="1"/>
       <c r="R45" s="1"/>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A46" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C46" s="3"/>
+      <c r="C46" s="11">
+        <v>1</v>
+      </c>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
@@ -1304,16 +1314,14 @@
       <c r="Q46" s="2"/>
       <c r="R46" s="2"/>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A47" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C47" s="10" t="s">
-        <v>60</v>
-      </c>
+      <c r="C47" s="10"/>
       <c r="D47" s="5"/>
       <c r="E47" s="5"/>
       <c r="F47" s="5"/>
@@ -1330,317 +1338,419 @@
       <c r="Q47" s="4"/>
       <c r="R47" s="4"/>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A49" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A50" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B50" s="8"/>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A51" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A52" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1"/>
+      <c r="I52" s="1"/>
+      <c r="J52" s="1"/>
+      <c r="K52" s="1"/>
+      <c r="L52" s="1"/>
+      <c r="M52" s="1"/>
+      <c r="N52" s="1"/>
+      <c r="O52" s="1"/>
+      <c r="P52" s="1"/>
+      <c r="Q52" s="1"/>
+      <c r="R52" s="1"/>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A53" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
+      <c r="F53" s="3"/>
+      <c r="G53" s="3"/>
+      <c r="H53" s="3"/>
+      <c r="I53" s="2"/>
+      <c r="J53" s="2"/>
+      <c r="K53" s="2"/>
+      <c r="L53" s="2"/>
+      <c r="M53" s="2"/>
+      <c r="N53" s="2"/>
+      <c r="O53" s="2"/>
+      <c r="P53" s="2"/>
+      <c r="Q53" s="2"/>
+      <c r="R53" s="2"/>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A54" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C54" s="10">
+        <v>1</v>
+      </c>
+      <c r="D54" s="5"/>
+      <c r="E54" s="5"/>
+      <c r="F54" s="5"/>
+      <c r="G54" s="5"/>
+      <c r="H54" s="5"/>
+      <c r="I54" s="4"/>
+      <c r="J54" s="4"/>
+      <c r="K54" s="4"/>
+      <c r="L54" s="4"/>
+      <c r="M54" s="4"/>
+      <c r="N54" s="4"/>
+      <c r="O54" s="4"/>
+      <c r="P54" s="4"/>
+      <c r="Q54" s="4"/>
+      <c r="R54" s="4"/>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A56" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B50" s="8" t="s">
+      <c r="B56" s="8" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A51" s="7" t="s">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A57" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B51" s="8" t="s">
+      <c r="B57" s="8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A52" s="7" t="s">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A58" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B52" s="8" t="s">
+      <c r="B58" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A59" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B59" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C59" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="D59" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E53" s="1" t="s">
+      <c r="E59" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
-      <c r="H53" s="1"/>
-      <c r="I53" s="1"/>
-      <c r="J53" s="1"/>
-      <c r="K53" s="1"/>
-      <c r="L53" s="1"/>
-      <c r="M53" s="1"/>
-      <c r="N53" s="1"/>
-      <c r="O53" s="1"/>
-      <c r="P53" s="1"/>
-      <c r="Q53" s="1"/>
-      <c r="R53" s="1"/>
-    </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
+      <c r="F59" s="1"/>
+      <c r="G59" s="1"/>
+      <c r="H59" s="1"/>
+      <c r="I59" s="1"/>
+      <c r="J59" s="1"/>
+      <c r="K59" s="1"/>
+      <c r="L59" s="1"/>
+      <c r="M59" s="1"/>
+      <c r="N59" s="1"/>
+      <c r="O59" s="1"/>
+      <c r="P59" s="1"/>
+      <c r="Q59" s="1"/>
+      <c r="R59" s="1"/>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A60" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="B60" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C54" s="3" t="s">
+      <c r="C60" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D54" s="3"/>
-      <c r="E54" s="3"/>
-      <c r="F54" s="3"/>
-      <c r="G54" s="3"/>
-      <c r="H54" s="3"/>
-      <c r="I54" s="2"/>
-      <c r="J54" s="2"/>
-      <c r="K54" s="2"/>
-      <c r="L54" s="2"/>
-      <c r="M54" s="2"/>
-      <c r="N54" s="2"/>
-      <c r="O54" s="2"/>
-      <c r="P54" s="2"/>
-      <c r="Q54" s="2"/>
-      <c r="R54" s="2"/>
-    </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A55" s="4" t="s">
+      <c r="D60" s="3"/>
+      <c r="E60" s="3"/>
+      <c r="F60" s="3"/>
+      <c r="G60" s="3"/>
+      <c r="H60" s="3"/>
+      <c r="I60" s="2"/>
+      <c r="J60" s="2"/>
+      <c r="K60" s="2"/>
+      <c r="L60" s="2"/>
+      <c r="M60" s="2"/>
+      <c r="N60" s="2"/>
+      <c r="O60" s="2"/>
+      <c r="P60" s="2"/>
+      <c r="Q60" s="2"/>
+      <c r="R60" s="2"/>
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A61" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B55" s="5" t="s">
+      <c r="B61" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C55" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D55" s="5"/>
-      <c r="E55" s="5"/>
-      <c r="F55" s="5"/>
-      <c r="G55" s="5"/>
-      <c r="H55" s="5"/>
-      <c r="I55" s="4"/>
-      <c r="J55" s="4"/>
-      <c r="K55" s="4"/>
-      <c r="L55" s="4"/>
-      <c r="M55" s="4"/>
-      <c r="N55" s="4"/>
-      <c r="O55" s="4"/>
-      <c r="P55" s="4"/>
-      <c r="Q55" s="4"/>
-      <c r="R55" s="4"/>
-    </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A58" s="7" t="s">
+      <c r="C61" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D61" s="5"/>
+      <c r="E61" s="5"/>
+      <c r="F61" s="5"/>
+      <c r="G61" s="5"/>
+      <c r="H61" s="5"/>
+      <c r="I61" s="4"/>
+      <c r="J61" s="4"/>
+      <c r="K61" s="4"/>
+      <c r="L61" s="4"/>
+      <c r="M61" s="4"/>
+      <c r="N61" s="4"/>
+      <c r="O61" s="4"/>
+      <c r="P61" s="4"/>
+      <c r="Q61" s="4"/>
+      <c r="R61" s="4"/>
+    </row>
+    <row r="64" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A64" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B58" s="8" t="s">
+      <c r="B64" s="8" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A59" s="7" t="s">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A65" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B59" s="8"/>
-    </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A60" s="7" t="s">
+      <c r="B65" s="8"/>
+    </row>
+    <row r="66" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A66" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B60" s="8" t="s">
+      <c r="B66" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A67" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B67" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="C67" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D61" s="1" t="s">
+      <c r="D67" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E61" s="1" t="s">
+      <c r="E67" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F61" s="1"/>
-      <c r="G61" s="1"/>
-      <c r="H61" s="1"/>
-      <c r="I61" s="1"/>
-      <c r="J61" s="1"/>
-      <c r="K61" s="1"/>
-      <c r="L61" s="1"/>
-      <c r="M61" s="1"/>
-      <c r="N61" s="1"/>
-      <c r="O61" s="1"/>
-      <c r="P61" s="1"/>
-      <c r="Q61" s="1"/>
-      <c r="R61" s="1"/>
-    </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A62" s="2" t="s">
+      <c r="F67" s="1"/>
+      <c r="G67" s="1"/>
+      <c r="H67" s="1"/>
+      <c r="I67" s="1"/>
+      <c r="J67" s="1"/>
+      <c r="K67" s="1"/>
+      <c r="L67" s="1"/>
+      <c r="M67" s="1"/>
+      <c r="N67" s="1"/>
+      <c r="O67" s="1"/>
+      <c r="P67" s="1"/>
+      <c r="Q67" s="1"/>
+      <c r="R67" s="1"/>
+    </row>
+    <row r="68" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A68" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B62" s="3" t="s">
+      <c r="B68" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C62" s="3" t="s">
+      <c r="C68" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D62" s="12"/>
-      <c r="E62" s="3"/>
-      <c r="F62" s="3"/>
-      <c r="G62" s="3"/>
-      <c r="H62" s="3"/>
-      <c r="I62" s="2"/>
-      <c r="J62" s="2"/>
-      <c r="K62" s="2"/>
-      <c r="L62" s="2"/>
-      <c r="M62" s="2"/>
-      <c r="N62" s="2"/>
-      <c r="O62" s="2"/>
-      <c r="P62" s="2"/>
-      <c r="Q62" s="2"/>
-      <c r="R62" s="2"/>
-    </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A63" s="4" t="s">
+      <c r="D68" s="12"/>
+      <c r="E68" s="3"/>
+      <c r="F68" s="3"/>
+      <c r="G68" s="3"/>
+      <c r="H68" s="3"/>
+      <c r="I68" s="2"/>
+      <c r="J68" s="2"/>
+      <c r="K68" s="2"/>
+      <c r="L68" s="2"/>
+      <c r="M68" s="2"/>
+      <c r="N68" s="2"/>
+      <c r="O68" s="2"/>
+      <c r="P68" s="2"/>
+      <c r="Q68" s="2"/>
+      <c r="R68" s="2"/>
+    </row>
+    <row r="69" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A69" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B63" s="5" t="s">
+      <c r="B69" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C63" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D63" s="5"/>
-      <c r="E63" s="5"/>
-      <c r="F63" s="5"/>
-      <c r="G63" s="5"/>
-      <c r="H63" s="5"/>
-      <c r="I63" s="4"/>
-      <c r="J63" s="4"/>
-      <c r="K63" s="4"/>
-      <c r="L63" s="4"/>
-      <c r="M63" s="4"/>
-      <c r="N63" s="4"/>
-      <c r="O63" s="4"/>
-      <c r="P63" s="4"/>
-      <c r="Q63" s="4"/>
-      <c r="R63" s="4"/>
-    </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A66" s="7" t="s">
+      <c r="C69" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D69" s="5"/>
+      <c r="E69" s="5"/>
+      <c r="F69" s="5"/>
+      <c r="G69" s="5"/>
+      <c r="H69" s="5"/>
+      <c r="I69" s="4"/>
+      <c r="J69" s="4"/>
+      <c r="K69" s="4"/>
+      <c r="L69" s="4"/>
+      <c r="M69" s="4"/>
+      <c r="N69" s="4"/>
+      <c r="O69" s="4"/>
+      <c r="P69" s="4"/>
+      <c r="Q69" s="4"/>
+      <c r="R69" s="4"/>
+    </row>
+    <row r="72" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A72" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B66" s="8" t="s">
+      <c r="B72" s="8" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A67" s="7" t="s">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A73" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B67" s="8" t="s">
+      <c r="B73" s="8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A68" s="7" t="s">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A74" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B68" s="8" t="s">
+      <c r="B74" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A75" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="B75" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C69" s="1" t="s">
+      <c r="C75" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D69" s="1" t="s">
+      <c r="D75" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E69" s="1" t="s">
+      <c r="E75" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F69" s="1"/>
-      <c r="G69" s="1"/>
-      <c r="H69" s="1"/>
-      <c r="I69" s="1"/>
-      <c r="J69" s="1"/>
-      <c r="K69" s="1"/>
-      <c r="L69" s="1"/>
-      <c r="M69" s="1"/>
-      <c r="N69" s="1"/>
-      <c r="O69" s="1"/>
-      <c r="P69" s="1"/>
-      <c r="Q69" s="1"/>
-      <c r="R69" s="1"/>
-    </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A70" s="2" t="s">
+      <c r="F75" s="1"/>
+      <c r="G75" s="1"/>
+      <c r="H75" s="1"/>
+      <c r="I75" s="1"/>
+      <c r="J75" s="1"/>
+      <c r="K75" s="1"/>
+      <c r="L75" s="1"/>
+      <c r="M75" s="1"/>
+      <c r="N75" s="1"/>
+      <c r="O75" s="1"/>
+      <c r="P75" s="1"/>
+      <c r="Q75" s="1"/>
+      <c r="R75" s="1"/>
+    </row>
+    <row r="76" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A76" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B70" s="3"/>
-      <c r="C70" s="3" t="s">
+      <c r="B76" s="3"/>
+      <c r="C76" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D70" s="3"/>
-      <c r="E70" s="3"/>
-      <c r="F70" s="3"/>
-      <c r="G70" s="3"/>
-      <c r="H70" s="3"/>
-      <c r="I70" s="2"/>
-      <c r="J70" s="2"/>
-      <c r="K70" s="2"/>
-      <c r="L70" s="2"/>
-      <c r="M70" s="2"/>
-      <c r="N70" s="2"/>
-      <c r="O70" s="2"/>
-      <c r="P70" s="2"/>
-      <c r="Q70" s="2"/>
-      <c r="R70" s="2"/>
-    </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A71" s="4" t="s">
+      <c r="D76" s="3"/>
+      <c r="E76" s="3"/>
+      <c r="F76" s="3"/>
+      <c r="G76" s="3"/>
+      <c r="H76" s="3"/>
+      <c r="I76" s="2"/>
+      <c r="J76" s="2"/>
+      <c r="K76" s="2"/>
+      <c r="L76" s="2"/>
+      <c r="M76" s="2"/>
+      <c r="N76" s="2"/>
+      <c r="O76" s="2"/>
+      <c r="P76" s="2"/>
+      <c r="Q76" s="2"/>
+      <c r="R76" s="2"/>
+    </row>
+    <row r="77" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A77" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B71" s="5"/>
-      <c r="C71" s="5" t="s">
+      <c r="B77" s="5"/>
+      <c r="C77" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D71" s="5"/>
-      <c r="E71" s="5"/>
-      <c r="F71" s="5"/>
-      <c r="G71" s="5"/>
-      <c r="H71" s="5"/>
-      <c r="I71" s="4"/>
-      <c r="J71" s="4"/>
-      <c r="K71" s="4"/>
-      <c r="L71" s="4"/>
-      <c r="M71" s="4"/>
-      <c r="N71" s="4"/>
-      <c r="O71" s="4"/>
-      <c r="P71" s="4"/>
-      <c r="Q71" s="4"/>
-      <c r="R71" s="4"/>
+      <c r="D77" s="5"/>
+      <c r="E77" s="5"/>
+      <c r="F77" s="5"/>
+      <c r="G77" s="5"/>
+      <c r="H77" s="5"/>
+      <c r="I77" s="4"/>
+      <c r="J77" s="4"/>
+      <c r="K77" s="4"/>
+      <c r="L77" s="4"/>
+      <c r="M77" s="4"/>
+      <c r="N77" s="4"/>
+      <c r="O77" s="4"/>
+      <c r="P77" s="4"/>
+      <c r="Q77" s="4"/>
+      <c r="R77" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
check-in: 10100423 zhongshu_wangge update
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="61">
   <si>
     <t>交易品种：</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -253,14 +253,6 @@
   </si>
   <si>
     <t>0.974/0.990</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>pending</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>pending</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -681,8 +673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -771,9 +763,7 @@
       <c r="B7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="9">
-        <v>1</v>
-      </c>
+      <c r="C7" s="9"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -1287,7 +1277,9 @@
       <c r="B46" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C46" s="3"/>
+      <c r="C46" s="11">
+        <v>1</v>
+      </c>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
@@ -1311,9 +1303,7 @@
       <c r="B47" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C47" s="10" t="s">
-        <v>60</v>
-      </c>
+      <c r="C47" s="10"/>
       <c r="D47" s="5"/>
       <c r="E47" s="5"/>
       <c r="F47" s="5"/>
@@ -1418,7 +1408,7 @@
         <v>59</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="D55" s="5"/>
       <c r="E55" s="5"/>
@@ -1522,7 +1512,7 @@
         <v>47</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D63" s="5"/>
       <c r="E63" s="5"/>

</xml_diff>

<commit_message>
check-in: 20200425 zhongshu_wangge.xlsl update
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="66">
   <si>
     <t>交易品种：</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -204,10 +204,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>0.875/0.919</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>pending</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -220,50 +216,46 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>13.05/14.14</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>30.38/31.75</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.23/4.42</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.214/0.264</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.242/0.264</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>88.412/94.20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>89.818/90.200</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.974/0.990</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>pending</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>13.05/14.14</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>30.38/31.75</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4.23/4.42</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.214/0.264</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.242/0.264</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>88.412/94.20</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>89.818/90.200</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.974/0.990</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>pending</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>pending</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>众兴转债（128026）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -273,6 +265,18 @@
   </si>
   <si>
     <t>93.503/99.117</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.920/0.940</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.878/0.916</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.723/0.746</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -689,8 +693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F64" sqref="F64"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C80" sqref="C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -779,9 +783,7 @@
       <c r="B7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="9">
-        <v>1</v>
-      </c>
+      <c r="C7" s="9"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -803,11 +805,9 @@
         <v>8</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C8" s="10">
-        <v>1</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="C8" s="10"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
@@ -911,7 +911,7 @@
         <v>1</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
@@ -1109,7 +1109,7 @@
         <v>8</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C32" s="10">
         <v>1</v>
@@ -1189,7 +1189,7 @@
         <v>43</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C39" s="11">
         <v>1</v>
@@ -1215,7 +1215,7 @@
         <v>8</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C40" s="10">
         <v>1</v>
@@ -1293,7 +1293,7 @@
         <v>44</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C46" s="11">
         <v>1</v>
@@ -1319,7 +1319,7 @@
         <v>8</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C47" s="10"/>
       <c r="D47" s="5"/>
@@ -1343,7 +1343,7 @@
         <v>0</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.15">
@@ -1395,7 +1395,7 @@
         <v>41</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
@@ -1419,7 +1419,7 @@
         <v>8</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C54" s="10">
         <v>1</v>
@@ -1501,9 +1501,7 @@
       <c r="B60" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C60" s="3" t="s">
-        <v>48</v>
-      </c>
+      <c r="C60" s="3"/>
       <c r="D60" s="3"/>
       <c r="E60" s="3"/>
       <c r="F60" s="3"/>
@@ -1525,10 +1523,10 @@
         <v>8</v>
       </c>
       <c r="B61" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C61" s="5" t="s">
         <v>59</v>
-      </c>
-      <c r="C61" s="5" t="s">
-        <v>61</v>
       </c>
       <c r="D61" s="5"/>
       <c r="E61" s="5"/>
@@ -1606,7 +1604,7 @@
         <v>28</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D68" s="12"/>
       <c r="E68" s="3"/>
@@ -1629,10 +1627,10 @@
         <v>8</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D69" s="5"/>
       <c r="E69" s="5"/>
@@ -1708,9 +1706,11 @@
       <c r="A76" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B76" s="3"/>
+      <c r="B76" s="3" t="s">
+        <v>64</v>
+      </c>
       <c r="C76" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D76" s="3"/>
       <c r="E76" s="3"/>
@@ -1732,9 +1732,11 @@
       <c r="A77" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B77" s="5"/>
+      <c r="B77" s="5" t="s">
+        <v>65</v>
+      </c>
       <c r="C77" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D77" s="5"/>
       <c r="E77" s="5"/>

</xml_diff>

<commit_message>
check-in: 20200427 zhongshuwangge update
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7590"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30696" windowHeight="11856"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -283,7 +283,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0_);\(0\)"/>
   </numFmts>
@@ -405,7 +405,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -693,22 +693,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C80" sqref="C80"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.75" customWidth="1"/>
-    <col min="2" max="2" width="25.125" customWidth="1"/>
-    <col min="3" max="3" width="23.125" customWidth="1"/>
-    <col min="4" max="4" width="21.5" customWidth="1"/>
+    <col min="1" max="1" width="17.77734375" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="21.75" customWidth="1"/>
-    <col min="7" max="8" width="19.5" customWidth="1"/>
+    <col min="6" max="6" width="21.77734375" customWidth="1"/>
+    <col min="7" max="8" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="25.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="25.8" x14ac:dyDescent="0.4">
       <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
@@ -722,7 +722,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>29</v>
       </c>
@@ -730,7 +730,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>10</v>
       </c>
@@ -738,7 +738,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>11</v>
       </c>
@@ -746,7 +746,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -776,7 +776,7 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
@@ -800,7 +800,7 @@
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
@@ -824,7 +824,7 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>0</v>
       </c>
@@ -832,13 +832,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="8"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>17</v>
       </c>
@@ -846,7 +846,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
@@ -876,7 +876,7 @@
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>40</v>
       </c>
@@ -900,7 +900,7 @@
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>39</v>
       </c>
@@ -913,7 +913,9 @@
       <c r="D16" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E16" s="5"/>
+      <c r="E16" s="10">
+        <v>1</v>
+      </c>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
@@ -928,7 +930,7 @@
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>0</v>
       </c>
@@ -936,13 +938,13 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="8"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>21</v>
       </c>
@@ -950,7 +952,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>6</v>
       </c>
@@ -976,7 +978,7 @@
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>41</v>
       </c>
@@ -1000,7 +1002,7 @@
       <c r="Q23" s="2"/>
       <c r="R23" s="2"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>8</v>
       </c>
@@ -1026,7 +1028,7 @@
       <c r="Q24" s="4"/>
       <c r="R24" s="4"/>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>0</v>
       </c>
@@ -1034,13 +1036,13 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B28" s="8"/>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>17</v>
       </c>
@@ -1048,7 +1050,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>6</v>
       </c>
@@ -1078,7 +1080,7 @@
       <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>42</v>
       </c>
@@ -1104,7 +1106,7 @@
       <c r="Q31" s="2"/>
       <c r="R31" s="2"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>8</v>
       </c>
@@ -1130,7 +1132,7 @@
       <c r="Q32" s="4"/>
       <c r="R32" s="4"/>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>0</v>
       </c>
@@ -1138,7 +1140,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>16</v>
       </c>
@@ -1146,7 +1148,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
         <v>17</v>
       </c>
@@ -1154,7 +1156,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>6</v>
       </c>
@@ -1184,7 +1186,7 @@
       <c r="Q38" s="1"/>
       <c r="R38" s="1"/>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>43</v>
       </c>
@@ -1210,7 +1212,7 @@
       <c r="Q39" s="2"/>
       <c r="R39" s="2"/>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>8</v>
       </c>
@@ -1236,7 +1238,7 @@
       <c r="Q40" s="4"/>
       <c r="R40" s="4"/>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>0</v>
       </c>
@@ -1244,13 +1246,13 @@
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B43" s="8"/>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
         <v>17</v>
       </c>
@@ -1258,7 +1260,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>6</v>
       </c>
@@ -1288,7 +1290,7 @@
       <c r="Q45" s="1"/>
       <c r="R45" s="1"/>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>44</v>
       </c>
@@ -1314,7 +1316,7 @@
       <c r="Q46" s="2"/>
       <c r="R46" s="2"/>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>8</v>
       </c>
@@ -1338,7 +1340,7 @@
       <c r="Q47" s="4"/>
       <c r="R47" s="4"/>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>0</v>
       </c>
@@ -1346,13 +1348,13 @@
         <v>60</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B50" s="8"/>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
         <v>17</v>
       </c>
@@ -1360,7 +1362,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>6</v>
       </c>
@@ -1390,7 +1392,7 @@
       <c r="Q52" s="1"/>
       <c r="R52" s="1"/>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>41</v>
       </c>
@@ -1414,7 +1416,7 @@
       <c r="Q53" s="2"/>
       <c r="R53" s="2"/>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>8</v>
       </c>
@@ -1440,7 +1442,7 @@
       <c r="Q54" s="4"/>
       <c r="R54" s="4"/>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
         <v>0</v>
       </c>
@@ -1448,7 +1450,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
         <v>16</v>
       </c>
@@ -1456,7 +1458,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
         <v>17</v>
       </c>
@@ -1464,7 +1466,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>6</v>
       </c>
@@ -1494,7 +1496,7 @@
       <c r="Q59" s="1"/>
       <c r="R59" s="1"/>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>45</v>
       </c>
@@ -1518,7 +1520,7 @@
       <c r="Q60" s="2"/>
       <c r="R60" s="2"/>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>8</v>
       </c>
@@ -1544,7 +1546,7 @@
       <c r="Q61" s="4"/>
       <c r="R61" s="4"/>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
         <v>0</v>
       </c>
@@ -1552,13 +1554,13 @@
         <v>35</v>
       </c>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B65" s="8"/>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
         <v>17</v>
       </c>
@@ -1566,7 +1568,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>6</v>
       </c>
@@ -1596,7 +1598,7 @@
       <c r="Q67" s="1"/>
       <c r="R67" s="1"/>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>46</v>
       </c>
@@ -1622,7 +1624,7 @@
       <c r="Q68" s="2"/>
       <c r="R68" s="2"/>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>8</v>
       </c>
@@ -1648,7 +1650,7 @@
       <c r="Q69" s="4"/>
       <c r="R69" s="4"/>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
         <v>0</v>
       </c>
@@ -1656,7 +1658,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
         <v>16</v>
       </c>
@@ -1664,7 +1666,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
         <v>17</v>
       </c>
@@ -1672,7 +1674,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>6</v>
       </c>
@@ -1702,7 +1704,7 @@
       <c r="Q75" s="1"/>
       <c r="R75" s="1"/>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>45</v>
       </c>
@@ -1728,7 +1730,7 @@
       <c r="Q76" s="2"/>
       <c r="R76" s="2"/>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
check-in: 20200427 zhongshu_wangge.xlsl update
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -693,8 +693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -1423,9 +1423,7 @@
       <c r="B54" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C54" s="10">
-        <v>1</v>
-      </c>
+      <c r="C54" s="10"/>
       <c r="D54" s="5"/>
       <c r="E54" s="5"/>
       <c r="F54" s="5"/>

</xml_diff>

<commit_message>
check-in: 20200429 zhongshu_wangge update
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="67">
   <si>
     <t>交易品种：</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -277,6 +277,10 @@
   </si>
   <si>
     <t>0.723/0.746</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.07/4.22</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -693,8 +697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -807,7 +811,9 @@
       <c r="B8" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C8" s="10"/>
+      <c r="C8" s="10">
+        <v>1</v>
+      </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
@@ -1116,8 +1122,12 @@
       <c r="C32" s="10">
         <v>1</v>
       </c>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
+      <c r="D32" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E32" s="10">
+        <v>1</v>
+      </c>
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
       <c r="H32" s="5"/>
@@ -1219,9 +1229,7 @@
       <c r="B40" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C40" s="10">
-        <v>1</v>
-      </c>
+      <c r="C40" s="10"/>
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>

</xml_diff>

<commit_message>
check-in:  20200505 zhongshu_wangge.xlsx update
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30696" windowHeight="11856"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30690" windowHeight="11850"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="47">
   <si>
     <t>交易品种：</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -124,14 +124,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>0.947/0.968</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.095/1.215</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>交易品种：</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -148,30 +140,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>华宝油气（162411）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>亚药转债（128062）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>H股ETF（510900）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>有友食品（603697）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>豆粕ETF（159985）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>白银基金（161226）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>30F</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -192,30 +164,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1D</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1D</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1D</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>pending</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>pending</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>pending</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>13.05/14.14</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -228,70 +176,42 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>0.214/0.264</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.242/0.264</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>88.412/94.20</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>89.818/90.200</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.974/0.990</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>pending</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>pending</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>众兴转债（128026）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>100.28/101.87</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>93.503/99.117</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.920/0.940</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.878/0.916</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.723/0.746</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4.07/4.22</t>
+    <t>50ETF（510050）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5F</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.849/2.858</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>创业板50（159949）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.762/0.772</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中小板（159902）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.370/3.395</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0_);\(0\)"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -315,15 +235,8 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFFFF00"/>
-      <name val="宋体"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -351,6 +264,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF7DBC56"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -382,7 +301,7 @@
     <xf numFmtId="176" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="176" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="176" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -409,7 +328,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -695,24 +614,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R77"/>
+  <dimension ref="A1:R59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" customWidth="1"/>
-    <col min="2" max="2" width="25.109375" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" customWidth="1"/>
+    <col min="1" max="1" width="17.75" customWidth="1"/>
+    <col min="2" max="2" width="25.125" customWidth="1"/>
+    <col min="3" max="3" width="23.125" customWidth="1"/>
+    <col min="4" max="4" width="21.5" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="21.77734375" customWidth="1"/>
-    <col min="7" max="8" width="19.44140625" customWidth="1"/>
+    <col min="6" max="6" width="21.75" customWidth="1"/>
+    <col min="7" max="8" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="25.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:18" ht="25.5" x14ac:dyDescent="0.3">
       <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
@@ -726,15 +645,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
         <v>10</v>
       </c>
@@ -742,7 +661,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
         <v>11</v>
       </c>
@@ -750,7 +669,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -780,7 +699,7 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
@@ -804,16 +723,14 @@
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C8" s="10">
-        <v>1</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="C8" s="10"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
@@ -830,21 +747,21 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A11" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A12" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="8"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A13" s="7" t="s">
         <v>17</v>
       </c>
@@ -852,7 +769,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
@@ -882,9 +799,9 @@
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>14</v>
@@ -906,9 +823,9 @@
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A16" s="4" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>24</v>
@@ -917,7 +834,7 @@
         <v>1</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="E16" s="10">
         <v>1</v>
@@ -936,21 +853,21 @@
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A19" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A20" s="7" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="8"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A21" s="7" t="s">
         <v>21</v>
       </c>
@@ -958,7 +875,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>6</v>
       </c>
@@ -984,9 +901,9 @@
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A23" s="2" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>15</v>
@@ -1008,7 +925,7 @@
       <c r="Q23" s="2"/>
       <c r="R23" s="2"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A24" s="4" t="s">
         <v>8</v>
       </c>
@@ -1034,21 +951,21 @@
       <c r="Q24" s="4"/>
       <c r="R24" s="4"/>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A27" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A28" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B28" s="8"/>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A29" s="7" t="s">
         <v>17</v>
       </c>
@@ -1056,7 +973,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
         <v>6</v>
       </c>
@@ -1086,9 +1003,9 @@
       <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A31" s="2" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>26</v>
@@ -1112,22 +1029,18 @@
       <c r="Q31" s="2"/>
       <c r="R31" s="2"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A32" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="C32" s="10">
         <v>1</v>
       </c>
-      <c r="D32" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="E32" s="10">
-        <v>1</v>
-      </c>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
       <c r="H32" s="5"/>
@@ -1142,15 +1055,15 @@
       <c r="Q32" s="4"/>
       <c r="R32" s="4"/>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A35" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A36" s="7" t="s">
         <v>16</v>
       </c>
@@ -1158,7 +1071,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A37" s="7" t="s">
         <v>17</v>
       </c>
@@ -1166,7 +1079,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
         <v>6</v>
       </c>
@@ -1196,16 +1109,12 @@
       <c r="Q38" s="1"/>
       <c r="R38" s="1"/>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A39" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C39" s="11">
-        <v>1</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="B39" s="3"/>
+      <c r="C39" s="11"/>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
@@ -1222,13 +1131,11 @@
       <c r="Q39" s="2"/>
       <c r="R39" s="2"/>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A40" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B40" s="5" t="s">
-        <v>54</v>
-      </c>
+      <c r="B40" s="5"/>
       <c r="C40" s="10"/>
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
@@ -1246,521 +1153,273 @@
       <c r="Q40" s="4"/>
       <c r="R40" s="4"/>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A42" s="7" t="s">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A41" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C41" s="12"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="12"/>
+      <c r="F41" s="12"/>
+      <c r="G41" s="12"/>
+      <c r="H41" s="12"/>
+      <c r="I41" s="12"/>
+      <c r="J41" s="12"/>
+      <c r="K41" s="12"/>
+      <c r="L41" s="12"/>
+      <c r="M41" s="12"/>
+      <c r="N41" s="12"/>
+      <c r="O41" s="12"/>
+      <c r="P41" s="12"/>
+      <c r="Q41" s="12"/>
+      <c r="R41" s="12"/>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A44" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B42" s="8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A43" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B43" s="8"/>
-    </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A44" s="7" t="s">
+      <c r="B44" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A45" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A46" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B44" s="8" t="s">
+      <c r="B46" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A47" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B47" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C47" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="D47" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="E47" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F45" s="1"/>
-      <c r="G45" s="1"/>
-      <c r="H45" s="1"/>
-      <c r="I45" s="1"/>
-      <c r="J45" s="1"/>
-      <c r="K45" s="1"/>
-      <c r="L45" s="1"/>
-      <c r="M45" s="1"/>
-      <c r="N45" s="1"/>
-      <c r="O45" s="1"/>
-      <c r="P45" s="1"/>
-      <c r="Q45" s="1"/>
-      <c r="R45" s="1"/>
-    </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
+      <c r="J47" s="1"/>
+      <c r="K47" s="1"/>
+      <c r="L47" s="1"/>
+      <c r="M47" s="1"/>
+      <c r="N47" s="1"/>
+      <c r="O47" s="1"/>
+      <c r="P47" s="1"/>
+      <c r="Q47" s="1"/>
+      <c r="R47" s="1"/>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A48" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B48" s="3"/>
+      <c r="C48" s="11"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="3"/>
+      <c r="H48" s="3"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+      <c r="K48" s="2"/>
+      <c r="L48" s="2"/>
+      <c r="M48" s="2"/>
+      <c r="N48" s="2"/>
+      <c r="O48" s="2"/>
+      <c r="P48" s="2"/>
+      <c r="Q48" s="2"/>
+      <c r="R48" s="2"/>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A49" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B49" s="5"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="5"/>
+      <c r="H49" s="5"/>
+      <c r="I49" s="4"/>
+      <c r="J49" s="4"/>
+      <c r="K49" s="4"/>
+      <c r="L49" s="4"/>
+      <c r="M49" s="4"/>
+      <c r="N49" s="4"/>
+      <c r="O49" s="4"/>
+      <c r="P49" s="4"/>
+      <c r="Q49" s="4"/>
+      <c r="R49" s="4"/>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A50" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B50" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B46" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C46" s="11">
-        <v>1</v>
-      </c>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
-      <c r="F46" s="3"/>
-      <c r="G46" s="3"/>
-      <c r="H46" s="3"/>
-      <c r="I46" s="2"/>
-      <c r="J46" s="2"/>
-      <c r="K46" s="2"/>
-      <c r="L46" s="2"/>
-      <c r="M46" s="2"/>
-      <c r="N46" s="2"/>
-      <c r="O46" s="2"/>
-      <c r="P46" s="2"/>
-      <c r="Q46" s="2"/>
-      <c r="R46" s="2"/>
-    </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
+      <c r="C50" s="12"/>
+      <c r="D50" s="12"/>
+      <c r="E50" s="12"/>
+      <c r="F50" s="12"/>
+      <c r="G50" s="12"/>
+      <c r="H50" s="12"/>
+      <c r="I50" s="12"/>
+      <c r="J50" s="12"/>
+      <c r="K50" s="12"/>
+      <c r="L50" s="12"/>
+      <c r="M50" s="12"/>
+      <c r="N50" s="12"/>
+      <c r="O50" s="12"/>
+      <c r="P50" s="12"/>
+      <c r="Q50" s="12"/>
+      <c r="R50" s="12"/>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A53" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A54" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A55" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A56" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F56" s="1"/>
+      <c r="G56" s="1"/>
+      <c r="H56" s="1"/>
+      <c r="I56" s="1"/>
+      <c r="J56" s="1"/>
+      <c r="K56" s="1"/>
+      <c r="L56" s="1"/>
+      <c r="M56" s="1"/>
+      <c r="N56" s="1"/>
+      <c r="O56" s="1"/>
+      <c r="P56" s="1"/>
+      <c r="Q56" s="1"/>
+      <c r="R56" s="1"/>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A57" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B57" s="3"/>
+      <c r="C57" s="11"/>
+      <c r="D57" s="3"/>
+      <c r="E57" s="3"/>
+      <c r="F57" s="3"/>
+      <c r="G57" s="3"/>
+      <c r="H57" s="3"/>
+      <c r="I57" s="2"/>
+      <c r="J57" s="2"/>
+      <c r="K57" s="2"/>
+      <c r="L57" s="2"/>
+      <c r="M57" s="2"/>
+      <c r="N57" s="2"/>
+      <c r="O57" s="2"/>
+      <c r="P57" s="2"/>
+      <c r="Q57" s="2"/>
+      <c r="R57" s="2"/>
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A58" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B47" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C47" s="10"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="5"/>
-      <c r="F47" s="5"/>
-      <c r="G47" s="5"/>
-      <c r="H47" s="5"/>
-      <c r="I47" s="4"/>
-      <c r="J47" s="4"/>
-      <c r="K47" s="4"/>
-      <c r="L47" s="4"/>
-      <c r="M47" s="4"/>
-      <c r="N47" s="4"/>
-      <c r="O47" s="4"/>
-      <c r="P47" s="4"/>
-      <c r="Q47" s="4"/>
-      <c r="R47" s="4"/>
-    </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A49" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A50" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B50" s="8"/>
-    </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A51" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B51" s="8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F52" s="1"/>
-      <c r="G52" s="1"/>
-      <c r="H52" s="1"/>
-      <c r="I52" s="1"/>
-      <c r="J52" s="1"/>
-      <c r="K52" s="1"/>
-      <c r="L52" s="1"/>
-      <c r="M52" s="1"/>
-      <c r="N52" s="1"/>
-      <c r="O52" s="1"/>
-      <c r="P52" s="1"/>
-      <c r="Q52" s="1"/>
-      <c r="R52" s="1"/>
-    </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
+      <c r="B58" s="5"/>
+      <c r="C58" s="10"/>
+      <c r="D58" s="5"/>
+      <c r="E58" s="5"/>
+      <c r="F58" s="5"/>
+      <c r="G58" s="5"/>
+      <c r="H58" s="5"/>
+      <c r="I58" s="4"/>
+      <c r="J58" s="4"/>
+      <c r="K58" s="4"/>
+      <c r="L58" s="4"/>
+      <c r="M58" s="4"/>
+      <c r="N58" s="4"/>
+      <c r="O58" s="4"/>
+      <c r="P58" s="4"/>
+      <c r="Q58" s="4"/>
+      <c r="R58" s="4"/>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A59" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B53" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C53" s="3"/>
-      <c r="D53" s="3"/>
-      <c r="E53" s="3"/>
-      <c r="F53" s="3"/>
-      <c r="G53" s="3"/>
-      <c r="H53" s="3"/>
-      <c r="I53" s="2"/>
-      <c r="J53" s="2"/>
-      <c r="K53" s="2"/>
-      <c r="L53" s="2"/>
-      <c r="M53" s="2"/>
-      <c r="N53" s="2"/>
-      <c r="O53" s="2"/>
-      <c r="P53" s="2"/>
-      <c r="Q53" s="2"/>
-      <c r="R53" s="2"/>
-    </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A54" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B54" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C54" s="10"/>
-      <c r="D54" s="5"/>
-      <c r="E54" s="5"/>
-      <c r="F54" s="5"/>
-      <c r="G54" s="5"/>
-      <c r="H54" s="5"/>
-      <c r="I54" s="4"/>
-      <c r="J54" s="4"/>
-      <c r="K54" s="4"/>
-      <c r="L54" s="4"/>
-      <c r="M54" s="4"/>
-      <c r="N54" s="4"/>
-      <c r="O54" s="4"/>
-      <c r="P54" s="4"/>
-      <c r="Q54" s="4"/>
-      <c r="R54" s="4"/>
-    </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A56" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B56" s="8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A57" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B57" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A58" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B58" s="8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F59" s="1"/>
-      <c r="G59" s="1"/>
-      <c r="H59" s="1"/>
-      <c r="I59" s="1"/>
-      <c r="J59" s="1"/>
-      <c r="K59" s="1"/>
-      <c r="L59" s="1"/>
-      <c r="M59" s="1"/>
-      <c r="N59" s="1"/>
-      <c r="O59" s="1"/>
-      <c r="P59" s="1"/>
-      <c r="Q59" s="1"/>
-      <c r="R59" s="1"/>
-    </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C60" s="3"/>
-      <c r="D60" s="3"/>
-      <c r="E60" s="3"/>
-      <c r="F60" s="3"/>
-      <c r="G60" s="3"/>
-      <c r="H60" s="3"/>
-      <c r="I60" s="2"/>
-      <c r="J60" s="2"/>
-      <c r="K60" s="2"/>
-      <c r="L60" s="2"/>
-      <c r="M60" s="2"/>
-      <c r="N60" s="2"/>
-      <c r="O60" s="2"/>
-      <c r="P60" s="2"/>
-      <c r="Q60" s="2"/>
-      <c r="R60" s="2"/>
-    </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A61" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B61" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C61" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D61" s="5"/>
-      <c r="E61" s="5"/>
-      <c r="F61" s="5"/>
-      <c r="G61" s="5"/>
-      <c r="H61" s="5"/>
-      <c r="I61" s="4"/>
-      <c r="J61" s="4"/>
-      <c r="K61" s="4"/>
-      <c r="L61" s="4"/>
-      <c r="M61" s="4"/>
-      <c r="N61" s="4"/>
-      <c r="O61" s="4"/>
-      <c r="P61" s="4"/>
-      <c r="Q61" s="4"/>
-      <c r="R61" s="4"/>
-    </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A64" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B64" s="8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A65" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B65" s="8"/>
-    </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A66" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B66" s="8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F67" s="1"/>
-      <c r="G67" s="1"/>
-      <c r="H67" s="1"/>
-      <c r="I67" s="1"/>
-      <c r="J67" s="1"/>
-      <c r="K67" s="1"/>
-      <c r="L67" s="1"/>
-      <c r="M67" s="1"/>
-      <c r="N67" s="1"/>
-      <c r="O67" s="1"/>
-      <c r="P67" s="1"/>
-      <c r="Q67" s="1"/>
-      <c r="R67" s="1"/>
-    </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A68" s="2" t="s">
+      <c r="B59" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B68" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D68" s="12"/>
-      <c r="E68" s="3"/>
-      <c r="F68" s="3"/>
-      <c r="G68" s="3"/>
-      <c r="H68" s="3"/>
-      <c r="I68" s="2"/>
-      <c r="J68" s="2"/>
-      <c r="K68" s="2"/>
-      <c r="L68" s="2"/>
-      <c r="M68" s="2"/>
-      <c r="N68" s="2"/>
-      <c r="O68" s="2"/>
-      <c r="P68" s="2"/>
-      <c r="Q68" s="2"/>
-      <c r="R68" s="2"/>
-    </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A69" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B69" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C69" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D69" s="5"/>
-      <c r="E69" s="5"/>
-      <c r="F69" s="5"/>
-      <c r="G69" s="5"/>
-      <c r="H69" s="5"/>
-      <c r="I69" s="4"/>
-      <c r="J69" s="4"/>
-      <c r="K69" s="4"/>
-      <c r="L69" s="4"/>
-      <c r="M69" s="4"/>
-      <c r="N69" s="4"/>
-      <c r="O69" s="4"/>
-      <c r="P69" s="4"/>
-      <c r="Q69" s="4"/>
-      <c r="R69" s="4"/>
-    </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A72" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B72" s="8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A73" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B73" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A74" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B74" s="8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F75" s="1"/>
-      <c r="G75" s="1"/>
-      <c r="H75" s="1"/>
-      <c r="I75" s="1"/>
-      <c r="J75" s="1"/>
-      <c r="K75" s="1"/>
-      <c r="L75" s="1"/>
-      <c r="M75" s="1"/>
-      <c r="N75" s="1"/>
-      <c r="O75" s="1"/>
-      <c r="P75" s="1"/>
-      <c r="Q75" s="1"/>
-      <c r="R75" s="1"/>
-    </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A76" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B76" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C76" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D76" s="3"/>
-      <c r="E76" s="3"/>
-      <c r="F76" s="3"/>
-      <c r="G76" s="3"/>
-      <c r="H76" s="3"/>
-      <c r="I76" s="2"/>
-      <c r="J76" s="2"/>
-      <c r="K76" s="2"/>
-      <c r="L76" s="2"/>
-      <c r="M76" s="2"/>
-      <c r="N76" s="2"/>
-      <c r="O76" s="2"/>
-      <c r="P76" s="2"/>
-      <c r="Q76" s="2"/>
-      <c r="R76" s="2"/>
-    </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A77" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B77" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C77" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D77" s="5"/>
-      <c r="E77" s="5"/>
-      <c r="F77" s="5"/>
-      <c r="G77" s="5"/>
-      <c r="H77" s="5"/>
-      <c r="I77" s="4"/>
-      <c r="J77" s="4"/>
-      <c r="K77" s="4"/>
-      <c r="L77" s="4"/>
-      <c r="M77" s="4"/>
-      <c r="N77" s="4"/>
-      <c r="O77" s="4"/>
-      <c r="P77" s="4"/>
-      <c r="Q77" s="4"/>
-      <c r="R77" s="4"/>
+      <c r="C59" s="12"/>
+      <c r="D59" s="12"/>
+      <c r="E59" s="12"/>
+      <c r="F59" s="12"/>
+      <c r="G59" s="12"/>
+      <c r="H59" s="12"/>
+      <c r="I59" s="12"/>
+      <c r="J59" s="12"/>
+      <c r="K59" s="12"/>
+      <c r="L59" s="12"/>
+      <c r="M59" s="12"/>
+      <c r="N59" s="12"/>
+      <c r="O59" s="12"/>
+      <c r="P59" s="12"/>
+      <c r="Q59" s="12"/>
+      <c r="R59" s="12"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
check-in: 20200507 zhognshu_wangge.xlsx update
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30696" windowHeight="11856"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30690" windowHeight="11850"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -188,10 +188,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>3.370/3.395</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>交易数量：</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -205,13 +201,17 @@
   </si>
   <si>
     <t>pending</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.464/3.478</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0_);\(0\)"/>
   </numFmts>
@@ -332,7 +332,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -620,22 +620,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" customWidth="1"/>
-    <col min="2" max="2" width="25.109375" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" customWidth="1"/>
+    <col min="1" max="1" width="17.75" customWidth="1"/>
+    <col min="2" max="2" width="25.125" customWidth="1"/>
+    <col min="3" max="3" width="23.125" customWidth="1"/>
+    <col min="4" max="4" width="21.5" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="21.77734375" customWidth="1"/>
-    <col min="7" max="8" width="19.44140625" customWidth="1"/>
+    <col min="6" max="6" width="21.75" customWidth="1"/>
+    <col min="7" max="8" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="25.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:18" ht="25.5" x14ac:dyDescent="0.3">
       <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
@@ -649,7 +649,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
         <v>24</v>
       </c>
@@ -657,15 +657,15 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
         <v>10</v>
       </c>
@@ -673,7 +673,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -703,7 +703,7 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
@@ -729,7 +729,7 @@
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
@@ -755,7 +755,7 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A11" s="7" t="s">
         <v>0</v>
       </c>
@@ -763,13 +763,13 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A12" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B12" s="8"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A13" s="7" t="s">
         <v>15</v>
       </c>
@@ -777,7 +777,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
@@ -807,7 +807,7 @@
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
         <v>30</v>
       </c>
@@ -831,7 +831,7 @@
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A16" s="4" t="s">
         <v>29</v>
       </c>
@@ -861,7 +861,7 @@
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A19" s="7" t="s">
         <v>0</v>
       </c>
@@ -869,13 +869,13 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A20" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B20" s="8"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A21" s="7" t="s">
         <v>18</v>
       </c>
@@ -883,7 +883,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>6</v>
       </c>
@@ -909,7 +909,7 @@
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A23" s="2" t="s">
         <v>31</v>
       </c>
@@ -917,7 +917,7 @@
         <v>14</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
@@ -935,7 +935,7 @@
       <c r="Q23" s="2"/>
       <c r="R23" s="2"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A24" s="4" t="s">
         <v>8</v>
       </c>
@@ -943,7 +943,7 @@
         <v>22</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
@@ -961,7 +961,7 @@
       <c r="Q24" s="4"/>
       <c r="R24" s="4"/>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A27" s="7" t="s">
         <v>0</v>
       </c>
@@ -969,13 +969,13 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A28" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B28" s="8"/>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A29" s="7" t="s">
         <v>15</v>
       </c>
@@ -983,7 +983,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
         <v>6</v>
       </c>
@@ -1013,7 +1013,7 @@
       <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A31" s="2" t="s">
         <v>32</v>
       </c>
@@ -1039,7 +1039,7 @@
       <c r="Q31" s="2"/>
       <c r="R31" s="2"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A32" s="4" t="s">
         <v>8</v>
       </c>
@@ -1065,7 +1065,7 @@
       <c r="Q32" s="4"/>
       <c r="R32" s="4"/>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A35" s="7" t="s">
         <v>0</v>
       </c>
@@ -1073,15 +1073,15 @@
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A36" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B36" s="8">
         <v>5700</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A37" s="7" t="s">
         <v>15</v>
       </c>
@@ -1089,7 +1089,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
         <v>6</v>
       </c>
@@ -1119,7 +1119,7 @@
       <c r="Q38" s="1"/>
       <c r="R38" s="1"/>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A39" s="2" t="s">
         <v>33</v>
       </c>
@@ -1141,7 +1141,7 @@
       <c r="Q39" s="2"/>
       <c r="R39" s="2"/>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A40" s="4" t="s">
         <v>8</v>
       </c>
@@ -1163,7 +1163,7 @@
       <c r="Q40" s="4"/>
       <c r="R40" s="4"/>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A41" s="12" t="s">
         <v>38</v>
       </c>
@@ -1189,7 +1189,7 @@
       <c r="Q41" s="12"/>
       <c r="R41" s="12"/>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A44" s="7" t="s">
         <v>0</v>
       </c>
@@ -1197,15 +1197,15 @@
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A45" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B45" s="8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A46" s="7" t="s">
         <v>15</v>
       </c>
@@ -1213,7 +1213,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A47" s="1" t="s">
         <v>6</v>
       </c>
@@ -1243,7 +1243,7 @@
       <c r="Q47" s="1"/>
       <c r="R47" s="1"/>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A48" s="2" t="s">
         <v>30</v>
       </c>
@@ -1265,7 +1265,7 @@
       <c r="Q48" s="2"/>
       <c r="R48" s="2"/>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A49" s="4" t="s">
         <v>8</v>
       </c>
@@ -1287,7 +1287,7 @@
       <c r="Q49" s="4"/>
       <c r="R49" s="4"/>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A50" s="12" t="s">
         <v>38</v>
       </c>
@@ -1311,7 +1311,7 @@
       <c r="Q50" s="12"/>
       <c r="R50" s="12"/>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A53" s="7" t="s">
         <v>0</v>
       </c>
@@ -1319,13 +1319,13 @@
         <v>42</v>
       </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A54" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B54" s="8"/>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A55" s="7" t="s">
         <v>15</v>
       </c>
@@ -1333,7 +1333,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A56" s="1" t="s">
         <v>6</v>
       </c>
@@ -1363,7 +1363,7 @@
       <c r="Q56" s="1"/>
       <c r="R56" s="1"/>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A57" s="2" t="s">
         <v>30</v>
       </c>
@@ -1385,7 +1385,7 @@
       <c r="Q57" s="2"/>
       <c r="R57" s="2"/>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A58" s="4" t="s">
         <v>8</v>
       </c>
@@ -1407,12 +1407,12 @@
       <c r="Q58" s="4"/>
       <c r="R58" s="4"/>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A59" s="12" t="s">
         <v>38</v>
       </c>
       <c r="B59" s="12" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C59" s="12"/>
       <c r="D59" s="12"/>

</xml_diff>

<commit_message>
check-in: 20200507 zhongshu_wangge.xlsx update
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30690" windowHeight="11850"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30696" windowHeight="11856"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -211,7 +211,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0_);\(0\)"/>
   </numFmts>
@@ -332,7 +332,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -620,22 +620,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.75" customWidth="1"/>
-    <col min="2" max="2" width="25.125" customWidth="1"/>
-    <col min="3" max="3" width="23.125" customWidth="1"/>
-    <col min="4" max="4" width="21.5" customWidth="1"/>
+    <col min="1" max="1" width="17.77734375" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="21.75" customWidth="1"/>
-    <col min="7" max="8" width="19.5" customWidth="1"/>
+    <col min="6" max="6" width="21.77734375" customWidth="1"/>
+    <col min="7" max="8" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="25.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="25.8" x14ac:dyDescent="0.4">
       <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
@@ -649,7 +649,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>24</v>
       </c>
@@ -657,7 +657,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>43</v>
       </c>
@@ -665,7 +665,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>10</v>
       </c>
@@ -673,7 +673,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -703,16 +703,14 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="9">
-        <v>1</v>
-      </c>
+      <c r="C7" s="9"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -729,7 +727,7 @@
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
@@ -755,7 +753,7 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>0</v>
       </c>
@@ -763,13 +761,13 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>44</v>
       </c>
       <c r="B12" s="8"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>15</v>
       </c>
@@ -777,7 +775,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
@@ -807,7 +805,7 @@
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>30</v>
       </c>
@@ -831,7 +829,7 @@
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>29</v>
       </c>
@@ -861,7 +859,7 @@
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>0</v>
       </c>
@@ -869,13 +867,13 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>44</v>
       </c>
       <c r="B20" s="8"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>18</v>
       </c>
@@ -883,7 +881,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>6</v>
       </c>
@@ -909,7 +907,7 @@
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>31</v>
       </c>
@@ -935,7 +933,7 @@
       <c r="Q23" s="2"/>
       <c r="R23" s="2"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>8</v>
       </c>
@@ -961,7 +959,7 @@
       <c r="Q24" s="4"/>
       <c r="R24" s="4"/>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>0</v>
       </c>
@@ -969,13 +967,13 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>44</v>
       </c>
       <c r="B28" s="8"/>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>15</v>
       </c>
@@ -983,7 +981,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>6</v>
       </c>
@@ -1013,7 +1011,7 @@
       <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>32</v>
       </c>
@@ -1039,7 +1037,7 @@
       <c r="Q31" s="2"/>
       <c r="R31" s="2"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>8</v>
       </c>
@@ -1065,7 +1063,7 @@
       <c r="Q32" s="4"/>
       <c r="R32" s="4"/>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>0</v>
       </c>
@@ -1073,7 +1071,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>44</v>
       </c>
@@ -1081,7 +1079,7 @@
         <v>5700</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
         <v>15</v>
       </c>
@@ -1089,7 +1087,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>6</v>
       </c>
@@ -1119,7 +1117,7 @@
       <c r="Q38" s="1"/>
       <c r="R38" s="1"/>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>33</v>
       </c>
@@ -1141,7 +1139,7 @@
       <c r="Q39" s="2"/>
       <c r="R39" s="2"/>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>8</v>
       </c>
@@ -1163,7 +1161,7 @@
       <c r="Q40" s="4"/>
       <c r="R40" s="4"/>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
         <v>38</v>
       </c>
@@ -1189,7 +1187,7 @@
       <c r="Q41" s="12"/>
       <c r="R41" s="12"/>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
         <v>0</v>
       </c>
@@ -1197,7 +1195,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
         <v>44</v>
       </c>
@@ -1205,7 +1203,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
         <v>15</v>
       </c>
@@ -1213,7 +1211,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>6</v>
       </c>
@@ -1243,7 +1241,7 @@
       <c r="Q47" s="1"/>
       <c r="R47" s="1"/>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>30</v>
       </c>
@@ -1265,7 +1263,7 @@
       <c r="Q48" s="2"/>
       <c r="R48" s="2"/>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>8</v>
       </c>
@@ -1287,7 +1285,7 @@
       <c r="Q49" s="4"/>
       <c r="R49" s="4"/>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
         <v>38</v>
       </c>
@@ -1311,7 +1309,7 @@
       <c r="Q50" s="12"/>
       <c r="R50" s="12"/>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
         <v>0</v>
       </c>
@@ -1319,13 +1317,13 @@
         <v>42</v>
       </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
         <v>44</v>
       </c>
       <c r="B54" s="8"/>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
         <v>15</v>
       </c>
@@ -1333,7 +1331,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>6</v>
       </c>
@@ -1363,7 +1361,7 @@
       <c r="Q56" s="1"/>
       <c r="R56" s="1"/>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>30</v>
       </c>
@@ -1385,7 +1383,7 @@
       <c r="Q57" s="2"/>
       <c r="R57" s="2"/>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>8</v>
       </c>
@@ -1407,7 +1405,7 @@
       <c r="Q58" s="4"/>
       <c r="R58" s="4"/>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59" s="12" t="s">
         <v>38</v>
       </c>

</xml_diff>

<commit_message>
check-in: 20200508 zhongshu_wangge.xlsx update
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -620,8 +620,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -734,9 +734,7 @@
       <c r="B8" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="10">
-        <v>1</v>
-      </c>
+      <c r="C8" s="10"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
@@ -1168,9 +1166,7 @@
       <c r="B41" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C41" s="12">
-        <v>1</v>
-      </c>
+      <c r="C41" s="12"/>
       <c r="D41" s="12"/>
       <c r="E41" s="12"/>
       <c r="F41" s="12"/>

</xml_diff>

<commit_message>
check-in: 20200511 zhongshu_wangge.xlsx update
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30696" windowHeight="11856"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30690" windowHeight="11850"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="56">
   <si>
     <t>交易品种：</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -44,10 +44,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>12.99/13.90</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>30F</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -168,22 +164,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>5F</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2.849/2.858</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>创业板50（159949）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>0.762/0.772</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>中小板（159902）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -204,14 +188,62 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>3.464/3.478</t>
+    <t>豆粕ETF（159985）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.954/0.965</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.303/3.361</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.733/0.744</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.740/2.733</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.848/0.883</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>德国30（513030）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>日经225（513880）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.903/0.920</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>白银基金（161226）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.731/0.746</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.233/0.260</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>华宝油气（162411）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0_);\(0\)"/>
   </numFmts>
@@ -240,7 +272,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -271,12 +303,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -290,7 +316,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -305,7 +331,6 @@
     <xf numFmtId="176" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="176" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="176" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -332,7 +357,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -618,24 +643,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R59"/>
+  <dimension ref="A1:R96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D92" sqref="D92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" customWidth="1"/>
-    <col min="2" max="2" width="25.109375" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" customWidth="1"/>
+    <col min="1" max="1" width="17.75" customWidth="1"/>
+    <col min="2" max="2" width="25.125" customWidth="1"/>
+    <col min="3" max="3" width="23.125" customWidth="1"/>
+    <col min="4" max="4" width="21.5" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="21.77734375" customWidth="1"/>
-    <col min="7" max="8" width="19.44140625" customWidth="1"/>
+    <col min="6" max="6" width="21.75" customWidth="1"/>
+    <col min="7" max="8" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="25.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:18" ht="25.5" x14ac:dyDescent="0.3">
       <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
@@ -649,31 +674,31 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B4" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -681,13 +706,13 @@
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -703,13 +728,11 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>7</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="B7" s="3"/>
       <c r="C7" s="9"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
@@ -727,12 +750,12 @@
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="5"/>
@@ -751,29 +774,29 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A11" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A12" s="7" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B12" s="8"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A13" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
@@ -781,13 +804,13 @@
         <v>5</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
@@ -803,12 +826,12 @@
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -827,18 +850,18 @@
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A16" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C16" s="10">
         <v>1</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E16" s="10">
         <v>1</v>
@@ -857,29 +880,29 @@
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A19" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A20" s="7" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B20" s="8"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A21" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>6</v>
       </c>
@@ -887,7 +910,7 @@
         <v>5</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -905,15 +928,15 @@
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A23" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
@@ -931,15 +954,15 @@
       <c r="Q23" s="2"/>
       <c r="R23" s="2"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A24" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
@@ -957,29 +980,29 @@
       <c r="Q24" s="4"/>
       <c r="R24" s="4"/>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A27" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A28" s="7" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B28" s="8"/>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A29" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B29" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
         <v>6</v>
       </c>
@@ -987,13 +1010,13 @@
         <v>5</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
@@ -1009,12 +1032,12 @@
       <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A31" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C31" s="11">
         <v>1</v>
@@ -1035,12 +1058,12 @@
       <c r="Q31" s="2"/>
       <c r="R31" s="2"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A32" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C32" s="10">
         <v>1</v>
@@ -1061,31 +1084,31 @@
       <c r="Q32" s="4"/>
       <c r="R32" s="4"/>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A35" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A36" s="7" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B36" s="8">
         <v>5700</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A37" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B37" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
         <v>6</v>
       </c>
@@ -1093,13 +1116,13 @@
         <v>5</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
@@ -1115,9 +1138,9 @@
       <c r="Q38" s="1"/>
       <c r="R38" s="1"/>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A39" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B39" s="3"/>
       <c r="C39" s="11"/>
@@ -1137,11 +1160,13 @@
       <c r="Q39" s="2"/>
       <c r="R39" s="2"/>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A40" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B40" s="5"/>
+        <v>7</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="C40" s="10"/>
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
@@ -1159,271 +1184,693 @@
       <c r="Q40" s="4"/>
       <c r="R40" s="4"/>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A41" s="12" t="s">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A43" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A44" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A45" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A46" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+      <c r="J46" s="1"/>
+      <c r="K46" s="1"/>
+      <c r="L46" s="1"/>
+      <c r="M46" s="1"/>
+      <c r="N46" s="1"/>
+      <c r="O46" s="1"/>
+      <c r="P46" s="1"/>
+      <c r="Q46" s="1"/>
+      <c r="R46" s="1"/>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A47" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B47" s="3"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+      <c r="K47" s="2"/>
+      <c r="L47" s="2"/>
+      <c r="M47" s="2"/>
+      <c r="N47" s="2"/>
+      <c r="O47" s="2"/>
+      <c r="P47" s="2"/>
+      <c r="Q47" s="2"/>
+      <c r="R47" s="2"/>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A48" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C48" s="10"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
+      <c r="G48" s="5"/>
+      <c r="H48" s="5"/>
+      <c r="I48" s="4"/>
+      <c r="J48" s="4"/>
+      <c r="K48" s="4"/>
+      <c r="L48" s="4"/>
+      <c r="M48" s="4"/>
+      <c r="N48" s="4"/>
+      <c r="O48" s="4"/>
+      <c r="P48" s="4"/>
+      <c r="Q48" s="4"/>
+      <c r="R48" s="4"/>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A51" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B51" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B41" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C41" s="12"/>
-      <c r="D41" s="12"/>
-      <c r="E41" s="12"/>
-      <c r="F41" s="12"/>
-      <c r="G41" s="12"/>
-      <c r="H41" s="12"/>
-      <c r="I41" s="12"/>
-      <c r="J41" s="12"/>
-      <c r="K41" s="12"/>
-      <c r="L41" s="12"/>
-      <c r="M41" s="12"/>
-      <c r="N41" s="12"/>
-      <c r="O41" s="12"/>
-      <c r="P41" s="12"/>
-      <c r="Q41" s="12"/>
-      <c r="R41" s="12"/>
-    </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A44" s="7" t="s">
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A52" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B52" s="8"/>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A53" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A54" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
+      <c r="I54" s="1"/>
+      <c r="J54" s="1"/>
+      <c r="K54" s="1"/>
+      <c r="L54" s="1"/>
+      <c r="M54" s="1"/>
+      <c r="N54" s="1"/>
+      <c r="O54" s="1"/>
+      <c r="P54" s="1"/>
+      <c r="Q54" s="1"/>
+      <c r="R54" s="1"/>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A55" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B55" s="3"/>
+      <c r="C55" s="11"/>
+      <c r="D55" s="3"/>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3"/>
+      <c r="G55" s="3"/>
+      <c r="H55" s="3"/>
+      <c r="I55" s="2"/>
+      <c r="J55" s="2"/>
+      <c r="K55" s="2"/>
+      <c r="L55" s="2"/>
+      <c r="M55" s="2"/>
+      <c r="N55" s="2"/>
+      <c r="O55" s="2"/>
+      <c r="P55" s="2"/>
+      <c r="Q55" s="2"/>
+      <c r="R55" s="2"/>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A56" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C56" s="10"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="5"/>
+      <c r="F56" s="5"/>
+      <c r="G56" s="5"/>
+      <c r="H56" s="5"/>
+      <c r="I56" s="4"/>
+      <c r="J56" s="4"/>
+      <c r="K56" s="4"/>
+      <c r="L56" s="4"/>
+      <c r="M56" s="4"/>
+      <c r="N56" s="4"/>
+      <c r="O56" s="4"/>
+      <c r="P56" s="4"/>
+      <c r="Q56" s="4"/>
+      <c r="R56" s="4"/>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A59" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B44" s="8" t="s">
+      <c r="B59" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A60" s="7" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A45" s="7" t="s">
+      <c r="B60" s="8"/>
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A61" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B61" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A62" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F62" s="1"/>
+      <c r="G62" s="1"/>
+      <c r="H62" s="1"/>
+      <c r="I62" s="1"/>
+      <c r="J62" s="1"/>
+      <c r="K62" s="1"/>
+      <c r="L62" s="1"/>
+      <c r="M62" s="1"/>
+      <c r="N62" s="1"/>
+      <c r="O62" s="1"/>
+      <c r="P62" s="1"/>
+      <c r="Q62" s="1"/>
+      <c r="R62" s="1"/>
+    </row>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A63" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B63" s="3"/>
+      <c r="C63" s="11"/>
+      <c r="D63" s="3"/>
+      <c r="E63" s="3"/>
+      <c r="F63" s="3"/>
+      <c r="G63" s="3"/>
+      <c r="H63" s="3"/>
+      <c r="I63" s="2"/>
+      <c r="J63" s="2"/>
+      <c r="K63" s="2"/>
+      <c r="L63" s="2"/>
+      <c r="M63" s="2"/>
+      <c r="N63" s="2"/>
+      <c r="O63" s="2"/>
+      <c r="P63" s="2"/>
+      <c r="Q63" s="2"/>
+      <c r="R63" s="2"/>
+    </row>
+    <row r="64" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A64" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B64" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B45" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A46" s="7" t="s">
+      <c r="C64" s="10"/>
+      <c r="D64" s="5"/>
+      <c r="E64" s="5"/>
+      <c r="F64" s="5"/>
+      <c r="G64" s="5"/>
+      <c r="H64" s="5"/>
+      <c r="I64" s="4"/>
+      <c r="J64" s="4"/>
+      <c r="K64" s="4"/>
+      <c r="L64" s="4"/>
+      <c r="M64" s="4"/>
+      <c r="N64" s="4"/>
+      <c r="O64" s="4"/>
+      <c r="P64" s="4"/>
+      <c r="Q64" s="4"/>
+      <c r="R64" s="4"/>
+    </row>
+    <row r="67" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A67" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B67" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="68" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A68" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B68" s="8"/>
+    </row>
+    <row r="69" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A69" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B69" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B46" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
+    </row>
+    <row r="70" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A70" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B70" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C47" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E47" s="1" t="s">
+      <c r="C70" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D70" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
-      <c r="H47" s="1"/>
-      <c r="I47" s="1"/>
-      <c r="J47" s="1"/>
-      <c r="K47" s="1"/>
-      <c r="L47" s="1"/>
-      <c r="M47" s="1"/>
-      <c r="N47" s="1"/>
-      <c r="O47" s="1"/>
-      <c r="P47" s="1"/>
-      <c r="Q47" s="1"/>
-      <c r="R47" s="1"/>
-    </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B48" s="3"/>
-      <c r="C48" s="11"/>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
-      <c r="F48" s="3"/>
-      <c r="G48" s="3"/>
-      <c r="H48" s="3"/>
-      <c r="I48" s="2"/>
-      <c r="J48" s="2"/>
-      <c r="K48" s="2"/>
-      <c r="L48" s="2"/>
-      <c r="M48" s="2"/>
-      <c r="N48" s="2"/>
-      <c r="O48" s="2"/>
-      <c r="P48" s="2"/>
-      <c r="Q48" s="2"/>
-      <c r="R48" s="2"/>
-    </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A49" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B49" s="5"/>
-      <c r="C49" s="10"/>
-      <c r="D49" s="5"/>
-      <c r="E49" s="5"/>
-      <c r="F49" s="5"/>
-      <c r="G49" s="5"/>
-      <c r="H49" s="5"/>
-      <c r="I49" s="4"/>
-      <c r="J49" s="4"/>
-      <c r="K49" s="4"/>
-      <c r="L49" s="4"/>
-      <c r="M49" s="4"/>
-      <c r="N49" s="4"/>
-      <c r="O49" s="4"/>
-      <c r="P49" s="4"/>
-      <c r="Q49" s="4"/>
-      <c r="R49" s="4"/>
-    </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A50" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="B50" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C50" s="12"/>
-      <c r="D50" s="12"/>
-      <c r="E50" s="12"/>
-      <c r="F50" s="12"/>
-      <c r="G50" s="12"/>
-      <c r="H50" s="12"/>
-      <c r="I50" s="12"/>
-      <c r="J50" s="12"/>
-      <c r="K50" s="12"/>
-      <c r="L50" s="12"/>
-      <c r="M50" s="12"/>
-      <c r="N50" s="12"/>
-      <c r="O50" s="12"/>
-      <c r="P50" s="12"/>
-      <c r="Q50" s="12"/>
-      <c r="R50" s="12"/>
-    </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A53" s="7" t="s">
+      <c r="E70" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F70" s="1"/>
+      <c r="G70" s="1"/>
+      <c r="H70" s="1"/>
+      <c r="I70" s="1"/>
+      <c r="J70" s="1"/>
+      <c r="K70" s="1"/>
+      <c r="L70" s="1"/>
+      <c r="M70" s="1"/>
+      <c r="N70" s="1"/>
+      <c r="O70" s="1"/>
+      <c r="P70" s="1"/>
+      <c r="Q70" s="1"/>
+      <c r="R70" s="1"/>
+    </row>
+    <row r="71" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A71" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B71" s="3"/>
+      <c r="C71" s="11"/>
+      <c r="D71" s="3"/>
+      <c r="E71" s="3"/>
+      <c r="F71" s="3"/>
+      <c r="G71" s="3"/>
+      <c r="H71" s="3"/>
+      <c r="I71" s="2"/>
+      <c r="J71" s="2"/>
+      <c r="K71" s="2"/>
+      <c r="L71" s="2"/>
+      <c r="M71" s="2"/>
+      <c r="N71" s="2"/>
+      <c r="O71" s="2"/>
+      <c r="P71" s="2"/>
+      <c r="Q71" s="2"/>
+      <c r="R71" s="2"/>
+    </row>
+    <row r="72" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A72" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C72" s="10"/>
+      <c r="D72" s="5"/>
+      <c r="E72" s="5"/>
+      <c r="F72" s="5"/>
+      <c r="G72" s="5"/>
+      <c r="H72" s="5"/>
+      <c r="I72" s="4"/>
+      <c r="J72" s="4"/>
+      <c r="K72" s="4"/>
+      <c r="L72" s="4"/>
+      <c r="M72" s="4"/>
+      <c r="N72" s="4"/>
+      <c r="O72" s="4"/>
+      <c r="P72" s="4"/>
+      <c r="Q72" s="4"/>
+      <c r="R72" s="4"/>
+    </row>
+    <row r="75" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A75" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B53" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A54" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="B54" s="8"/>
-    </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A55" s="7" t="s">
+      <c r="B75" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="76" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A76" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B76" s="8"/>
+    </row>
+    <row r="77" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A77" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B77" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B55" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
+    </row>
+    <row r="78" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A78" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B78" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C56" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E56" s="1" t="s">
+      <c r="C78" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D78" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F56" s="1"/>
-      <c r="G56" s="1"/>
-      <c r="H56" s="1"/>
-      <c r="I56" s="1"/>
-      <c r="J56" s="1"/>
-      <c r="K56" s="1"/>
-      <c r="L56" s="1"/>
-      <c r="M56" s="1"/>
-      <c r="N56" s="1"/>
-      <c r="O56" s="1"/>
-      <c r="P56" s="1"/>
-      <c r="Q56" s="1"/>
-      <c r="R56" s="1"/>
-    </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B57" s="3"/>
-      <c r="C57" s="11"/>
-      <c r="D57" s="3"/>
-      <c r="E57" s="3"/>
-      <c r="F57" s="3"/>
-      <c r="G57" s="3"/>
-      <c r="H57" s="3"/>
-      <c r="I57" s="2"/>
-      <c r="J57" s="2"/>
-      <c r="K57" s="2"/>
-      <c r="L57" s="2"/>
-      <c r="M57" s="2"/>
-      <c r="N57" s="2"/>
-      <c r="O57" s="2"/>
-      <c r="P57" s="2"/>
-      <c r="Q57" s="2"/>
-      <c r="R57" s="2"/>
-    </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A58" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B58" s="5"/>
-      <c r="C58" s="10"/>
-      <c r="D58" s="5"/>
-      <c r="E58" s="5"/>
-      <c r="F58" s="5"/>
-      <c r="G58" s="5"/>
-      <c r="H58" s="5"/>
-      <c r="I58" s="4"/>
-      <c r="J58" s="4"/>
-      <c r="K58" s="4"/>
-      <c r="L58" s="4"/>
-      <c r="M58" s="4"/>
-      <c r="N58" s="4"/>
-      <c r="O58" s="4"/>
-      <c r="P58" s="4"/>
-      <c r="Q58" s="4"/>
-      <c r="R58" s="4"/>
-    </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A59" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="B59" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="C59" s="12"/>
-      <c r="D59" s="12"/>
-      <c r="E59" s="12"/>
-      <c r="F59" s="12"/>
-      <c r="G59" s="12"/>
-      <c r="H59" s="12"/>
-      <c r="I59" s="12"/>
-      <c r="J59" s="12"/>
-      <c r="K59" s="12"/>
-      <c r="L59" s="12"/>
-      <c r="M59" s="12"/>
-      <c r="N59" s="12"/>
-      <c r="O59" s="12"/>
-      <c r="P59" s="12"/>
-      <c r="Q59" s="12"/>
-      <c r="R59" s="12"/>
+      <c r="E78" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F78" s="1"/>
+      <c r="G78" s="1"/>
+      <c r="H78" s="1"/>
+      <c r="I78" s="1"/>
+      <c r="J78" s="1"/>
+      <c r="K78" s="1"/>
+      <c r="L78" s="1"/>
+      <c r="M78" s="1"/>
+      <c r="N78" s="1"/>
+      <c r="O78" s="1"/>
+      <c r="P78" s="1"/>
+      <c r="Q78" s="1"/>
+      <c r="R78" s="1"/>
+    </row>
+    <row r="79" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A79" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B79" s="3"/>
+      <c r="C79" s="11"/>
+      <c r="D79" s="3"/>
+      <c r="E79" s="3"/>
+      <c r="F79" s="3"/>
+      <c r="G79" s="3"/>
+      <c r="H79" s="3"/>
+      <c r="I79" s="2"/>
+      <c r="J79" s="2"/>
+      <c r="K79" s="2"/>
+      <c r="L79" s="2"/>
+      <c r="M79" s="2"/>
+      <c r="N79" s="2"/>
+      <c r="O79" s="2"/>
+      <c r="P79" s="2"/>
+      <c r="Q79" s="2"/>
+      <c r="R79" s="2"/>
+    </row>
+    <row r="80" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A80" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B80" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C80" s="10"/>
+      <c r="D80" s="5"/>
+      <c r="E80" s="5"/>
+      <c r="F80" s="5"/>
+      <c r="G80" s="5"/>
+      <c r="H80" s="5"/>
+      <c r="I80" s="4"/>
+      <c r="J80" s="4"/>
+      <c r="K80" s="4"/>
+      <c r="L80" s="4"/>
+      <c r="M80" s="4"/>
+      <c r="N80" s="4"/>
+      <c r="O80" s="4"/>
+      <c r="P80" s="4"/>
+      <c r="Q80" s="4"/>
+      <c r="R80" s="4"/>
+    </row>
+    <row r="83" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A83" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B83" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="84" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A84" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B84" s="8"/>
+    </row>
+    <row r="85" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A85" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B85" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="86" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A86" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F86" s="1"/>
+      <c r="G86" s="1"/>
+      <c r="H86" s="1"/>
+      <c r="I86" s="1"/>
+      <c r="J86" s="1"/>
+      <c r="K86" s="1"/>
+      <c r="L86" s="1"/>
+      <c r="M86" s="1"/>
+      <c r="N86" s="1"/>
+      <c r="O86" s="1"/>
+      <c r="P86" s="1"/>
+      <c r="Q86" s="1"/>
+      <c r="R86" s="1"/>
+    </row>
+    <row r="87" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A87" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B87" s="3"/>
+      <c r="C87" s="11"/>
+      <c r="D87" s="3"/>
+      <c r="E87" s="3"/>
+      <c r="F87" s="3"/>
+      <c r="G87" s="3"/>
+      <c r="H87" s="3"/>
+      <c r="I87" s="2"/>
+      <c r="J87" s="2"/>
+      <c r="K87" s="2"/>
+      <c r="L87" s="2"/>
+      <c r="M87" s="2"/>
+      <c r="N87" s="2"/>
+      <c r="O87" s="2"/>
+      <c r="P87" s="2"/>
+      <c r="Q87" s="2"/>
+      <c r="R87" s="2"/>
+    </row>
+    <row r="88" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A88" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B88" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C88" s="10"/>
+      <c r="D88" s="5"/>
+      <c r="E88" s="5"/>
+      <c r="F88" s="5"/>
+      <c r="G88" s="5"/>
+      <c r="H88" s="5"/>
+      <c r="I88" s="4"/>
+      <c r="J88" s="4"/>
+      <c r="K88" s="4"/>
+      <c r="L88" s="4"/>
+      <c r="M88" s="4"/>
+      <c r="N88" s="4"/>
+      <c r="O88" s="4"/>
+      <c r="P88" s="4"/>
+      <c r="Q88" s="4"/>
+      <c r="R88" s="4"/>
+    </row>
+    <row r="91" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A91" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B91" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="92" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A92" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B92" s="8"/>
+    </row>
+    <row r="93" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A93" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B93" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="94" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A94" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F94" s="1"/>
+      <c r="G94" s="1"/>
+      <c r="H94" s="1"/>
+      <c r="I94" s="1"/>
+      <c r="J94" s="1"/>
+      <c r="K94" s="1"/>
+      <c r="L94" s="1"/>
+      <c r="M94" s="1"/>
+      <c r="N94" s="1"/>
+      <c r="O94" s="1"/>
+      <c r="P94" s="1"/>
+      <c r="Q94" s="1"/>
+      <c r="R94" s="1"/>
+    </row>
+    <row r="95" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A95" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B95" s="3"/>
+      <c r="C95" s="11"/>
+      <c r="D95" s="3"/>
+      <c r="E95" s="3"/>
+      <c r="F95" s="3"/>
+      <c r="G95" s="3"/>
+      <c r="H95" s="3"/>
+      <c r="I95" s="2"/>
+      <c r="J95" s="2"/>
+      <c r="K95" s="2"/>
+      <c r="L95" s="2"/>
+      <c r="M95" s="2"/>
+      <c r="N95" s="2"/>
+      <c r="O95" s="2"/>
+      <c r="P95" s="2"/>
+      <c r="Q95" s="2"/>
+      <c r="R95" s="2"/>
+    </row>
+    <row r="96" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A96" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B96" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C96" s="10"/>
+      <c r="D96" s="5"/>
+      <c r="E96" s="5"/>
+      <c r="F96" s="5"/>
+      <c r="G96" s="5"/>
+      <c r="H96" s="5"/>
+      <c r="I96" s="4"/>
+      <c r="J96" s="4"/>
+      <c r="K96" s="4"/>
+      <c r="L96" s="4"/>
+      <c r="M96" s="4"/>
+      <c r="N96" s="4"/>
+      <c r="O96" s="4"/>
+      <c r="P96" s="4"/>
+      <c r="Q96" s="4"/>
+      <c r="R96" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
check-in: 20200513 zhongshu_wangge.xlsx update
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -646,7 +646,7 @@
   <dimension ref="A1:R96"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67"/>
+      <selection activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1463,7 +1463,9 @@
       <c r="B64" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C64" s="10"/>
+      <c r="C64" s="10">
+        <v>1</v>
+      </c>
       <c r="D64" s="5"/>
       <c r="E64" s="5"/>
       <c r="F64" s="5"/>

</xml_diff>

<commit_message>
check-in: 20200515 zhongshu_wangge.xlsx update
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30690" windowHeight="11850"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30696" windowHeight="11856"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="56">
   <si>
     <t>交易品种：</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -233,13 +233,17 @@
   </si>
   <si>
     <t>0.783/0.805</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pending</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0_);\(0\)"/>
   </numFmts>
@@ -353,7 +357,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -639,24 +643,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R113"/>
+  <dimension ref="A1:R112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C113" sqref="C113"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C81" sqref="C81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.75" customWidth="1"/>
-    <col min="2" max="2" width="25.125" customWidth="1"/>
-    <col min="3" max="3" width="23.125" customWidth="1"/>
-    <col min="4" max="4" width="21.5" customWidth="1"/>
+    <col min="1" max="1" width="17.77734375" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="21.75" customWidth="1"/>
-    <col min="7" max="8" width="19.5" customWidth="1"/>
+    <col min="6" max="6" width="21.77734375" customWidth="1"/>
+    <col min="7" max="8" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="25.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="25.8" x14ac:dyDescent="0.4">
       <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
@@ -670,7 +674,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
@@ -678,7 +682,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>35</v>
       </c>
@@ -686,7 +690,7 @@
         <v>5700</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>12</v>
       </c>
@@ -694,7 +698,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -724,7 +728,7 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>28</v>
       </c>
@@ -746,7 +750,7 @@
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
@@ -770,7 +774,7 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>0</v>
       </c>
@@ -778,7 +782,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>35</v>
       </c>
@@ -786,7 +790,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>12</v>
       </c>
@@ -794,7 +798,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
@@ -824,7 +828,7 @@
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>25</v>
       </c>
@@ -846,7 +850,7 @@
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>7</v>
       </c>
@@ -870,7 +874,7 @@
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>0</v>
       </c>
@@ -878,13 +882,13 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>35</v>
       </c>
       <c r="B19" s="8"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>12</v>
       </c>
@@ -892,7 +896,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>6</v>
       </c>
@@ -922,7 +926,7 @@
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>25</v>
       </c>
@@ -944,7 +948,7 @@
       <c r="Q22" s="2"/>
       <c r="R22" s="2"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>7</v>
       </c>
@@ -968,7 +972,7 @@
       <c r="Q23" s="4"/>
       <c r="R23" s="4"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>0</v>
       </c>
@@ -976,13 +980,13 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>34</v>
       </c>
       <c r="B27" s="8"/>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>9</v>
       </c>
@@ -990,7 +994,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>6</v>
       </c>
@@ -1020,7 +1024,7 @@
       <c r="Q29" s="1"/>
       <c r="R29" s="1"/>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>25</v>
       </c>
@@ -1042,7 +1046,7 @@
       <c r="Q30" s="2"/>
       <c r="R30" s="2"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>7</v>
       </c>
@@ -1066,7 +1070,7 @@
       <c r="Q31" s="4"/>
       <c r="R31" s="4"/>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>0</v>
       </c>
@@ -1074,13 +1078,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>34</v>
       </c>
       <c r="B35" s="8"/>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>9</v>
       </c>
@@ -1088,7 +1092,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>6</v>
       </c>
@@ -1118,7 +1122,7 @@
       <c r="Q37" s="1"/>
       <c r="R37" s="1"/>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>25</v>
       </c>
@@ -1140,14 +1144,16 @@
       <c r="Q38" s="2"/>
       <c r="R38" s="2"/>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C39" s="10"/>
+      <c r="C39" s="10" t="s">
+        <v>55</v>
+      </c>
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
@@ -1164,7 +1170,7 @@
       <c r="Q39" s="4"/>
       <c r="R39" s="4"/>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>0</v>
       </c>
@@ -1172,13 +1178,13 @@
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
         <v>35</v>
       </c>
       <c r="B43" s="8"/>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
         <v>12</v>
       </c>
@@ -1186,7 +1192,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>6</v>
       </c>
@@ -1216,7 +1222,7 @@
       <c r="Q45" s="1"/>
       <c r="R45" s="1"/>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>25</v>
       </c>
@@ -1238,7 +1244,7 @@
       <c r="Q46" s="2"/>
       <c r="R46" s="2"/>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>7</v>
       </c>
@@ -1262,817 +1268,799 @@
       <c r="Q47" s="4"/>
       <c r="R47" s="4"/>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A48" s="4"/>
-      <c r="B48" s="5"/>
-      <c r="C48" s="10"/>
-      <c r="D48" s="5"/>
-      <c r="E48" s="5"/>
-      <c r="F48" s="5"/>
-      <c r="G48" s="5"/>
-      <c r="H48" s="5"/>
-      <c r="I48" s="4"/>
-      <c r="J48" s="4"/>
-      <c r="K48" s="4"/>
-      <c r="L48" s="4"/>
-      <c r="M48" s="4"/>
-      <c r="N48" s="4"/>
-      <c r="O48" s="4"/>
-      <c r="P48" s="4"/>
-      <c r="Q48" s="4"/>
-      <c r="R48" s="4"/>
-    </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A49" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B50" s="8"/>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A51" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1"/>
+      <c r="I52" s="1"/>
+      <c r="J52" s="1"/>
+      <c r="K52" s="1"/>
+      <c r="L52" s="1"/>
+      <c r="M52" s="1"/>
+      <c r="N52" s="1"/>
+      <c r="O52" s="1"/>
+      <c r="P52" s="1"/>
+      <c r="Q52" s="1"/>
+      <c r="R52" s="1"/>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B53" s="3"/>
+      <c r="C53" s="11"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
+      <c r="F53" s="3"/>
+      <c r="G53" s="3"/>
+      <c r="H53" s="3"/>
+      <c r="I53" s="2"/>
+      <c r="J53" s="2"/>
+      <c r="K53" s="2"/>
+      <c r="L53" s="2"/>
+      <c r="M53" s="2"/>
+      <c r="N53" s="2"/>
+      <c r="O53" s="2"/>
+      <c r="P53" s="2"/>
+      <c r="Q53" s="2"/>
+      <c r="R53" s="2"/>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C54" s="10"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="5"/>
+      <c r="F54" s="5"/>
+      <c r="G54" s="5"/>
+      <c r="H54" s="5"/>
+      <c r="I54" s="4"/>
+      <c r="J54" s="4"/>
+      <c r="K54" s="4"/>
+      <c r="L54" s="4"/>
+      <c r="M54" s="4"/>
+      <c r="N54" s="4"/>
+      <c r="O54" s="4"/>
+      <c r="P54" s="4"/>
+      <c r="Q54" s="4"/>
+      <c r="R54" s="4"/>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A57" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A58" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B58" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A59" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B59" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F60" s="1"/>
+      <c r="G60" s="1"/>
+      <c r="H60" s="1"/>
+      <c r="I60" s="1"/>
+      <c r="J60" s="1"/>
+      <c r="K60" s="1"/>
+      <c r="L60" s="1"/>
+      <c r="M60" s="1"/>
+      <c r="N60" s="1"/>
+      <c r="O60" s="1"/>
+      <c r="P60" s="1"/>
+      <c r="Q60" s="1"/>
+      <c r="R60" s="1"/>
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B61" s="3"/>
+      <c r="C61" s="9"/>
+      <c r="D61" s="3"/>
+      <c r="E61" s="3"/>
+      <c r="F61" s="3"/>
+      <c r="G61" s="3"/>
+      <c r="H61" s="3"/>
+      <c r="I61" s="2"/>
+      <c r="J61" s="2"/>
+      <c r="K61" s="2"/>
+      <c r="L61" s="2"/>
+      <c r="M61" s="2"/>
+      <c r="N61" s="2"/>
+      <c r="O61" s="2"/>
+      <c r="P61" s="2"/>
+      <c r="Q61" s="2"/>
+      <c r="R61" s="2"/>
+    </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A62" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C62" s="10"/>
+      <c r="D62" s="5"/>
+      <c r="E62" s="5"/>
+      <c r="F62" s="5"/>
+      <c r="G62" s="5"/>
+      <c r="H62" s="5"/>
+      <c r="I62" s="4"/>
+      <c r="J62" s="4"/>
+      <c r="K62" s="4"/>
+      <c r="L62" s="4"/>
+      <c r="M62" s="4"/>
+      <c r="N62" s="4"/>
+      <c r="O62" s="4"/>
+      <c r="P62" s="4"/>
+      <c r="Q62" s="4"/>
+      <c r="R62" s="4"/>
+    </row>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A65" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B50" s="8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A51" s="7" t="s">
+      <c r="B65" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A66" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B51" s="8"/>
-    </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A52" s="7" t="s">
+      <c r="B66" s="8"/>
+    </row>
+    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A67" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B52" s="8" t="s">
+      <c r="B67" s="8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A53" s="1" t="s">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B68" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C68" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="D68" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E53" s="1" t="s">
+      <c r="E68" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
-      <c r="H53" s="1"/>
-      <c r="I53" s="1"/>
-      <c r="J53" s="1"/>
-      <c r="K53" s="1"/>
-      <c r="L53" s="1"/>
-      <c r="M53" s="1"/>
-      <c r="N53" s="1"/>
-      <c r="O53" s="1"/>
-      <c r="P53" s="1"/>
-      <c r="Q53" s="1"/>
-      <c r="R53" s="1"/>
-    </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A54" s="2" t="s">
+      <c r="F68" s="1"/>
+      <c r="G68" s="1"/>
+      <c r="H68" s="1"/>
+      <c r="I68" s="1"/>
+      <c r="J68" s="1"/>
+      <c r="K68" s="1"/>
+      <c r="L68" s="1"/>
+      <c r="M68" s="1"/>
+      <c r="N68" s="1"/>
+      <c r="O68" s="1"/>
+      <c r="P68" s="1"/>
+      <c r="Q68" s="1"/>
+      <c r="R68" s="1"/>
+    </row>
+    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B54" s="3"/>
-      <c r="C54" s="11"/>
-      <c r="D54" s="3"/>
-      <c r="E54" s="3"/>
-      <c r="F54" s="3"/>
-      <c r="G54" s="3"/>
-      <c r="H54" s="3"/>
-      <c r="I54" s="2"/>
-      <c r="J54" s="2"/>
-      <c r="K54" s="2"/>
-      <c r="L54" s="2"/>
-      <c r="M54" s="2"/>
-      <c r="N54" s="2"/>
-      <c r="O54" s="2"/>
-      <c r="P54" s="2"/>
-      <c r="Q54" s="2"/>
-      <c r="R54" s="2"/>
-    </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A55" s="4" t="s">
+      <c r="B69" s="3"/>
+      <c r="C69" s="3"/>
+      <c r="D69" s="3"/>
+      <c r="E69" s="3"/>
+      <c r="F69" s="3"/>
+      <c r="G69" s="3"/>
+      <c r="H69" s="3"/>
+      <c r="I69" s="2"/>
+      <c r="J69" s="2"/>
+      <c r="K69" s="2"/>
+      <c r="L69" s="2"/>
+      <c r="M69" s="2"/>
+      <c r="N69" s="2"/>
+      <c r="O69" s="2"/>
+      <c r="P69" s="2"/>
+      <c r="Q69" s="2"/>
+      <c r="R69" s="2"/>
+    </row>
+    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A70" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C70" s="10"/>
+      <c r="D70" s="5"/>
+      <c r="E70" s="10"/>
+      <c r="F70" s="5"/>
+      <c r="G70" s="5"/>
+      <c r="H70" s="5"/>
+      <c r="I70" s="4"/>
+      <c r="J70" s="4"/>
+      <c r="K70" s="4"/>
+      <c r="L70" s="4"/>
+      <c r="M70" s="4"/>
+      <c r="N70" s="4"/>
+      <c r="O70" s="4"/>
+      <c r="P70" s="4"/>
+      <c r="Q70" s="4"/>
+      <c r="R70" s="4"/>
+    </row>
+    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A73" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B73" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A74" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B74" s="8"/>
+    </row>
+    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A75" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B75" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D76" s="1"/>
+      <c r="E76" s="1"/>
+      <c r="F76" s="1"/>
+      <c r="G76" s="1"/>
+      <c r="H76" s="1"/>
+      <c r="I76" s="1"/>
+      <c r="J76" s="1"/>
+      <c r="K76" s="1"/>
+      <c r="L76" s="1"/>
+      <c r="M76" s="1"/>
+      <c r="N76" s="1"/>
+      <c r="O76" s="1"/>
+      <c r="P76" s="1"/>
+      <c r="Q76" s="1"/>
+      <c r="R76" s="1"/>
+    </row>
+    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B77" s="3"/>
+      <c r="C77" s="3"/>
+      <c r="D77" s="3"/>
+      <c r="E77" s="3"/>
+      <c r="F77" s="3"/>
+      <c r="G77" s="3"/>
+      <c r="H77" s="3"/>
+      <c r="I77" s="2"/>
+      <c r="J77" s="2"/>
+      <c r="K77" s="2"/>
+      <c r="L77" s="2"/>
+      <c r="M77" s="2"/>
+      <c r="N77" s="2"/>
+      <c r="O77" s="2"/>
+      <c r="P77" s="2"/>
+      <c r="Q77" s="2"/>
+      <c r="R77" s="2"/>
+    </row>
+    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A78" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B55" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C55" s="10"/>
-      <c r="D55" s="5"/>
-      <c r="E55" s="5"/>
-      <c r="F55" s="5"/>
-      <c r="G55" s="5"/>
-      <c r="H55" s="5"/>
-      <c r="I55" s="4"/>
-      <c r="J55" s="4"/>
-      <c r="K55" s="4"/>
-      <c r="L55" s="4"/>
-      <c r="M55" s="4"/>
-      <c r="N55" s="4"/>
-      <c r="O55" s="4"/>
-      <c r="P55" s="4"/>
-      <c r="Q55" s="4"/>
-      <c r="R55" s="4"/>
-    </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A58" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B58" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A59" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B59" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A60" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B60" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A61" s="1" t="s">
+      <c r="B78" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C78" s="10">
+        <v>1</v>
+      </c>
+      <c r="D78" s="5"/>
+      <c r="E78" s="5"/>
+      <c r="F78" s="5"/>
+      <c r="G78" s="5"/>
+      <c r="H78" s="5"/>
+      <c r="I78" s="4"/>
+      <c r="J78" s="4"/>
+      <c r="K78" s="4"/>
+      <c r="L78" s="4"/>
+      <c r="M78" s="4"/>
+      <c r="N78" s="4"/>
+      <c r="O78" s="4"/>
+      <c r="P78" s="4"/>
+      <c r="Q78" s="4"/>
+      <c r="R78" s="4"/>
+    </row>
+    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A81" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B81" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A82" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B82" s="8"/>
+    </row>
+    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A83" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B83" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B84" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="C84" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D61" s="1" t="s">
+      <c r="D84" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E61" s="1" t="s">
+      <c r="E84" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F61" s="1"/>
-      <c r="G61" s="1"/>
-      <c r="H61" s="1"/>
-      <c r="I61" s="1"/>
-      <c r="J61" s="1"/>
-      <c r="K61" s="1"/>
-      <c r="L61" s="1"/>
-      <c r="M61" s="1"/>
-      <c r="N61" s="1"/>
-      <c r="O61" s="1"/>
-      <c r="P61" s="1"/>
-      <c r="Q61" s="1"/>
-      <c r="R61" s="1"/>
-    </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A62" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B62" s="3"/>
-      <c r="C62" s="9"/>
-      <c r="D62" s="3"/>
-      <c r="E62" s="3"/>
-      <c r="F62" s="3"/>
-      <c r="G62" s="3"/>
-      <c r="H62" s="3"/>
-      <c r="I62" s="2"/>
-      <c r="J62" s="2"/>
-      <c r="K62" s="2"/>
-      <c r="L62" s="2"/>
-      <c r="M62" s="2"/>
-      <c r="N62" s="2"/>
-      <c r="O62" s="2"/>
-      <c r="P62" s="2"/>
-      <c r="Q62" s="2"/>
-      <c r="R62" s="2"/>
-    </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A63" s="4" t="s">
+      <c r="F84" s="1"/>
+      <c r="G84" s="1"/>
+      <c r="H84" s="1"/>
+      <c r="I84" s="1"/>
+      <c r="J84" s="1"/>
+      <c r="K84" s="1"/>
+      <c r="L84" s="1"/>
+      <c r="M84" s="1"/>
+      <c r="N84" s="1"/>
+      <c r="O84" s="1"/>
+      <c r="P84" s="1"/>
+      <c r="Q84" s="1"/>
+      <c r="R84" s="1"/>
+    </row>
+    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A85" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C85" s="11">
+        <v>1</v>
+      </c>
+      <c r="D85" s="3"/>
+      <c r="E85" s="3"/>
+      <c r="F85" s="3"/>
+      <c r="G85" s="3"/>
+      <c r="H85" s="3"/>
+      <c r="I85" s="2"/>
+      <c r="J85" s="2"/>
+      <c r="K85" s="2"/>
+      <c r="L85" s="2"/>
+      <c r="M85" s="2"/>
+      <c r="N85" s="2"/>
+      <c r="O85" s="2"/>
+      <c r="P85" s="2"/>
+      <c r="Q85" s="2"/>
+      <c r="R85" s="2"/>
+    </row>
+    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A86" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B63" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C63" s="10"/>
-      <c r="D63" s="5"/>
-      <c r="E63" s="5"/>
-      <c r="F63" s="5"/>
-      <c r="G63" s="5"/>
-      <c r="H63" s="5"/>
-      <c r="I63" s="4"/>
-      <c r="J63" s="4"/>
-      <c r="K63" s="4"/>
-      <c r="L63" s="4"/>
-      <c r="M63" s="4"/>
-      <c r="N63" s="4"/>
-      <c r="O63" s="4"/>
-      <c r="P63" s="4"/>
-      <c r="Q63" s="4"/>
-      <c r="R63" s="4"/>
-    </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A66" s="7" t="s">
+      <c r="B86" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C86" s="10">
+        <v>1</v>
+      </c>
+      <c r="D86" s="5"/>
+      <c r="E86" s="5"/>
+      <c r="F86" s="5"/>
+      <c r="G86" s="5"/>
+      <c r="H86" s="5"/>
+      <c r="I86" s="4"/>
+      <c r="J86" s="4"/>
+      <c r="K86" s="4"/>
+      <c r="L86" s="4"/>
+      <c r="M86" s="4"/>
+      <c r="N86" s="4"/>
+      <c r="O86" s="4"/>
+      <c r="P86" s="4"/>
+      <c r="Q86" s="4"/>
+      <c r="R86" s="4"/>
+    </row>
+    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A89" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B66" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A67" s="7" t="s">
+      <c r="B89" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A90" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B67" s="8"/>
-    </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A68" s="7" t="s">
+      <c r="B90" s="8"/>
+    </row>
+    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A91" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B68" s="8" t="s">
+      <c r="B91" s="8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A69" s="1" t="s">
+    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="B92" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C69" s="1" t="s">
+      <c r="C92" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D69" s="1" t="s">
+      <c r="D92" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E69" s="1" t="s">
+      <c r="E92" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F69" s="1"/>
-      <c r="G69" s="1"/>
-      <c r="H69" s="1"/>
-      <c r="I69" s="1"/>
-      <c r="J69" s="1"/>
-      <c r="K69" s="1"/>
-      <c r="L69" s="1"/>
-      <c r="M69" s="1"/>
-      <c r="N69" s="1"/>
-      <c r="O69" s="1"/>
-      <c r="P69" s="1"/>
-      <c r="Q69" s="1"/>
-      <c r="R69" s="1"/>
-    </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A70" s="2" t="s">
+      <c r="F92" s="1"/>
+      <c r="G92" s="1"/>
+      <c r="H92" s="1"/>
+      <c r="I92" s="1"/>
+      <c r="J92" s="1"/>
+      <c r="K92" s="1"/>
+      <c r="L92" s="1"/>
+      <c r="M92" s="1"/>
+      <c r="N92" s="1"/>
+      <c r="O92" s="1"/>
+      <c r="P92" s="1"/>
+      <c r="Q92" s="1"/>
+      <c r="R92" s="1"/>
+    </row>
+    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A93" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B70" s="3"/>
-      <c r="C70" s="3"/>
-      <c r="D70" s="3"/>
-      <c r="E70" s="3"/>
-      <c r="F70" s="3"/>
-      <c r="G70" s="3"/>
-      <c r="H70" s="3"/>
-      <c r="I70" s="2"/>
-      <c r="J70" s="2"/>
-      <c r="K70" s="2"/>
-      <c r="L70" s="2"/>
-      <c r="M70" s="2"/>
-      <c r="N70" s="2"/>
-      <c r="O70" s="2"/>
-      <c r="P70" s="2"/>
-      <c r="Q70" s="2"/>
-      <c r="R70" s="2"/>
-    </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A71" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B71" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C71" s="10"/>
-      <c r="D71" s="5"/>
-      <c r="E71" s="10"/>
-      <c r="F71" s="5"/>
-      <c r="G71" s="5"/>
-      <c r="H71" s="5"/>
-      <c r="I71" s="4"/>
-      <c r="J71" s="4"/>
-      <c r="K71" s="4"/>
-      <c r="L71" s="4"/>
-      <c r="M71" s="4"/>
-      <c r="N71" s="4"/>
-      <c r="O71" s="4"/>
-      <c r="P71" s="4"/>
-      <c r="Q71" s="4"/>
-      <c r="R71" s="4"/>
-    </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A74" s="7" t="s">
+      <c r="B93" s="3"/>
+      <c r="C93" s="11"/>
+      <c r="D93" s="3"/>
+      <c r="E93" s="3"/>
+      <c r="F93" s="3"/>
+      <c r="G93" s="3"/>
+      <c r="H93" s="3"/>
+      <c r="I93" s="2"/>
+      <c r="J93" s="2"/>
+      <c r="K93" s="2"/>
+      <c r="L93" s="2"/>
+      <c r="M93" s="2"/>
+      <c r="N93" s="2"/>
+      <c r="O93" s="2"/>
+      <c r="P93" s="2"/>
+      <c r="Q93" s="2"/>
+      <c r="R93" s="2"/>
+    </row>
+    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A94" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B94" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C94" s="10">
+        <v>1</v>
+      </c>
+      <c r="D94" s="5"/>
+      <c r="E94" s="5"/>
+      <c r="F94" s="5"/>
+      <c r="G94" s="5"/>
+      <c r="H94" s="5"/>
+      <c r="I94" s="4"/>
+      <c r="J94" s="4"/>
+      <c r="K94" s="4"/>
+      <c r="L94" s="4"/>
+      <c r="M94" s="4"/>
+      <c r="N94" s="4"/>
+      <c r="O94" s="4"/>
+      <c r="P94" s="4"/>
+      <c r="Q94" s="4"/>
+      <c r="R94" s="4"/>
+    </row>
+    <row r="97" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A97" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B74" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A75" s="7" t="s">
+      <c r="B97" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="98" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A98" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B75" s="8"/>
-    </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A76" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B76" s="8" t="s">
+      <c r="B98" s="8"/>
+    </row>
+    <row r="99" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A99" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B99" s="8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A77" s="1" t="s">
+    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="B100" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C77" s="1" t="s">
+      <c r="C100" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D77" s="1"/>
-      <c r="E77" s="1"/>
-      <c r="F77" s="1"/>
-      <c r="G77" s="1"/>
-      <c r="H77" s="1"/>
-      <c r="I77" s="1"/>
-      <c r="J77" s="1"/>
-      <c r="K77" s="1"/>
-      <c r="L77" s="1"/>
-      <c r="M77" s="1"/>
-      <c r="N77" s="1"/>
-      <c r="O77" s="1"/>
-      <c r="P77" s="1"/>
-      <c r="Q77" s="1"/>
-      <c r="R77" s="1"/>
-    </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A78" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B78" s="3"/>
-      <c r="C78" s="3"/>
-      <c r="D78" s="3"/>
-      <c r="E78" s="3"/>
-      <c r="F78" s="3"/>
-      <c r="G78" s="3"/>
-      <c r="H78" s="3"/>
-      <c r="I78" s="2"/>
-      <c r="J78" s="2"/>
-      <c r="K78" s="2"/>
-      <c r="L78" s="2"/>
-      <c r="M78" s="2"/>
-      <c r="N78" s="2"/>
-      <c r="O78" s="2"/>
-      <c r="P78" s="2"/>
-      <c r="Q78" s="2"/>
-      <c r="R78" s="2"/>
-    </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A79" s="4" t="s">
+      <c r="D100" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F100" s="1"/>
+      <c r="G100" s="1"/>
+      <c r="H100" s="1"/>
+      <c r="I100" s="1"/>
+      <c r="J100" s="1"/>
+      <c r="K100" s="1"/>
+      <c r="L100" s="1"/>
+      <c r="M100" s="1"/>
+      <c r="N100" s="1"/>
+      <c r="O100" s="1"/>
+      <c r="P100" s="1"/>
+      <c r="Q100" s="1"/>
+      <c r="R100" s="1"/>
+    </row>
+    <row r="101" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A101" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B101" s="3"/>
+      <c r="C101" s="11"/>
+      <c r="D101" s="3"/>
+      <c r="E101" s="3"/>
+      <c r="F101" s="3"/>
+      <c r="G101" s="3"/>
+      <c r="H101" s="3"/>
+      <c r="I101" s="2"/>
+      <c r="J101" s="2"/>
+      <c r="K101" s="2"/>
+      <c r="L101" s="2"/>
+      <c r="M101" s="2"/>
+      <c r="N101" s="2"/>
+      <c r="O101" s="2"/>
+      <c r="P101" s="2"/>
+      <c r="Q101" s="2"/>
+      <c r="R101" s="2"/>
+    </row>
+    <row r="102" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A102" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B79" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C79" s="10"/>
-      <c r="D79" s="5"/>
-      <c r="E79" s="5"/>
-      <c r="F79" s="5"/>
-      <c r="G79" s="5"/>
-      <c r="H79" s="5"/>
-      <c r="I79" s="4"/>
-      <c r="J79" s="4"/>
-      <c r="K79" s="4"/>
-      <c r="L79" s="4"/>
-      <c r="M79" s="4"/>
-      <c r="N79" s="4"/>
-      <c r="O79" s="4"/>
-      <c r="P79" s="4"/>
-      <c r="Q79" s="4"/>
-      <c r="R79" s="4"/>
-    </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A82" s="7" t="s">
+      <c r="B102" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C102" s="10"/>
+      <c r="D102" s="5"/>
+      <c r="E102" s="5"/>
+      <c r="F102" s="5"/>
+      <c r="G102" s="5"/>
+      <c r="H102" s="5"/>
+      <c r="I102" s="4"/>
+      <c r="J102" s="4"/>
+      <c r="K102" s="4"/>
+      <c r="L102" s="4"/>
+      <c r="M102" s="4"/>
+      <c r="N102" s="4"/>
+      <c r="O102" s="4"/>
+      <c r="P102" s="4"/>
+      <c r="Q102" s="4"/>
+      <c r="R102" s="4"/>
+    </row>
+    <row r="105" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A105" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B82" s="8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A83" s="7" t="s">
+      <c r="B105" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="106" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A106" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B83" s="8"/>
-    </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A84" s="7" t="s">
+      <c r="B106" s="8"/>
+    </row>
+    <row r="107" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A107" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B84" s="8" t="s">
+      <c r="B107" s="8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A85" s="1" t="s">
+    <row r="108" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A108" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B85" s="1" t="s">
+      <c r="B108" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C85" s="1" t="s">
+      <c r="C108" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D85" s="1" t="s">
+      <c r="D108" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E85" s="1" t="s">
+      <c r="E108" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F85" s="1"/>
-      <c r="G85" s="1"/>
-      <c r="H85" s="1"/>
-      <c r="I85" s="1"/>
-      <c r="J85" s="1"/>
-      <c r="K85" s="1"/>
-      <c r="L85" s="1"/>
-      <c r="M85" s="1"/>
-      <c r="N85" s="1"/>
-      <c r="O85" s="1"/>
-      <c r="P85" s="1"/>
-      <c r="Q85" s="1"/>
-      <c r="R85" s="1"/>
-    </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A86" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B86" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C86" s="11">
-        <v>1</v>
-      </c>
-      <c r="D86" s="3"/>
-      <c r="E86" s="3"/>
-      <c r="F86" s="3"/>
-      <c r="G86" s="3"/>
-      <c r="H86" s="3"/>
-      <c r="I86" s="2"/>
-      <c r="J86" s="2"/>
-      <c r="K86" s="2"/>
-      <c r="L86" s="2"/>
-      <c r="M86" s="2"/>
-      <c r="N86" s="2"/>
-      <c r="O86" s="2"/>
-      <c r="P86" s="2"/>
-      <c r="Q86" s="2"/>
-      <c r="R86" s="2"/>
-    </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A87" s="4" t="s">
+      <c r="F108" s="1"/>
+      <c r="G108" s="1"/>
+      <c r="H108" s="1"/>
+      <c r="I108" s="1"/>
+      <c r="J108" s="1"/>
+      <c r="K108" s="1"/>
+      <c r="L108" s="1"/>
+      <c r="M108" s="1"/>
+      <c r="N108" s="1"/>
+      <c r="O108" s="1"/>
+      <c r="P108" s="1"/>
+      <c r="Q108" s="1"/>
+      <c r="R108" s="1"/>
+    </row>
+    <row r="109" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A109" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B109" s="3"/>
+      <c r="C109" s="11"/>
+      <c r="D109" s="3"/>
+      <c r="E109" s="3"/>
+      <c r="F109" s="3"/>
+      <c r="G109" s="3"/>
+      <c r="H109" s="3"/>
+      <c r="I109" s="2"/>
+      <c r="J109" s="2"/>
+      <c r="K109" s="2"/>
+      <c r="L109" s="2"/>
+      <c r="M109" s="2"/>
+      <c r="N109" s="2"/>
+      <c r="O109" s="2"/>
+      <c r="P109" s="2"/>
+      <c r="Q109" s="2"/>
+      <c r="R109" s="2"/>
+    </row>
+    <row r="110" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A110" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B87" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C87" s="10">
-        <v>1</v>
-      </c>
-      <c r="D87" s="5"/>
-      <c r="E87" s="5"/>
-      <c r="F87" s="5"/>
-      <c r="G87" s="5"/>
-      <c r="H87" s="5"/>
-      <c r="I87" s="4"/>
-      <c r="J87" s="4"/>
-      <c r="K87" s="4"/>
-      <c r="L87" s="4"/>
-      <c r="M87" s="4"/>
-      <c r="N87" s="4"/>
-      <c r="O87" s="4"/>
-      <c r="P87" s="4"/>
-      <c r="Q87" s="4"/>
-      <c r="R87" s="4"/>
-    </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A90" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B90" s="8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A91" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B91" s="8"/>
-    </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A92" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B92" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="93" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A93" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D93" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E93" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F93" s="1"/>
-      <c r="G93" s="1"/>
-      <c r="H93" s="1"/>
-      <c r="I93" s="1"/>
-      <c r="J93" s="1"/>
-      <c r="K93" s="1"/>
-      <c r="L93" s="1"/>
-      <c r="M93" s="1"/>
-      <c r="N93" s="1"/>
-      <c r="O93" s="1"/>
-      <c r="P93" s="1"/>
-      <c r="Q93" s="1"/>
-      <c r="R93" s="1"/>
-    </row>
-    <row r="94" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A94" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B94" s="3"/>
-      <c r="C94" s="11"/>
-      <c r="D94" s="3"/>
-      <c r="E94" s="3"/>
-      <c r="F94" s="3"/>
-      <c r="G94" s="3"/>
-      <c r="H94" s="3"/>
-      <c r="I94" s="2"/>
-      <c r="J94" s="2"/>
-      <c r="K94" s="2"/>
-      <c r="L94" s="2"/>
-      <c r="M94" s="2"/>
-      <c r="N94" s="2"/>
-      <c r="O94" s="2"/>
-      <c r="P94" s="2"/>
-      <c r="Q94" s="2"/>
-      <c r="R94" s="2"/>
-    </row>
-    <row r="95" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A95" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B95" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C95" s="10">
-        <v>1</v>
-      </c>
-      <c r="D95" s="5"/>
-      <c r="E95" s="5"/>
-      <c r="F95" s="5"/>
-      <c r="G95" s="5"/>
-      <c r="H95" s="5"/>
-      <c r="I95" s="4"/>
-      <c r="J95" s="4"/>
-      <c r="K95" s="4"/>
-      <c r="L95" s="4"/>
-      <c r="M95" s="4"/>
-      <c r="N95" s="4"/>
-      <c r="O95" s="4"/>
-      <c r="P95" s="4"/>
-      <c r="Q95" s="4"/>
-      <c r="R95" s="4"/>
-    </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A98" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B98" s="8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A99" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B99" s="8"/>
-    </row>
-    <row r="100" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A100" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B100" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="101" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A101" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C101" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D101" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E101" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F101" s="1"/>
-      <c r="G101" s="1"/>
-      <c r="H101" s="1"/>
-      <c r="I101" s="1"/>
-      <c r="J101" s="1"/>
-      <c r="K101" s="1"/>
-      <c r="L101" s="1"/>
-      <c r="M101" s="1"/>
-      <c r="N101" s="1"/>
-      <c r="O101" s="1"/>
-      <c r="P101" s="1"/>
-      <c r="Q101" s="1"/>
-      <c r="R101" s="1"/>
-    </row>
-    <row r="102" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A102" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B102" s="3"/>
-      <c r="C102" s="11"/>
-      <c r="D102" s="3"/>
-      <c r="E102" s="3"/>
-      <c r="F102" s="3"/>
-      <c r="G102" s="3"/>
-      <c r="H102" s="3"/>
-      <c r="I102" s="2"/>
-      <c r="J102" s="2"/>
-      <c r="K102" s="2"/>
-      <c r="L102" s="2"/>
-      <c r="M102" s="2"/>
-      <c r="N102" s="2"/>
-      <c r="O102" s="2"/>
-      <c r="P102" s="2"/>
-      <c r="Q102" s="2"/>
-      <c r="R102" s="2"/>
-    </row>
-    <row r="103" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A103" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B103" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C103" s="10"/>
-      <c r="D103" s="5"/>
-      <c r="E103" s="5"/>
-      <c r="F103" s="5"/>
-      <c r="G103" s="5"/>
-      <c r="H103" s="5"/>
-      <c r="I103" s="4"/>
-      <c r="J103" s="4"/>
-      <c r="K103" s="4"/>
-      <c r="L103" s="4"/>
-      <c r="M103" s="4"/>
-      <c r="N103" s="4"/>
-      <c r="O103" s="4"/>
-      <c r="P103" s="4"/>
-      <c r="Q103" s="4"/>
-      <c r="R103" s="4"/>
-    </row>
-    <row r="106" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A106" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B106" s="8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="107" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A107" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B107" s="8"/>
-    </row>
-    <row r="108" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A108" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B108" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="109" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A109" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B109" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C109" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D109" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E109" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F109" s="1"/>
-      <c r="G109" s="1"/>
-      <c r="H109" s="1"/>
-      <c r="I109" s="1"/>
-      <c r="J109" s="1"/>
-      <c r="K109" s="1"/>
-      <c r="L109" s="1"/>
-      <c r="M109" s="1"/>
-      <c r="N109" s="1"/>
-      <c r="O109" s="1"/>
-      <c r="P109" s="1"/>
-      <c r="Q109" s="1"/>
-      <c r="R109" s="1"/>
-    </row>
-    <row r="110" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A110" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B110" s="3"/>
-      <c r="C110" s="11"/>
-      <c r="D110" s="3"/>
-      <c r="E110" s="3"/>
-      <c r="F110" s="3"/>
-      <c r="G110" s="3"/>
-      <c r="H110" s="3"/>
-      <c r="I110" s="2"/>
-      <c r="J110" s="2"/>
-      <c r="K110" s="2"/>
-      <c r="L110" s="2"/>
-      <c r="M110" s="2"/>
-      <c r="N110" s="2"/>
-      <c r="O110" s="2"/>
-      <c r="P110" s="2"/>
-      <c r="Q110" s="2"/>
-      <c r="R110" s="2"/>
-    </row>
-    <row r="111" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A111" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B111" s="5" t="s">
+      <c r="B110" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C111" s="10"/>
-      <c r="D111" s="5"/>
-      <c r="E111" s="5"/>
-      <c r="F111" s="5"/>
-      <c r="G111" s="5"/>
-      <c r="H111" s="5"/>
-      <c r="I111" s="4"/>
-      <c r="J111" s="4"/>
-      <c r="K111" s="4"/>
-      <c r="L111" s="4"/>
-      <c r="M111" s="4"/>
-      <c r="N111" s="4"/>
-      <c r="O111" s="4"/>
-      <c r="P111" s="4"/>
-      <c r="Q111" s="4"/>
-      <c r="R111" s="4"/>
-    </row>
-    <row r="113" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+      <c r="C110" s="10"/>
+      <c r="D110" s="5"/>
+      <c r="E110" s="5"/>
+      <c r="F110" s="5"/>
+      <c r="G110" s="5"/>
+      <c r="H110" s="5"/>
+      <c r="I110" s="4"/>
+      <c r="J110" s="4"/>
+      <c r="K110" s="4"/>
+      <c r="L110" s="4"/>
+      <c r="M110" s="4"/>
+      <c r="N110" s="4"/>
+      <c r="O110" s="4"/>
+      <c r="P110" s="4"/>
+      <c r="Q110" s="4"/>
+      <c r="R110" s="4"/>
+    </row>
+    <row r="112" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
check-in: 20200519 zhongshu_wangge.xlsx update
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="55">
   <si>
     <t>交易品种：</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -233,10 +233,6 @@
   </si>
   <si>
     <t>0.783/0.805</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>pending</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -645,8 +641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C81" sqref="C81"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C113" sqref="C113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -1151,9 +1147,7 @@
       <c r="B39" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C39" s="10" t="s">
-        <v>55</v>
-      </c>
+      <c r="C39" s="10"/>
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
@@ -1641,9 +1635,7 @@
       <c r="B78" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C78" s="10">
-        <v>1</v>
-      </c>
+      <c r="C78" s="10"/>
       <c r="D78" s="5"/>
       <c r="E78" s="5"/>
       <c r="F78" s="5"/>

</xml_diff>

<commit_message>
check-in: 20200520 zhongshu_wangge.xlsx update
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30690" windowHeight="11850"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30696" windowHeight="11856"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -235,7 +235,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0_);\(0\)"/>
   </numFmts>
@@ -349,7 +349,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -637,22 +637,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C87" sqref="C87"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C88" sqref="C88"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.75" customWidth="1"/>
-    <col min="2" max="2" width="25.125" customWidth="1"/>
-    <col min="3" max="3" width="23.125" customWidth="1"/>
-    <col min="4" max="4" width="21.5" customWidth="1"/>
+    <col min="1" max="1" width="17.77734375" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="21.75" customWidth="1"/>
-    <col min="7" max="8" width="19.5" customWidth="1"/>
+    <col min="6" max="6" width="21.77734375" customWidth="1"/>
+    <col min="7" max="8" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="25.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="25.8" x14ac:dyDescent="0.4">
       <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
@@ -666,7 +666,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
@@ -674,7 +674,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>32</v>
       </c>
@@ -682,7 +682,7 @@
         <v>5700</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>12</v>
       </c>
@@ -690,7 +690,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -720,7 +720,7 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>27</v>
       </c>
@@ -742,7 +742,7 @@
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
@@ -766,7 +766,7 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>0</v>
       </c>
@@ -774,7 +774,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>32</v>
       </c>
@@ -782,7 +782,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>12</v>
       </c>
@@ -790,7 +790,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
@@ -820,7 +820,7 @@
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>24</v>
       </c>
@@ -842,7 +842,7 @@
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>7</v>
       </c>
@@ -866,7 +866,7 @@
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>0</v>
       </c>
@@ -874,13 +874,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B19" s="8"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>12</v>
       </c>
@@ -888,7 +888,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>6</v>
       </c>
@@ -918,7 +918,7 @@
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>24</v>
       </c>
@@ -940,7 +940,7 @@
       <c r="Q22" s="2"/>
       <c r="R22" s="2"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>7</v>
       </c>
@@ -964,7 +964,7 @@
       <c r="Q23" s="4"/>
       <c r="R23" s="4"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>0</v>
       </c>
@@ -972,13 +972,13 @@
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>31</v>
       </c>
       <c r="B27" s="8"/>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>9</v>
       </c>
@@ -986,7 +986,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>6</v>
       </c>
@@ -1016,7 +1016,7 @@
       <c r="Q29" s="1"/>
       <c r="R29" s="1"/>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>24</v>
       </c>
@@ -1038,7 +1038,7 @@
       <c r="Q30" s="2"/>
       <c r="R30" s="2"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>7</v>
       </c>
@@ -1062,7 +1062,7 @@
       <c r="Q31" s="4"/>
       <c r="R31" s="4"/>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>0</v>
       </c>
@@ -1070,13 +1070,13 @@
         <v>49</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>31</v>
       </c>
       <c r="B35" s="8"/>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>9</v>
       </c>
@@ -1084,7 +1084,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>6</v>
       </c>
@@ -1114,7 +1114,7 @@
       <c r="Q37" s="1"/>
       <c r="R37" s="1"/>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>24</v>
       </c>
@@ -1136,7 +1136,7 @@
       <c r="Q38" s="2"/>
       <c r="R38" s="2"/>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>7</v>
       </c>
@@ -1160,7 +1160,7 @@
       <c r="Q39" s="4"/>
       <c r="R39" s="4"/>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>0</v>
       </c>
@@ -1168,13 +1168,13 @@
         <v>37</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B43" s="8"/>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
         <v>12</v>
       </c>
@@ -1182,7 +1182,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>6</v>
       </c>
@@ -1212,7 +1212,7 @@
       <c r="Q45" s="1"/>
       <c r="R45" s="1"/>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>24</v>
       </c>
@@ -1234,7 +1234,7 @@
       <c r="Q46" s="2"/>
       <c r="R46" s="2"/>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>7</v>
       </c>
@@ -1258,7 +1258,7 @@
       <c r="Q47" s="4"/>
       <c r="R47" s="4"/>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>0</v>
       </c>
@@ -1266,13 +1266,13 @@
         <v>36</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B50" s="8"/>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
         <v>12</v>
       </c>
@@ -1280,7 +1280,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>6</v>
       </c>
@@ -1310,7 +1310,7 @@
       <c r="Q52" s="1"/>
       <c r="R52" s="1"/>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>24</v>
       </c>
@@ -1332,7 +1332,7 @@
       <c r="Q53" s="2"/>
       <c r="R53" s="2"/>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>7</v>
       </c>
@@ -1356,7 +1356,7 @@
       <c r="Q54" s="4"/>
       <c r="R54" s="4"/>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
         <v>18</v>
       </c>
@@ -1364,7 +1364,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
         <v>31</v>
       </c>
@@ -1372,7 +1372,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>9</v>
       </c>
@@ -1380,7 +1380,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>6</v>
       </c>
@@ -1410,7 +1410,7 @@
       <c r="Q60" s="1"/>
       <c r="R60" s="1"/>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>8</v>
       </c>
@@ -1432,7 +1432,7 @@
       <c r="Q61" s="2"/>
       <c r="R61" s="2"/>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>7</v>
       </c>
@@ -1456,7 +1456,7 @@
       <c r="Q62" s="4"/>
       <c r="R62" s="4"/>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
         <v>0</v>
       </c>
@@ -1464,13 +1464,13 @@
         <v>19</v>
       </c>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B66" s="8"/>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
         <v>12</v>
       </c>
@@ -1478,7 +1478,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>6</v>
       </c>
@@ -1508,7 +1508,7 @@
       <c r="Q68" s="1"/>
       <c r="R68" s="1"/>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>24</v>
       </c>
@@ -1530,7 +1530,7 @@
       <c r="Q69" s="2"/>
       <c r="R69" s="2"/>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>23</v>
       </c>
@@ -1554,7 +1554,7 @@
       <c r="Q70" s="4"/>
       <c r="R70" s="4"/>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
         <v>0</v>
       </c>
@@ -1562,13 +1562,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B74" s="8"/>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A75" s="7" t="s">
         <v>15</v>
       </c>
@@ -1576,7 +1576,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>6</v>
       </c>
@@ -1602,7 +1602,7 @@
       <c r="Q76" s="1"/>
       <c r="R76" s="1"/>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>25</v>
       </c>
@@ -1624,7 +1624,7 @@
       <c r="Q77" s="2"/>
       <c r="R77" s="2"/>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
         <v>7</v>
       </c>
@@ -1648,7 +1648,7 @@
       <c r="Q78" s="4"/>
       <c r="R78" s="4"/>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
         <v>0</v>
       </c>
@@ -1656,13 +1656,13 @@
         <v>21</v>
       </c>
     </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A82" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B82" s="8"/>
     </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A83" s="7" t="s">
         <v>12</v>
       </c>
@@ -1670,7 +1670,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>6</v>
       </c>
@@ -1700,7 +1700,7 @@
       <c r="Q84" s="1"/>
       <c r="R84" s="1"/>
     </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>26</v>
       </c>
@@ -1722,14 +1722,16 @@
       <c r="Q85" s="2"/>
       <c r="R85" s="2"/>
     </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B86" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C86" s="10"/>
+      <c r="C86" s="10">
+        <v>1</v>
+      </c>
       <c r="D86" s="5"/>
       <c r="E86" s="5"/>
       <c r="F86" s="5"/>
@@ -1746,7 +1748,7 @@
       <c r="Q86" s="4"/>
       <c r="R86" s="4"/>
     </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A89" s="7" t="s">
         <v>0</v>
       </c>
@@ -1754,13 +1756,13 @@
         <v>33</v>
       </c>
     </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A90" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B90" s="8"/>
     </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A91" s="7" t="s">
         <v>12</v>
       </c>
@@ -1768,7 +1770,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>6</v>
       </c>
@@ -1798,7 +1800,7 @@
       <c r="Q92" s="1"/>
       <c r="R92" s="1"/>
     </row>
-    <row r="93" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>24</v>
       </c>
@@ -1820,7 +1822,7 @@
       <c r="Q93" s="2"/>
       <c r="R93" s="2"/>
     </row>
-    <row r="94" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
         <v>7</v>
       </c>
@@ -1846,7 +1848,7 @@
       <c r="Q94" s="4"/>
       <c r="R94" s="4"/>
     </row>
-    <row r="97" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A97" s="7" t="s">
         <v>0</v>
       </c>
@@ -1854,13 +1856,13 @@
         <v>38</v>
       </c>
     </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A98" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B98" s="8"/>
     </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A99" s="7" t="s">
         <v>12</v>
       </c>
@@ -1868,7 +1870,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="100" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>6</v>
       </c>
@@ -1898,7 +1900,7 @@
       <c r="Q100" s="1"/>
       <c r="R100" s="1"/>
     </row>
-    <row r="101" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>24</v>
       </c>
@@ -1920,7 +1922,7 @@
       <c r="Q101" s="2"/>
       <c r="R101" s="2"/>
     </row>
-    <row r="102" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
         <v>7</v>
       </c>
@@ -1944,7 +1946,7 @@
       <c r="Q102" s="4"/>
       <c r="R102" s="4"/>
     </row>
-    <row r="105" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A105" s="7" t="s">
         <v>0</v>
       </c>
@@ -1952,13 +1954,13 @@
         <v>41</v>
       </c>
     </row>
-    <row r="106" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A106" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B106" s="8"/>
     </row>
-    <row r="107" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A107" s="7" t="s">
         <v>12</v>
       </c>
@@ -1966,7 +1968,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="108" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>6</v>
       </c>
@@ -1996,7 +1998,7 @@
       <c r="Q108" s="1"/>
       <c r="R108" s="1"/>
     </row>
-    <row r="109" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="109" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>24</v>
       </c>
@@ -2018,7 +2020,7 @@
       <c r="Q109" s="2"/>
       <c r="R109" s="2"/>
     </row>
-    <row r="110" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
         <v>7</v>
       </c>
@@ -2042,7 +2044,7 @@
       <c r="Q110" s="4"/>
       <c r="R110" s="4"/>
     </row>
-    <row r="112" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="112" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
check-in: 20200522 zhongshu_wangge.xlsx update
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="55">
   <si>
     <t>交易品种：</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -229,6 +229,10 @@
   </si>
   <si>
     <t>4.09/4.23</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pending</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -637,8 +641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C88" sqref="C88"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -849,7 +853,9 @@
       <c r="B16" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C16" s="10"/>
+      <c r="C16" s="10">
+        <v>1</v>
+      </c>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
@@ -947,7 +953,9 @@
       <c r="B23" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C23" s="10"/>
+      <c r="C23" s="10">
+        <v>1</v>
+      </c>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
@@ -1045,7 +1053,9 @@
       <c r="B31" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C31" s="10"/>
+      <c r="C31" s="10">
+        <v>1</v>
+      </c>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
@@ -1439,7 +1449,9 @@
       <c r="B62" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C62" s="10"/>
+      <c r="C62" s="10">
+        <v>1</v>
+      </c>
       <c r="D62" s="5"/>
       <c r="E62" s="5"/>
       <c r="F62" s="5"/>
@@ -1631,7 +1643,9 @@
       <c r="B78" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C78" s="10"/>
+      <c r="C78" s="10">
+        <v>1</v>
+      </c>
       <c r="D78" s="5"/>
       <c r="E78" s="5"/>
       <c r="F78" s="5"/>
@@ -1729,8 +1743,8 @@
       <c r="B86" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C86" s="10">
-        <v>1</v>
+      <c r="C86" s="10" t="s">
+        <v>54</v>
       </c>
       <c r="D86" s="5"/>
       <c r="E86" s="5"/>

</xml_diff>

<commit_message>
check-in: 20200525 zhongshu_wangge.xlsx update
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30690" windowHeight="11850"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30696" windowHeight="11856"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -239,7 +239,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0_);\(0\)"/>
   </numFmts>
@@ -353,7 +353,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -641,22 +641,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C81" sqref="C81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.75" customWidth="1"/>
-    <col min="2" max="2" width="25.125" customWidth="1"/>
-    <col min="3" max="3" width="23.125" customWidth="1"/>
-    <col min="4" max="4" width="21.5" customWidth="1"/>
+    <col min="1" max="1" width="17.77734375" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="21.75" customWidth="1"/>
-    <col min="7" max="8" width="19.5" customWidth="1"/>
+    <col min="6" max="6" width="21.77734375" customWidth="1"/>
+    <col min="7" max="8" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="25.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="25.8" x14ac:dyDescent="0.4">
       <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
@@ -670,7 +670,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
@@ -678,7 +678,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>32</v>
       </c>
@@ -686,7 +686,7 @@
         <v>5700</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>12</v>
       </c>
@@ -694,7 +694,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -724,7 +724,7 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>27</v>
       </c>
@@ -746,7 +746,7 @@
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
@@ -770,7 +770,7 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>0</v>
       </c>
@@ -778,7 +778,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>32</v>
       </c>
@@ -786,7 +786,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>12</v>
       </c>
@@ -794,7 +794,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
@@ -824,7 +824,7 @@
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>24</v>
       </c>
@@ -846,7 +846,7 @@
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>7</v>
       </c>
@@ -872,7 +872,7 @@
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>0</v>
       </c>
@@ -880,13 +880,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B19" s="8"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>12</v>
       </c>
@@ -894,7 +894,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>6</v>
       </c>
@@ -924,7 +924,7 @@
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>24</v>
       </c>
@@ -946,7 +946,7 @@
       <c r="Q22" s="2"/>
       <c r="R22" s="2"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>7</v>
       </c>
@@ -972,7 +972,7 @@
       <c r="Q23" s="4"/>
       <c r="R23" s="4"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>0</v>
       </c>
@@ -980,13 +980,13 @@
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>31</v>
       </c>
       <c r="B27" s="8"/>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>9</v>
       </c>
@@ -994,7 +994,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>6</v>
       </c>
@@ -1024,7 +1024,7 @@
       <c r="Q29" s="1"/>
       <c r="R29" s="1"/>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>24</v>
       </c>
@@ -1046,7 +1046,7 @@
       <c r="Q30" s="2"/>
       <c r="R30" s="2"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>7</v>
       </c>
@@ -1072,7 +1072,7 @@
       <c r="Q31" s="4"/>
       <c r="R31" s="4"/>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>0</v>
       </c>
@@ -1080,13 +1080,13 @@
         <v>48</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>31</v>
       </c>
       <c r="B35" s="8"/>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>9</v>
       </c>
@@ -1094,7 +1094,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>6</v>
       </c>
@@ -1124,7 +1124,7 @@
       <c r="Q37" s="1"/>
       <c r="R37" s="1"/>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>24</v>
       </c>
@@ -1146,7 +1146,7 @@
       <c r="Q38" s="2"/>
       <c r="R38" s="2"/>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>7</v>
       </c>
@@ -1170,7 +1170,7 @@
       <c r="Q39" s="4"/>
       <c r="R39" s="4"/>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>0</v>
       </c>
@@ -1178,13 +1178,13 @@
         <v>37</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B43" s="8"/>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
         <v>12</v>
       </c>
@@ -1192,7 +1192,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>6</v>
       </c>
@@ -1222,7 +1222,7 @@
       <c r="Q45" s="1"/>
       <c r="R45" s="1"/>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>24</v>
       </c>
@@ -1244,7 +1244,7 @@
       <c r="Q46" s="2"/>
       <c r="R46" s="2"/>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>7</v>
       </c>
@@ -1268,7 +1268,7 @@
       <c r="Q47" s="4"/>
       <c r="R47" s="4"/>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>0</v>
       </c>
@@ -1276,13 +1276,13 @@
         <v>36</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B50" s="8"/>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
         <v>12</v>
       </c>
@@ -1290,7 +1290,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>6</v>
       </c>
@@ -1320,7 +1320,7 @@
       <c r="Q52" s="1"/>
       <c r="R52" s="1"/>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>24</v>
       </c>
@@ -1342,7 +1342,7 @@
       <c r="Q53" s="2"/>
       <c r="R53" s="2"/>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>7</v>
       </c>
@@ -1366,7 +1366,7 @@
       <c r="Q54" s="4"/>
       <c r="R54" s="4"/>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
         <v>18</v>
       </c>
@@ -1374,7 +1374,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
         <v>31</v>
       </c>
@@ -1382,7 +1382,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>9</v>
       </c>
@@ -1390,7 +1390,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>6</v>
       </c>
@@ -1420,7 +1420,7 @@
       <c r="Q60" s="1"/>
       <c r="R60" s="1"/>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>8</v>
       </c>
@@ -1442,16 +1442,14 @@
       <c r="Q61" s="2"/>
       <c r="R61" s="2"/>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B62" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C62" s="10">
-        <v>1</v>
-      </c>
+      <c r="C62" s="10"/>
       <c r="D62" s="5"/>
       <c r="E62" s="5"/>
       <c r="F62" s="5"/>
@@ -1468,7 +1466,7 @@
       <c r="Q62" s="4"/>
       <c r="R62" s="4"/>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
         <v>0</v>
       </c>
@@ -1476,13 +1474,13 @@
         <v>19</v>
       </c>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B66" s="8"/>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
         <v>12</v>
       </c>
@@ -1490,7 +1488,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>6</v>
       </c>
@@ -1520,7 +1518,7 @@
       <c r="Q68" s="1"/>
       <c r="R68" s="1"/>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>24</v>
       </c>
@@ -1542,14 +1540,16 @@
       <c r="Q69" s="2"/>
       <c r="R69" s="2"/>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B70" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C70" s="10"/>
+      <c r="C70" s="10">
+        <v>1</v>
+      </c>
       <c r="D70" s="5"/>
       <c r="E70" s="10"/>
       <c r="F70" s="5"/>
@@ -1566,7 +1566,7 @@
       <c r="Q70" s="4"/>
       <c r="R70" s="4"/>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
         <v>0</v>
       </c>
@@ -1574,13 +1574,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B74" s="8"/>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A75" s="7" t="s">
         <v>15</v>
       </c>
@@ -1588,7 +1588,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>6</v>
       </c>
@@ -1614,7 +1614,7 @@
       <c r="Q76" s="1"/>
       <c r="R76" s="1"/>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>25</v>
       </c>
@@ -1636,7 +1636,7 @@
       <c r="Q77" s="2"/>
       <c r="R77" s="2"/>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
         <v>7</v>
       </c>
@@ -1662,7 +1662,7 @@
       <c r="Q78" s="4"/>
       <c r="R78" s="4"/>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
         <v>0</v>
       </c>
@@ -1670,13 +1670,13 @@
         <v>21</v>
       </c>
     </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A82" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B82" s="8"/>
     </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A83" s="7" t="s">
         <v>12</v>
       </c>
@@ -1684,7 +1684,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>6</v>
       </c>
@@ -1714,7 +1714,7 @@
       <c r="Q84" s="1"/>
       <c r="R84" s="1"/>
     </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>26</v>
       </c>
@@ -1736,7 +1736,7 @@
       <c r="Q85" s="2"/>
       <c r="R85" s="2"/>
     </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
         <v>7</v>
       </c>
@@ -1762,7 +1762,7 @@
       <c r="Q86" s="4"/>
       <c r="R86" s="4"/>
     </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A89" s="7" t="s">
         <v>0</v>
       </c>
@@ -1770,13 +1770,13 @@
         <v>33</v>
       </c>
     </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A90" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B90" s="8"/>
     </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A91" s="7" t="s">
         <v>12</v>
       </c>
@@ -1784,7 +1784,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>6</v>
       </c>
@@ -1814,7 +1814,7 @@
       <c r="Q92" s="1"/>
       <c r="R92" s="1"/>
     </row>
-    <row r="93" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>24</v>
       </c>
@@ -1836,16 +1836,14 @@
       <c r="Q93" s="2"/>
       <c r="R93" s="2"/>
     </row>
-    <row r="94" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B94" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C94" s="10">
-        <v>1</v>
-      </c>
+      <c r="C94" s="10"/>
       <c r="D94" s="5"/>
       <c r="E94" s="5"/>
       <c r="F94" s="5"/>
@@ -1862,7 +1860,7 @@
       <c r="Q94" s="4"/>
       <c r="R94" s="4"/>
     </row>
-    <row r="97" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A97" s="7" t="s">
         <v>0</v>
       </c>
@@ -1870,13 +1868,13 @@
         <v>38</v>
       </c>
     </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A98" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B98" s="8"/>
     </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A99" s="7" t="s">
         <v>12</v>
       </c>
@@ -1884,7 +1882,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="100" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>6</v>
       </c>
@@ -1914,7 +1912,7 @@
       <c r="Q100" s="1"/>
       <c r="R100" s="1"/>
     </row>
-    <row r="101" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>24</v>
       </c>
@@ -1936,7 +1934,7 @@
       <c r="Q101" s="2"/>
       <c r="R101" s="2"/>
     </row>
-    <row r="102" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
         <v>7</v>
       </c>
@@ -1960,7 +1958,7 @@
       <c r="Q102" s="4"/>
       <c r="R102" s="4"/>
     </row>
-    <row r="105" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A105" s="7" t="s">
         <v>0</v>
       </c>
@@ -1968,13 +1966,13 @@
         <v>41</v>
       </c>
     </row>
-    <row r="106" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A106" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B106" s="8"/>
     </row>
-    <row r="107" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A107" s="7" t="s">
         <v>12</v>
       </c>
@@ -1982,7 +1980,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="108" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>6</v>
       </c>
@@ -2012,7 +2010,7 @@
       <c r="Q108" s="1"/>
       <c r="R108" s="1"/>
     </row>
-    <row r="109" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="109" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>24</v>
       </c>
@@ -2034,7 +2032,7 @@
       <c r="Q109" s="2"/>
       <c r="R109" s="2"/>
     </row>
-    <row r="110" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
         <v>7</v>
       </c>
@@ -2058,7 +2056,7 @@
       <c r="Q110" s="4"/>
       <c r="R110" s="4"/>
     </row>
-    <row r="112" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="112" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
check-in: 20200526 zhongshu_wangge.xlsx update
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30690" windowHeight="11850"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30696" windowHeight="11856"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="55">
   <si>
     <t>交易品种：</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -229,13 +229,17 @@
   </si>
   <si>
     <t>15.02/16.65</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pending</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0_);\(0\)"/>
   </numFmts>
@@ -349,7 +353,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -637,22 +641,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C88" sqref="C88"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C114" sqref="C114"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.75" customWidth="1"/>
-    <col min="2" max="2" width="25.125" customWidth="1"/>
-    <col min="3" max="3" width="23.125" customWidth="1"/>
-    <col min="4" max="4" width="21.5" customWidth="1"/>
+    <col min="1" max="1" width="17.77734375" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="21.75" customWidth="1"/>
-    <col min="7" max="8" width="19.5" customWidth="1"/>
+    <col min="6" max="6" width="21.77734375" customWidth="1"/>
+    <col min="7" max="8" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="25.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="25.8" x14ac:dyDescent="0.4">
       <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
@@ -666,7 +670,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
@@ -674,7 +678,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>32</v>
       </c>
@@ -682,7 +686,7 @@
         <v>5700</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>12</v>
       </c>
@@ -690,7 +694,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -720,7 +724,7 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>27</v>
       </c>
@@ -742,14 +746,16 @@
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="10"/>
+      <c r="C8" s="10" t="s">
+        <v>54</v>
+      </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
@@ -766,7 +772,7 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>0</v>
       </c>
@@ -774,7 +780,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>32</v>
       </c>
@@ -782,7 +788,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>12</v>
       </c>
@@ -790,7 +796,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
@@ -820,7 +826,7 @@
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>24</v>
       </c>
@@ -842,16 +848,14 @@
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C16" s="10">
-        <v>1</v>
-      </c>
+      <c r="C16" s="10"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
@@ -868,7 +872,7 @@
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>0</v>
       </c>
@@ -876,13 +880,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B19" s="8"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>12</v>
       </c>
@@ -890,7 +894,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>6</v>
       </c>
@@ -920,7 +924,7 @@
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>24</v>
       </c>
@@ -942,16 +946,14 @@
       <c r="Q22" s="2"/>
       <c r="R22" s="2"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C23" s="10">
-        <v>1</v>
-      </c>
+      <c r="C23" s="10"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
@@ -968,7 +970,7 @@
       <c r="Q23" s="4"/>
       <c r="R23" s="4"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>0</v>
       </c>
@@ -976,13 +978,13 @@
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>31</v>
       </c>
       <c r="B27" s="8"/>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>9</v>
       </c>
@@ -990,7 +992,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>6</v>
       </c>
@@ -1020,7 +1022,7 @@
       <c r="Q29" s="1"/>
       <c r="R29" s="1"/>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>24</v>
       </c>
@@ -1042,7 +1044,7 @@
       <c r="Q30" s="2"/>
       <c r="R30" s="2"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>7</v>
       </c>
@@ -1068,7 +1070,7 @@
       <c r="Q31" s="4"/>
       <c r="R31" s="4"/>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>0</v>
       </c>
@@ -1076,13 +1078,13 @@
         <v>48</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>31</v>
       </c>
       <c r="B35" s="8"/>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>9</v>
       </c>
@@ -1090,7 +1092,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>6</v>
       </c>
@@ -1120,7 +1122,7 @@
       <c r="Q37" s="1"/>
       <c r="R37" s="1"/>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>24</v>
       </c>
@@ -1142,7 +1144,7 @@
       <c r="Q38" s="2"/>
       <c r="R38" s="2"/>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>7</v>
       </c>
@@ -1166,7 +1168,7 @@
       <c r="Q39" s="4"/>
       <c r="R39" s="4"/>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>0</v>
       </c>
@@ -1174,13 +1176,13 @@
         <v>37</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B43" s="8"/>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
         <v>12</v>
       </c>
@@ -1188,7 +1190,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>6</v>
       </c>
@@ -1218,7 +1220,7 @@
       <c r="Q45" s="1"/>
       <c r="R45" s="1"/>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>24</v>
       </c>
@@ -1240,7 +1242,7 @@
       <c r="Q46" s="2"/>
       <c r="R46" s="2"/>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>7</v>
       </c>
@@ -1264,7 +1266,7 @@
       <c r="Q47" s="4"/>
       <c r="R47" s="4"/>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>0</v>
       </c>
@@ -1272,13 +1274,13 @@
         <v>36</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B50" s="8"/>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
         <v>12</v>
       </c>
@@ -1286,7 +1288,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>6</v>
       </c>
@@ -1316,7 +1318,7 @@
       <c r="Q52" s="1"/>
       <c r="R52" s="1"/>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>24</v>
       </c>
@@ -1338,7 +1340,7 @@
       <c r="Q53" s="2"/>
       <c r="R53" s="2"/>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>7</v>
       </c>
@@ -1362,7 +1364,7 @@
       <c r="Q54" s="4"/>
       <c r="R54" s="4"/>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
         <v>18</v>
       </c>
@@ -1370,7 +1372,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
         <v>31</v>
       </c>
@@ -1378,7 +1380,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>9</v>
       </c>
@@ -1386,7 +1388,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>6</v>
       </c>
@@ -1416,7 +1418,7 @@
       <c r="Q60" s="1"/>
       <c r="R60" s="1"/>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>8</v>
       </c>
@@ -1438,7 +1440,7 @@
       <c r="Q61" s="2"/>
       <c r="R61" s="2"/>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>7</v>
       </c>
@@ -1462,7 +1464,7 @@
       <c r="Q62" s="4"/>
       <c r="R62" s="4"/>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
         <v>0</v>
       </c>
@@ -1470,13 +1472,13 @@
         <v>19</v>
       </c>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B66" s="8"/>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
         <v>12</v>
       </c>
@@ -1484,7 +1486,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>6</v>
       </c>
@@ -1514,7 +1516,7 @@
       <c r="Q68" s="1"/>
       <c r="R68" s="1"/>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>24</v>
       </c>
@@ -1536,16 +1538,14 @@
       <c r="Q69" s="2"/>
       <c r="R69" s="2"/>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B70" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C70" s="10">
-        <v>1</v>
-      </c>
+      <c r="C70" s="10"/>
       <c r="D70" s="5"/>
       <c r="E70" s="10"/>
       <c r="F70" s="5"/>
@@ -1562,7 +1562,7 @@
       <c r="Q70" s="4"/>
       <c r="R70" s="4"/>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
         <v>0</v>
       </c>
@@ -1570,13 +1570,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B74" s="8"/>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A75" s="7" t="s">
         <v>15</v>
       </c>
@@ -1584,7 +1584,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>6</v>
       </c>
@@ -1610,7 +1610,7 @@
       <c r="Q76" s="1"/>
       <c r="R76" s="1"/>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>25</v>
       </c>
@@ -1632,7 +1632,7 @@
       <c r="Q77" s="2"/>
       <c r="R77" s="2"/>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
         <v>7</v>
       </c>
@@ -1658,7 +1658,7 @@
       <c r="Q78" s="4"/>
       <c r="R78" s="4"/>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
         <v>0</v>
       </c>
@@ -1666,13 +1666,13 @@
         <v>21</v>
       </c>
     </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A82" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B82" s="8"/>
     </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A83" s="7" t="s">
         <v>12</v>
       </c>
@@ -1680,7 +1680,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>6</v>
       </c>
@@ -1710,7 +1710,7 @@
       <c r="Q84" s="1"/>
       <c r="R84" s="1"/>
     </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>26</v>
       </c>
@@ -1732,14 +1732,16 @@
       <c r="Q85" s="2"/>
       <c r="R85" s="2"/>
     </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B86" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C86" s="10"/>
+      <c r="C86" s="10">
+        <v>1</v>
+      </c>
       <c r="D86" s="5"/>
       <c r="E86" s="5"/>
       <c r="F86" s="5"/>
@@ -1756,7 +1758,7 @@
       <c r="Q86" s="4"/>
       <c r="R86" s="4"/>
     </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A89" s="7" t="s">
         <v>0</v>
       </c>
@@ -1764,13 +1766,13 @@
         <v>33</v>
       </c>
     </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A90" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B90" s="8"/>
     </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A91" s="7" t="s">
         <v>12</v>
       </c>
@@ -1778,7 +1780,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>6</v>
       </c>
@@ -1808,7 +1810,7 @@
       <c r="Q92" s="1"/>
       <c r="R92" s="1"/>
     </row>
-    <row r="93" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>24</v>
       </c>
@@ -1830,7 +1832,7 @@
       <c r="Q93" s="2"/>
       <c r="R93" s="2"/>
     </row>
-    <row r="94" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
         <v>7</v>
       </c>
@@ -1854,7 +1856,7 @@
       <c r="Q94" s="4"/>
       <c r="R94" s="4"/>
     </row>
-    <row r="97" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A97" s="7" t="s">
         <v>0</v>
       </c>
@@ -1862,13 +1864,13 @@
         <v>38</v>
       </c>
     </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A98" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B98" s="8"/>
     </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A99" s="7" t="s">
         <v>12</v>
       </c>
@@ -1876,7 +1878,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="100" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>6</v>
       </c>
@@ -1906,7 +1908,7 @@
       <c r="Q100" s="1"/>
       <c r="R100" s="1"/>
     </row>
-    <row r="101" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>24</v>
       </c>
@@ -1928,7 +1930,7 @@
       <c r="Q101" s="2"/>
       <c r="R101" s="2"/>
     </row>
-    <row r="102" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
         <v>7</v>
       </c>
@@ -1952,7 +1954,7 @@
       <c r="Q102" s="4"/>
       <c r="R102" s="4"/>
     </row>
-    <row r="105" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A105" s="7" t="s">
         <v>0</v>
       </c>
@@ -1960,13 +1962,13 @@
         <v>41</v>
       </c>
     </row>
-    <row r="106" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A106" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B106" s="8"/>
     </row>
-    <row r="107" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A107" s="7" t="s">
         <v>12</v>
       </c>
@@ -1974,7 +1976,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="108" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>6</v>
       </c>
@@ -2004,7 +2006,7 @@
       <c r="Q108" s="1"/>
       <c r="R108" s="1"/>
     </row>
-    <row r="109" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="109" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>24</v>
       </c>
@@ -2026,7 +2028,7 @@
       <c r="Q109" s="2"/>
       <c r="R109" s="2"/>
     </row>
-    <row r="110" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
         <v>7</v>
       </c>
@@ -2050,7 +2052,7 @@
       <c r="Q110" s="4"/>
       <c r="R110" s="4"/>
     </row>
-    <row r="112" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="112" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
check-in: 20200528 zhongshu_wangge.xlsx update
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -1545,7 +1545,9 @@
       <c r="B70" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C70" s="10"/>
+      <c r="C70" s="10">
+        <v>1</v>
+      </c>
       <c r="D70" s="5"/>
       <c r="E70" s="10"/>
       <c r="F70" s="5"/>
@@ -1739,9 +1741,7 @@
       <c r="B86" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C86" s="10">
-        <v>1</v>
-      </c>
+      <c r="C86" s="10"/>
       <c r="D86" s="5"/>
       <c r="E86" s="5"/>
       <c r="F86" s="5"/>

</xml_diff>

<commit_message>
check-in: 20200529 zhongshu_wangge.xlsx update
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -641,8 +641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C114" sqref="C114"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -1545,9 +1545,7 @@
       <c r="B70" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C70" s="10">
-        <v>1</v>
-      </c>
+      <c r="C70" s="10"/>
       <c r="D70" s="5"/>
       <c r="E70" s="10"/>
       <c r="F70" s="5"/>

</xml_diff>

<commit_message>
check-in: 20200601 zhongshu_wangge.xlsx update
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30696" windowHeight="11856"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30690" windowHeight="11850"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="57">
   <si>
     <t>交易品种：</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -172,14 +172,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>0.731/0.746</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.233/0.260</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>华宝油气（162411）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -233,13 +225,29 @@
   </si>
   <si>
     <t>pending</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.362/3.454</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.293/1.329</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.791/0.832</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.266/0.277</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0_);\(0\)"/>
   </numFmts>
@@ -353,7 +361,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -641,22 +649,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R112"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D116" sqref="D116"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" customWidth="1"/>
-    <col min="2" max="2" width="25.109375" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" customWidth="1"/>
+    <col min="1" max="1" width="17.75" customWidth="1"/>
+    <col min="2" max="2" width="25.125" customWidth="1"/>
+    <col min="3" max="3" width="23.125" customWidth="1"/>
+    <col min="4" max="4" width="21.5" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="21.77734375" customWidth="1"/>
-    <col min="7" max="8" width="19.44140625" customWidth="1"/>
+    <col min="6" max="6" width="21.75" customWidth="1"/>
+    <col min="7" max="8" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="25.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:18" ht="25.5" x14ac:dyDescent="0.3">
       <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
@@ -670,7 +678,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
@@ -678,7 +686,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
         <v>32</v>
       </c>
@@ -686,7 +694,7 @@
         <v>5700</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
         <v>12</v>
       </c>
@@ -694,7 +702,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -724,7 +732,7 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>27</v>
       </c>
@@ -746,15 +754,15 @@
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
@@ -772,7 +780,7 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A11" s="7" t="s">
         <v>0</v>
       </c>
@@ -780,7 +788,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A12" s="7" t="s">
         <v>32</v>
       </c>
@@ -788,7 +796,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A13" s="7" t="s">
         <v>12</v>
       </c>
@@ -796,7 +804,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
@@ -826,7 +834,7 @@
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
         <v>24</v>
       </c>
@@ -848,12 +856,12 @@
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A16" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="5"/>
@@ -872,7 +880,7 @@
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A18" s="7" t="s">
         <v>0</v>
       </c>
@@ -880,13 +888,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A19" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B19" s="8"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A20" s="7" t="s">
         <v>12</v>
       </c>
@@ -894,7 +902,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>6</v>
       </c>
@@ -924,7 +932,7 @@
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A22" s="2" t="s">
         <v>24</v>
       </c>
@@ -946,15 +954,17 @@
       <c r="Q22" s="2"/>
       <c r="R22" s="2"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A23" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C23" s="10"/>
-      <c r="D23" s="5"/>
+      <c r="D23" s="5" t="s">
+        <v>53</v>
+      </c>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
@@ -970,21 +980,21 @@
       <c r="Q23" s="4"/>
       <c r="R23" s="4"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A26" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A27" s="7" t="s">
         <v>31</v>
       </c>
       <c r="B27" s="8"/>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A28" s="7" t="s">
         <v>9</v>
       </c>
@@ -992,7 +1002,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
         <v>6</v>
       </c>
@@ -1022,7 +1032,7 @@
       <c r="Q29" s="1"/>
       <c r="R29" s="1"/>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A30" s="2" t="s">
         <v>24</v>
       </c>
@@ -1044,17 +1054,19 @@
       <c r="Q30" s="2"/>
       <c r="R30" s="2"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A31" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C31" s="10">
         <v>1</v>
       </c>
-      <c r="D31" s="5"/>
+      <c r="D31" s="5" t="s">
+        <v>54</v>
+      </c>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
@@ -1070,21 +1082,21 @@
       <c r="Q31" s="4"/>
       <c r="R31" s="4"/>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A34" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A35" s="7" t="s">
         <v>31</v>
       </c>
       <c r="B35" s="8"/>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A36" s="7" t="s">
         <v>9</v>
       </c>
@@ -1092,7 +1104,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
         <v>6</v>
       </c>
@@ -1122,7 +1134,7 @@
       <c r="Q37" s="1"/>
       <c r="R37" s="1"/>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A38" s="2" t="s">
         <v>24</v>
       </c>
@@ -1144,12 +1156,12 @@
       <c r="Q38" s="2"/>
       <c r="R38" s="2"/>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A39" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C39" s="10"/>
       <c r="D39" s="5"/>
@@ -1168,7 +1180,7 @@
       <c r="Q39" s="4"/>
       <c r="R39" s="4"/>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A42" s="7" t="s">
         <v>0</v>
       </c>
@@ -1176,13 +1188,13 @@
         <v>37</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A43" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B43" s="8"/>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A44" s="7" t="s">
         <v>12</v>
       </c>
@@ -1190,7 +1202,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A45" s="1" t="s">
         <v>6</v>
       </c>
@@ -1220,7 +1232,7 @@
       <c r="Q45" s="1"/>
       <c r="R45" s="1"/>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A46" s="2" t="s">
         <v>24</v>
       </c>
@@ -1242,12 +1254,12 @@
       <c r="Q46" s="2"/>
       <c r="R46" s="2"/>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A47" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C47" s="10"/>
       <c r="D47" s="5"/>
@@ -1266,7 +1278,7 @@
       <c r="Q47" s="4"/>
       <c r="R47" s="4"/>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A49" s="7" t="s">
         <v>0</v>
       </c>
@@ -1274,13 +1286,13 @@
         <v>36</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A50" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B50" s="8"/>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A51" s="7" t="s">
         <v>12</v>
       </c>
@@ -1288,7 +1300,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A52" s="1" t="s">
         <v>6</v>
       </c>
@@ -1318,7 +1330,7 @@
       <c r="Q52" s="1"/>
       <c r="R52" s="1"/>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A53" s="2" t="s">
         <v>24</v>
       </c>
@@ -1340,7 +1352,7 @@
       <c r="Q53" s="2"/>
       <c r="R53" s="2"/>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A54" s="4" t="s">
         <v>7</v>
       </c>
@@ -1364,7 +1376,7 @@
       <c r="Q54" s="4"/>
       <c r="R54" s="4"/>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A57" s="7" t="s">
         <v>18</v>
       </c>
@@ -1372,7 +1384,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A58" s="7" t="s">
         <v>31</v>
       </c>
@@ -1380,7 +1392,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A59" s="7" t="s">
         <v>9</v>
       </c>
@@ -1388,7 +1400,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A60" s="1" t="s">
         <v>6</v>
       </c>
@@ -1418,7 +1430,7 @@
       <c r="Q60" s="1"/>
       <c r="R60" s="1"/>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A61" s="2" t="s">
         <v>8</v>
       </c>
@@ -1440,12 +1452,12 @@
       <c r="Q61" s="2"/>
       <c r="R61" s="2"/>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A62" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C62" s="10"/>
       <c r="D62" s="5"/>
@@ -1464,7 +1476,7 @@
       <c r="Q62" s="4"/>
       <c r="R62" s="4"/>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A65" s="7" t="s">
         <v>0</v>
       </c>
@@ -1472,13 +1484,13 @@
         <v>19</v>
       </c>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A66" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B66" s="8"/>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A67" s="7" t="s">
         <v>12</v>
       </c>
@@ -1486,7 +1498,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A68" s="1" t="s">
         <v>6</v>
       </c>
@@ -1516,7 +1528,7 @@
       <c r="Q68" s="1"/>
       <c r="R68" s="1"/>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A69" s="2" t="s">
         <v>24</v>
       </c>
@@ -1538,12 +1550,12 @@
       <c r="Q69" s="2"/>
       <c r="R69" s="2"/>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A70" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C70" s="10"/>
       <c r="D70" s="5"/>
@@ -1562,7 +1574,7 @@
       <c r="Q70" s="4"/>
       <c r="R70" s="4"/>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A73" s="7" t="s">
         <v>0</v>
       </c>
@@ -1570,13 +1582,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A74" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B74" s="8"/>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A75" s="7" t="s">
         <v>15</v>
       </c>
@@ -1584,7 +1596,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A76" s="1" t="s">
         <v>6</v>
       </c>
@@ -1610,7 +1622,7 @@
       <c r="Q76" s="1"/>
       <c r="R76" s="1"/>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A77" s="2" t="s">
         <v>25</v>
       </c>
@@ -1632,12 +1644,12 @@
       <c r="Q77" s="2"/>
       <c r="R77" s="2"/>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A78" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C78" s="10">
         <v>1</v>
@@ -1658,7 +1670,7 @@
       <c r="Q78" s="4"/>
       <c r="R78" s="4"/>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A81" s="7" t="s">
         <v>0</v>
       </c>
@@ -1666,13 +1678,13 @@
         <v>21</v>
       </c>
     </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A82" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B82" s="8"/>
     </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A83" s="7" t="s">
         <v>12</v>
       </c>
@@ -1680,7 +1692,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A84" s="1" t="s">
         <v>6</v>
       </c>
@@ -1710,7 +1722,7 @@
       <c r="Q84" s="1"/>
       <c r="R84" s="1"/>
     </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A85" s="2" t="s">
         <v>26</v>
       </c>
@@ -1732,12 +1744,12 @@
       <c r="Q85" s="2"/>
       <c r="R85" s="2"/>
     </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A86" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C86" s="10"/>
       <c r="D86" s="5"/>
@@ -1756,7 +1768,7 @@
       <c r="Q86" s="4"/>
       <c r="R86" s="4"/>
     </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A89" s="7" t="s">
         <v>0</v>
       </c>
@@ -1764,13 +1776,13 @@
         <v>33</v>
       </c>
     </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A90" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B90" s="8"/>
     </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A91" s="7" t="s">
         <v>12</v>
       </c>
@@ -1778,7 +1790,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A92" s="1" t="s">
         <v>6</v>
       </c>
@@ -1808,7 +1820,7 @@
       <c r="Q92" s="1"/>
       <c r="R92" s="1"/>
     </row>
-    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A93" s="2" t="s">
         <v>24</v>
       </c>
@@ -1830,7 +1842,7 @@
       <c r="Q93" s="2"/>
       <c r="R93" s="2"/>
     </row>
-    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A94" s="4" t="s">
         <v>7</v>
       </c>
@@ -1854,7 +1866,7 @@
       <c r="Q94" s="4"/>
       <c r="R94" s="4"/>
     </row>
-    <row r="97" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A97" s="7" t="s">
         <v>0</v>
       </c>
@@ -1862,13 +1874,13 @@
         <v>38</v>
       </c>
     </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A98" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B98" s="8"/>
     </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A99" s="7" t="s">
         <v>12</v>
       </c>
@@ -1876,7 +1888,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A100" s="1" t="s">
         <v>6</v>
       </c>
@@ -1906,7 +1918,7 @@
       <c r="Q100" s="1"/>
       <c r="R100" s="1"/>
     </row>
-    <row r="101" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A101" s="2" t="s">
         <v>24</v>
       </c>
@@ -1928,12 +1940,12 @@
       <c r="Q101" s="2"/>
       <c r="R101" s="2"/>
     </row>
-    <row r="102" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A102" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="C102" s="10"/>
       <c r="D102" s="5"/>
@@ -1952,21 +1964,21 @@
       <c r="Q102" s="4"/>
       <c r="R102" s="4"/>
     </row>
-    <row r="105" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A105" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B105" s="8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="106" spans="1:18" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="106" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A106" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B106" s="8"/>
     </row>
-    <row r="107" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A107" s="7" t="s">
         <v>12</v>
       </c>
@@ -1974,7 +1986,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="108" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A108" s="1" t="s">
         <v>6</v>
       </c>
@@ -2004,7 +2016,7 @@
       <c r="Q108" s="1"/>
       <c r="R108" s="1"/>
     </row>
-    <row r="109" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A109" s="2" t="s">
         <v>24</v>
       </c>
@@ -2026,12 +2038,12 @@
       <c r="Q109" s="2"/>
       <c r="R109" s="2"/>
     </row>
-    <row r="110" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A110" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B110" s="5" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="C110" s="10"/>
       <c r="D110" s="5"/>
@@ -2050,7 +2062,7 @@
       <c r="Q110" s="4"/>
       <c r="R110" s="4"/>
     </row>
-    <row r="112" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="112" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
check-in: 20200604 zhongshu_wangge.xlsx update
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30690" windowHeight="11850"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30696" windowHeight="11856"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="54">
   <si>
     <t>交易品种：</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -176,10 +176,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>3.499/3.536</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>2.811/2.870</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -196,10 +192,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1.336/1.354</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>纳指ETF（513100）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -224,30 +216,26 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>pending</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>3.362/3.454</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>0.791/0.832</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.266/0.277</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>1.293/1.329</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.791/0.832</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.266/0.277</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0_);\(0\)"/>
   </numFmts>
@@ -361,7 +349,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -649,22 +637,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D116" sqref="D116"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C116" sqref="C116"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.75" customWidth="1"/>
-    <col min="2" max="2" width="25.125" customWidth="1"/>
-    <col min="3" max="3" width="23.125" customWidth="1"/>
-    <col min="4" max="4" width="21.5" customWidth="1"/>
+    <col min="1" max="1" width="17.77734375" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="21.75" customWidth="1"/>
-    <col min="7" max="8" width="19.5" customWidth="1"/>
+    <col min="6" max="6" width="21.77734375" customWidth="1"/>
+    <col min="7" max="8" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="25.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="25.8" x14ac:dyDescent="0.4">
       <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
@@ -678,7 +666,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
@@ -686,7 +674,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>32</v>
       </c>
@@ -694,7 +682,7 @@
         <v>5700</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>12</v>
       </c>
@@ -702,7 +690,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -732,7 +720,7 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>27</v>
       </c>
@@ -754,16 +742,14 @@
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>52</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="C8" s="10"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
@@ -780,7 +766,7 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>0</v>
       </c>
@@ -788,7 +774,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>32</v>
       </c>
@@ -796,7 +782,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>12</v>
       </c>
@@ -804,7 +790,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
@@ -834,7 +820,7 @@
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>24</v>
       </c>
@@ -856,12 +842,12 @@
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="5"/>
@@ -880,7 +866,7 @@
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>0</v>
       </c>
@@ -888,13 +874,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B19" s="8"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>12</v>
       </c>
@@ -902,7 +888,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>6</v>
       </c>
@@ -932,7 +918,7 @@
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>24</v>
       </c>
@@ -954,17 +940,15 @@
       <c r="Q22" s="2"/>
       <c r="R22" s="2"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="C23" s="10"/>
-      <c r="D23" s="5" t="s">
-        <v>53</v>
-      </c>
+      <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
@@ -980,21 +964,21 @@
       <c r="Q23" s="4"/>
       <c r="R23" s="4"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.15">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>31</v>
       </c>
       <c r="B27" s="8"/>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>9</v>
       </c>
@@ -1002,7 +986,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>6</v>
       </c>
@@ -1032,7 +1016,7 @@
       <c r="Q29" s="1"/>
       <c r="R29" s="1"/>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>24</v>
       </c>
@@ -1054,19 +1038,15 @@
       <c r="Q30" s="2"/>
       <c r="R30" s="2"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C31" s="10">
-        <v>1</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>54</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="C31" s="10"/>
+      <c r="D31" s="5"/>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
@@ -1082,21 +1062,21 @@
       <c r="Q31" s="4"/>
       <c r="R31" s="4"/>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.15">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>31</v>
       </c>
       <c r="B35" s="8"/>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>9</v>
       </c>
@@ -1104,7 +1084,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>6</v>
       </c>
@@ -1134,7 +1114,7 @@
       <c r="Q37" s="1"/>
       <c r="R37" s="1"/>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>24</v>
       </c>
@@ -1156,12 +1136,12 @@
       <c r="Q38" s="2"/>
       <c r="R38" s="2"/>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C39" s="10"/>
       <c r="D39" s="5"/>
@@ -1180,7 +1160,7 @@
       <c r="Q39" s="4"/>
       <c r="R39" s="4"/>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>0</v>
       </c>
@@ -1188,13 +1168,13 @@
         <v>37</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B43" s="8"/>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
         <v>12</v>
       </c>
@@ -1202,7 +1182,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>6</v>
       </c>
@@ -1232,7 +1212,7 @@
       <c r="Q45" s="1"/>
       <c r="R45" s="1"/>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>24</v>
       </c>
@@ -1254,12 +1234,12 @@
       <c r="Q46" s="2"/>
       <c r="R46" s="2"/>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C47" s="10"/>
       <c r="D47" s="5"/>
@@ -1278,7 +1258,7 @@
       <c r="Q47" s="4"/>
       <c r="R47" s="4"/>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>0</v>
       </c>
@@ -1286,13 +1266,13 @@
         <v>36</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B50" s="8"/>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
         <v>12</v>
       </c>
@@ -1300,7 +1280,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>6</v>
       </c>
@@ -1330,7 +1310,7 @@
       <c r="Q52" s="1"/>
       <c r="R52" s="1"/>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>24</v>
       </c>
@@ -1352,7 +1332,7 @@
       <c r="Q53" s="2"/>
       <c r="R53" s="2"/>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>7</v>
       </c>
@@ -1376,7 +1356,7 @@
       <c r="Q54" s="4"/>
       <c r="R54" s="4"/>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
         <v>18</v>
       </c>
@@ -1384,7 +1364,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
         <v>31</v>
       </c>
@@ -1392,7 +1372,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>9</v>
       </c>
@@ -1400,7 +1380,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>6</v>
       </c>
@@ -1430,7 +1410,7 @@
       <c r="Q60" s="1"/>
       <c r="R60" s="1"/>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>8</v>
       </c>
@@ -1452,12 +1432,12 @@
       <c r="Q61" s="2"/>
       <c r="R61" s="2"/>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C62" s="10"/>
       <c r="D62" s="5"/>
@@ -1476,7 +1456,7 @@
       <c r="Q62" s="4"/>
       <c r="R62" s="4"/>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
         <v>0</v>
       </c>
@@ -1484,13 +1464,13 @@
         <v>19</v>
       </c>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B66" s="8"/>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
         <v>12</v>
       </c>
@@ -1498,7 +1478,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>6</v>
       </c>
@@ -1528,7 +1508,7 @@
       <c r="Q68" s="1"/>
       <c r="R68" s="1"/>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>24</v>
       </c>
@@ -1550,12 +1530,12 @@
       <c r="Q69" s="2"/>
       <c r="R69" s="2"/>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C70" s="10"/>
       <c r="D70" s="5"/>
@@ -1574,7 +1554,7 @@
       <c r="Q70" s="4"/>
       <c r="R70" s="4"/>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
         <v>0</v>
       </c>
@@ -1582,13 +1562,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B74" s="8"/>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A75" s="7" t="s">
         <v>15</v>
       </c>
@@ -1596,7 +1576,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>6</v>
       </c>
@@ -1622,7 +1602,7 @@
       <c r="Q76" s="1"/>
       <c r="R76" s="1"/>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>25</v>
       </c>
@@ -1644,16 +1624,14 @@
       <c r="Q77" s="2"/>
       <c r="R77" s="2"/>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C78" s="10">
-        <v>1</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="C78" s="10"/>
       <c r="D78" s="5"/>
       <c r="E78" s="5"/>
       <c r="F78" s="5"/>
@@ -1670,7 +1648,7 @@
       <c r="Q78" s="4"/>
       <c r="R78" s="4"/>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
         <v>0</v>
       </c>
@@ -1678,13 +1656,13 @@
         <v>21</v>
       </c>
     </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A82" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B82" s="8"/>
     </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A83" s="7" t="s">
         <v>12</v>
       </c>
@@ -1692,7 +1670,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>6</v>
       </c>
@@ -1722,7 +1700,7 @@
       <c r="Q84" s="1"/>
       <c r="R84" s="1"/>
     </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>26</v>
       </c>
@@ -1744,12 +1722,12 @@
       <c r="Q85" s="2"/>
       <c r="R85" s="2"/>
     </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C86" s="10"/>
       <c r="D86" s="5"/>
@@ -1768,7 +1746,7 @@
       <c r="Q86" s="4"/>
       <c r="R86" s="4"/>
     </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A89" s="7" t="s">
         <v>0</v>
       </c>
@@ -1776,13 +1754,13 @@
         <v>33</v>
       </c>
     </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A90" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B90" s="8"/>
     </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A91" s="7" t="s">
         <v>12</v>
       </c>
@@ -1790,7 +1768,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>6</v>
       </c>
@@ -1820,7 +1798,7 @@
       <c r="Q92" s="1"/>
       <c r="R92" s="1"/>
     </row>
-    <row r="93" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>24</v>
       </c>
@@ -1842,7 +1820,7 @@
       <c r="Q93" s="2"/>
       <c r="R93" s="2"/>
     </row>
-    <row r="94" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
         <v>7</v>
       </c>
@@ -1866,7 +1844,7 @@
       <c r="Q94" s="4"/>
       <c r="R94" s="4"/>
     </row>
-    <row r="97" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A97" s="7" t="s">
         <v>0</v>
       </c>
@@ -1874,13 +1852,13 @@
         <v>38</v>
       </c>
     </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A98" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B98" s="8"/>
     </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A99" s="7" t="s">
         <v>12</v>
       </c>
@@ -1888,7 +1866,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="100" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>6</v>
       </c>
@@ -1918,7 +1896,7 @@
       <c r="Q100" s="1"/>
       <c r="R100" s="1"/>
     </row>
-    <row r="101" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>24</v>
       </c>
@@ -1940,12 +1918,12 @@
       <c r="Q101" s="2"/>
       <c r="R101" s="2"/>
     </row>
-    <row r="102" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C102" s="10"/>
       <c r="D102" s="5"/>
@@ -1964,7 +1942,7 @@
       <c r="Q102" s="4"/>
       <c r="R102" s="4"/>
     </row>
-    <row r="105" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A105" s="7" t="s">
         <v>0</v>
       </c>
@@ -1972,13 +1950,13 @@
         <v>39</v>
       </c>
     </row>
-    <row r="106" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A106" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B106" s="8"/>
     </row>
-    <row r="107" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A107" s="7" t="s">
         <v>12</v>
       </c>
@@ -1986,7 +1964,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="108" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>6</v>
       </c>
@@ -2016,7 +1994,7 @@
       <c r="Q108" s="1"/>
       <c r="R108" s="1"/>
     </row>
-    <row r="109" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="109" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>24</v>
       </c>
@@ -2038,12 +2016,12 @@
       <c r="Q109" s="2"/>
       <c r="R109" s="2"/>
     </row>
-    <row r="110" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B110" s="5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C110" s="10"/>
       <c r="D110" s="5"/>
@@ -2062,7 +2040,7 @@
       <c r="Q110" s="4"/>
       <c r="R110" s="4"/>
     </row>
-    <row r="112" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="112" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
check-in: 20200610 zhongshu_wangge.xlsx update
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30696" windowHeight="11856"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30690" windowHeight="11850"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -152,10 +152,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>0.954/0.965</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>0.848/0.883</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -176,14 +172,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2.811/2.870</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>30.00/31.08</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>3.49/3.63</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -200,10 +188,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>0.783/0.805</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>4.09/4.23</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -212,14 +196,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>3.362/3.454</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.791/0.832</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>0.266/0.277</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -229,13 +205,37 @@
   </si>
   <si>
     <t>17.02/19.48</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.867/2.919</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.811/0.819</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.59/3.616</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>32.90/33.65</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.974/0.983</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.813/0.831</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0_);\(0\)"/>
   </numFmts>
@@ -349,7 +349,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -637,22 +637,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D89" sqref="D89"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C105" sqref="C105"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" customWidth="1"/>
-    <col min="2" max="2" width="25.109375" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" customWidth="1"/>
+    <col min="1" max="1" width="17.75" customWidth="1"/>
+    <col min="2" max="2" width="25.125" customWidth="1"/>
+    <col min="3" max="3" width="23.125" customWidth="1"/>
+    <col min="4" max="4" width="21.5" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="21.77734375" customWidth="1"/>
-    <col min="7" max="8" width="19.44140625" customWidth="1"/>
+    <col min="6" max="6" width="21.75" customWidth="1"/>
+    <col min="7" max="8" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="25.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:18" ht="25.5" x14ac:dyDescent="0.3">
       <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
@@ -666,7 +666,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
@@ -674,7 +674,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
         <v>32</v>
       </c>
@@ -682,7 +682,7 @@
         <v>5700</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
         <v>12</v>
       </c>
@@ -690,7 +690,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -720,7 +720,7 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>27</v>
       </c>
@@ -742,12 +742,12 @@
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="5"/>
@@ -766,7 +766,7 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A11" s="7" t="s">
         <v>0</v>
       </c>
@@ -774,7 +774,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A12" s="7" t="s">
         <v>32</v>
       </c>
@@ -782,7 +782,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A13" s="7" t="s">
         <v>12</v>
       </c>
@@ -790,7 +790,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
@@ -820,7 +820,7 @@
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
         <v>24</v>
       </c>
@@ -842,12 +842,12 @@
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A16" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="5"/>
@@ -866,7 +866,7 @@
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A18" s="7" t="s">
         <v>0</v>
       </c>
@@ -874,13 +874,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A19" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B19" s="8"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A20" s="7" t="s">
         <v>12</v>
       </c>
@@ -888,7 +888,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>6</v>
       </c>
@@ -918,7 +918,7 @@
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A22" s="2" t="s">
         <v>24</v>
       </c>
@@ -940,12 +940,12 @@
       <c r="Q22" s="2"/>
       <c r="R22" s="2"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A23" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C23" s="10"/>
       <c r="D23" s="5"/>
@@ -964,21 +964,21 @@
       <c r="Q23" s="4"/>
       <c r="R23" s="4"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A26" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A27" s="7" t="s">
         <v>31</v>
       </c>
       <c r="B27" s="8"/>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A28" s="7" t="s">
         <v>9</v>
       </c>
@@ -986,7 +986,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
         <v>6</v>
       </c>
@@ -1016,7 +1016,7 @@
       <c r="Q29" s="1"/>
       <c r="R29" s="1"/>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A30" s="2" t="s">
         <v>24</v>
       </c>
@@ -1038,12 +1038,12 @@
       <c r="Q30" s="2"/>
       <c r="R30" s="2"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A31" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C31" s="10"/>
       <c r="D31" s="5"/>
@@ -1062,21 +1062,21 @@
       <c r="Q31" s="4"/>
       <c r="R31" s="4"/>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A34" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A35" s="7" t="s">
         <v>31</v>
       </c>
       <c r="B35" s="8"/>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A36" s="7" t="s">
         <v>9</v>
       </c>
@@ -1084,7 +1084,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
         <v>6</v>
       </c>
@@ -1114,7 +1114,7 @@
       <c r="Q37" s="1"/>
       <c r="R37" s="1"/>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A38" s="2" t="s">
         <v>24</v>
       </c>
@@ -1136,12 +1136,12 @@
       <c r="Q38" s="2"/>
       <c r="R38" s="2"/>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A39" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C39" s="10"/>
       <c r="D39" s="5"/>
@@ -1160,21 +1160,21 @@
       <c r="Q39" s="4"/>
       <c r="R39" s="4"/>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A42" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A43" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B43" s="8"/>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A44" s="7" t="s">
         <v>12</v>
       </c>
@@ -1182,7 +1182,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A45" s="1" t="s">
         <v>6</v>
       </c>
@@ -1212,7 +1212,7 @@
       <c r="Q45" s="1"/>
       <c r="R45" s="1"/>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A46" s="2" t="s">
         <v>24</v>
       </c>
@@ -1234,12 +1234,12 @@
       <c r="Q46" s="2"/>
       <c r="R46" s="2"/>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A47" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C47" s="10"/>
       <c r="D47" s="5"/>
@@ -1258,21 +1258,21 @@
       <c r="Q47" s="4"/>
       <c r="R47" s="4"/>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A49" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A50" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B50" s="8"/>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A51" s="7" t="s">
         <v>12</v>
       </c>
@@ -1280,7 +1280,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A52" s="1" t="s">
         <v>6</v>
       </c>
@@ -1310,7 +1310,7 @@
       <c r="Q52" s="1"/>
       <c r="R52" s="1"/>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A53" s="2" t="s">
         <v>24</v>
       </c>
@@ -1332,12 +1332,12 @@
       <c r="Q53" s="2"/>
       <c r="R53" s="2"/>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A54" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C54" s="10"/>
       <c r="D54" s="5"/>
@@ -1356,7 +1356,7 @@
       <c r="Q54" s="4"/>
       <c r="R54" s="4"/>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A57" s="7" t="s">
         <v>18</v>
       </c>
@@ -1364,7 +1364,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A58" s="7" t="s">
         <v>31</v>
       </c>
@@ -1372,7 +1372,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A59" s="7" t="s">
         <v>9</v>
       </c>
@@ -1380,7 +1380,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A60" s="1" t="s">
         <v>6</v>
       </c>
@@ -1410,7 +1410,7 @@
       <c r="Q60" s="1"/>
       <c r="R60" s="1"/>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A61" s="2" t="s">
         <v>8</v>
       </c>
@@ -1432,12 +1432,12 @@
       <c r="Q61" s="2"/>
       <c r="R61" s="2"/>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A62" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C62" s="10">
         <v>1</v>
@@ -1458,7 +1458,7 @@
       <c r="Q62" s="4"/>
       <c r="R62" s="4"/>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A65" s="7" t="s">
         <v>0</v>
       </c>
@@ -1466,13 +1466,13 @@
         <v>19</v>
       </c>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A66" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B66" s="8"/>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A67" s="7" t="s">
         <v>12</v>
       </c>
@@ -1480,7 +1480,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A68" s="1" t="s">
         <v>6</v>
       </c>
@@ -1510,7 +1510,7 @@
       <c r="Q68" s="1"/>
       <c r="R68" s="1"/>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A69" s="2" t="s">
         <v>24</v>
       </c>
@@ -1532,12 +1532,12 @@
       <c r="Q69" s="2"/>
       <c r="R69" s="2"/>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A70" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="C70" s="10"/>
       <c r="D70" s="5"/>
@@ -1556,7 +1556,7 @@
       <c r="Q70" s="4"/>
       <c r="R70" s="4"/>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A73" s="7" t="s">
         <v>0</v>
       </c>
@@ -1564,13 +1564,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A74" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B74" s="8"/>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A75" s="7" t="s">
         <v>15</v>
       </c>
@@ -1578,7 +1578,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A76" s="1" t="s">
         <v>6</v>
       </c>
@@ -1604,7 +1604,7 @@
       <c r="Q76" s="1"/>
       <c r="R76" s="1"/>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A77" s="2" t="s">
         <v>25</v>
       </c>
@@ -1626,12 +1626,12 @@
       <c r="Q77" s="2"/>
       <c r="R77" s="2"/>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A78" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C78" s="10"/>
       <c r="D78" s="5"/>
@@ -1650,7 +1650,7 @@
       <c r="Q78" s="4"/>
       <c r="R78" s="4"/>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A81" s="7" t="s">
         <v>0</v>
       </c>
@@ -1658,13 +1658,13 @@
         <v>21</v>
       </c>
     </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A82" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B82" s="8"/>
     </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A83" s="7" t="s">
         <v>12</v>
       </c>
@@ -1672,7 +1672,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A84" s="1" t="s">
         <v>6</v>
       </c>
@@ -1702,7 +1702,7 @@
       <c r="Q84" s="1"/>
       <c r="R84" s="1"/>
     </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A85" s="2" t="s">
         <v>26</v>
       </c>
@@ -1724,12 +1724,12 @@
       <c r="Q85" s="2"/>
       <c r="R85" s="2"/>
     </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A86" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C86" s="10">
         <v>1</v>
@@ -1750,7 +1750,7 @@
       <c r="Q86" s="4"/>
       <c r="R86" s="4"/>
     </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A89" s="7" t="s">
         <v>0</v>
       </c>
@@ -1758,13 +1758,13 @@
         <v>33</v>
       </c>
     </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A90" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B90" s="8"/>
     </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A91" s="7" t="s">
         <v>12</v>
       </c>
@@ -1772,7 +1772,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A92" s="1" t="s">
         <v>6</v>
       </c>
@@ -1802,7 +1802,7 @@
       <c r="Q92" s="1"/>
       <c r="R92" s="1"/>
     </row>
-    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A93" s="2" t="s">
         <v>24</v>
       </c>
@@ -1824,12 +1824,12 @@
       <c r="Q93" s="2"/>
       <c r="R93" s="2"/>
     </row>
-    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A94" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="C94" s="10"/>
       <c r="D94" s="5"/>
@@ -1848,21 +1848,21 @@
       <c r="Q94" s="4"/>
       <c r="R94" s="4"/>
     </row>
-    <row r="97" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A97" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="98" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A98" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B98" s="8"/>
     </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A99" s="7" t="s">
         <v>12</v>
       </c>
@@ -1870,7 +1870,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A100" s="1" t="s">
         <v>6</v>
       </c>
@@ -1900,7 +1900,7 @@
       <c r="Q100" s="1"/>
       <c r="R100" s="1"/>
     </row>
-    <row r="101" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A101" s="2" t="s">
         <v>24</v>
       </c>
@@ -1922,12 +1922,12 @@
       <c r="Q101" s="2"/>
       <c r="R101" s="2"/>
     </row>
-    <row r="102" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A102" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C102" s="10"/>
       <c r="D102" s="5"/>
@@ -1946,21 +1946,21 @@
       <c r="Q102" s="4"/>
       <c r="R102" s="4"/>
     </row>
-    <row r="105" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A105" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B105" s="8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="106" spans="1:18" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="106" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A106" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B106" s="8"/>
     </row>
-    <row r="107" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A107" s="7" t="s">
         <v>12</v>
       </c>
@@ -1968,7 +1968,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="108" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A108" s="1" t="s">
         <v>6</v>
       </c>
@@ -1998,7 +1998,7 @@
       <c r="Q108" s="1"/>
       <c r="R108" s="1"/>
     </row>
-    <row r="109" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A109" s="2" t="s">
         <v>24</v>
       </c>
@@ -2020,12 +2020,12 @@
       <c r="Q109" s="2"/>
       <c r="R109" s="2"/>
     </row>
-    <row r="110" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A110" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B110" s="5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C110" s="10"/>
       <c r="D110" s="5"/>
@@ -2044,7 +2044,7 @@
       <c r="Q110" s="4"/>
       <c r="R110" s="4"/>
     </row>
-    <row r="112" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="112" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
check-in: 20200615 zhongshu_wangge.xlsx update
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30690" windowHeight="11850"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30696" windowHeight="11856"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -235,7 +235,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0_);\(0\)"/>
   </numFmts>
@@ -349,7 +349,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -637,22 +637,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C105" sqref="C105"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.75" customWidth="1"/>
-    <col min="2" max="2" width="25.125" customWidth="1"/>
-    <col min="3" max="3" width="23.125" customWidth="1"/>
-    <col min="4" max="4" width="21.5" customWidth="1"/>
+    <col min="1" max="1" width="17.77734375" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="21.75" customWidth="1"/>
-    <col min="7" max="8" width="19.5" customWidth="1"/>
+    <col min="6" max="6" width="21.77734375" customWidth="1"/>
+    <col min="7" max="8" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="25.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="25.8" x14ac:dyDescent="0.4">
       <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
@@ -666,7 +666,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
@@ -674,7 +674,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>32</v>
       </c>
@@ -682,7 +682,7 @@
         <v>5700</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>12</v>
       </c>
@@ -690,7 +690,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -720,7 +720,7 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>27</v>
       </c>
@@ -742,14 +742,16 @@
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="10"/>
+      <c r="C8" s="10">
+        <v>1</v>
+      </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
@@ -766,7 +768,7 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>0</v>
       </c>
@@ -774,7 +776,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>32</v>
       </c>
@@ -782,7 +784,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>12</v>
       </c>
@@ -790,7 +792,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
@@ -820,7 +822,7 @@
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>24</v>
       </c>
@@ -842,7 +844,7 @@
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>7</v>
       </c>
@@ -866,7 +868,7 @@
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>0</v>
       </c>
@@ -874,13 +876,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B19" s="8"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>12</v>
       </c>
@@ -888,7 +890,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>6</v>
       </c>
@@ -918,7 +920,7 @@
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>24</v>
       </c>
@@ -940,7 +942,7 @@
       <c r="Q22" s="2"/>
       <c r="R22" s="2"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>7</v>
       </c>
@@ -964,7 +966,7 @@
       <c r="Q23" s="4"/>
       <c r="R23" s="4"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>0</v>
       </c>
@@ -972,13 +974,13 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>31</v>
       </c>
       <c r="B27" s="8"/>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>9</v>
       </c>
@@ -986,7 +988,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>6</v>
       </c>
@@ -1016,7 +1018,7 @@
       <c r="Q29" s="1"/>
       <c r="R29" s="1"/>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>24</v>
       </c>
@@ -1038,7 +1040,7 @@
       <c r="Q30" s="2"/>
       <c r="R30" s="2"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>7</v>
       </c>
@@ -1062,7 +1064,7 @@
       <c r="Q31" s="4"/>
       <c r="R31" s="4"/>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>0</v>
       </c>
@@ -1070,13 +1072,13 @@
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>31</v>
       </c>
       <c r="B35" s="8"/>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>9</v>
       </c>
@@ -1084,7 +1086,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>6</v>
       </c>
@@ -1114,7 +1116,7 @@
       <c r="Q37" s="1"/>
       <c r="R37" s="1"/>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>24</v>
       </c>
@@ -1136,7 +1138,7 @@
       <c r="Q38" s="2"/>
       <c r="R38" s="2"/>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>7</v>
       </c>
@@ -1160,7 +1162,7 @@
       <c r="Q39" s="4"/>
       <c r="R39" s="4"/>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>0</v>
       </c>
@@ -1168,13 +1170,13 @@
         <v>36</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B43" s="8"/>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
         <v>12</v>
       </c>
@@ -1182,7 +1184,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>6</v>
       </c>
@@ -1212,7 +1214,7 @@
       <c r="Q45" s="1"/>
       <c r="R45" s="1"/>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>24</v>
       </c>
@@ -1234,7 +1236,7 @@
       <c r="Q46" s="2"/>
       <c r="R46" s="2"/>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>7</v>
       </c>
@@ -1258,7 +1260,7 @@
       <c r="Q47" s="4"/>
       <c r="R47" s="4"/>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>0</v>
       </c>
@@ -1266,13 +1268,13 @@
         <v>35</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B50" s="8"/>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
         <v>12</v>
       </c>
@@ -1280,7 +1282,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>6</v>
       </c>
@@ -1310,7 +1312,7 @@
       <c r="Q52" s="1"/>
       <c r="R52" s="1"/>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>24</v>
       </c>
@@ -1332,7 +1334,7 @@
       <c r="Q53" s="2"/>
       <c r="R53" s="2"/>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>7</v>
       </c>
@@ -1356,7 +1358,7 @@
       <c r="Q54" s="4"/>
       <c r="R54" s="4"/>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
         <v>18</v>
       </c>
@@ -1364,7 +1366,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
         <v>31</v>
       </c>
@@ -1372,7 +1374,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>9</v>
       </c>
@@ -1380,7 +1382,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>6</v>
       </c>
@@ -1410,7 +1412,7 @@
       <c r="Q60" s="1"/>
       <c r="R60" s="1"/>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>8</v>
       </c>
@@ -1432,7 +1434,7 @@
       <c r="Q61" s="2"/>
       <c r="R61" s="2"/>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>7</v>
       </c>
@@ -1458,7 +1460,7 @@
       <c r="Q62" s="4"/>
       <c r="R62" s="4"/>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
         <v>0</v>
       </c>
@@ -1466,13 +1468,13 @@
         <v>19</v>
       </c>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B66" s="8"/>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
         <v>12</v>
       </c>
@@ -1480,7 +1482,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>6</v>
       </c>
@@ -1510,7 +1512,7 @@
       <c r="Q68" s="1"/>
       <c r="R68" s="1"/>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>24</v>
       </c>
@@ -1532,7 +1534,7 @@
       <c r="Q69" s="2"/>
       <c r="R69" s="2"/>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>23</v>
       </c>
@@ -1556,7 +1558,7 @@
       <c r="Q70" s="4"/>
       <c r="R70" s="4"/>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
         <v>0</v>
       </c>
@@ -1564,13 +1566,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B74" s="8"/>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A75" s="7" t="s">
         <v>15</v>
       </c>
@@ -1578,7 +1580,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>6</v>
       </c>
@@ -1604,7 +1606,7 @@
       <c r="Q76" s="1"/>
       <c r="R76" s="1"/>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>25</v>
       </c>
@@ -1626,7 +1628,7 @@
       <c r="Q77" s="2"/>
       <c r="R77" s="2"/>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
         <v>7</v>
       </c>
@@ -1650,7 +1652,7 @@
       <c r="Q78" s="4"/>
       <c r="R78" s="4"/>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
         <v>0</v>
       </c>
@@ -1658,13 +1660,13 @@
         <v>21</v>
       </c>
     </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A82" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B82" s="8"/>
     </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A83" s="7" t="s">
         <v>12</v>
       </c>
@@ -1672,7 +1674,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>6</v>
       </c>
@@ -1702,7 +1704,7 @@
       <c r="Q84" s="1"/>
       <c r="R84" s="1"/>
     </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>26</v>
       </c>
@@ -1724,7 +1726,7 @@
       <c r="Q85" s="2"/>
       <c r="R85" s="2"/>
     </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
         <v>7</v>
       </c>
@@ -1750,7 +1752,7 @@
       <c r="Q86" s="4"/>
       <c r="R86" s="4"/>
     </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A89" s="7" t="s">
         <v>0</v>
       </c>
@@ -1758,13 +1760,13 @@
         <v>33</v>
       </c>
     </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A90" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B90" s="8"/>
     </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A91" s="7" t="s">
         <v>12</v>
       </c>
@@ -1772,7 +1774,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>6</v>
       </c>
@@ -1802,7 +1804,7 @@
       <c r="Q92" s="1"/>
       <c r="R92" s="1"/>
     </row>
-    <row r="93" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>24</v>
       </c>
@@ -1824,7 +1826,7 @@
       <c r="Q93" s="2"/>
       <c r="R93" s="2"/>
     </row>
-    <row r="94" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
         <v>7</v>
       </c>
@@ -1848,7 +1850,7 @@
       <c r="Q94" s="4"/>
       <c r="R94" s="4"/>
     </row>
-    <row r="97" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A97" s="7" t="s">
         <v>0</v>
       </c>
@@ -1856,13 +1858,13 @@
         <v>37</v>
       </c>
     </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A98" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B98" s="8"/>
     </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A99" s="7" t="s">
         <v>12</v>
       </c>
@@ -1870,7 +1872,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="100" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>6</v>
       </c>
@@ -1900,7 +1902,7 @@
       <c r="Q100" s="1"/>
       <c r="R100" s="1"/>
     </row>
-    <row r="101" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>24</v>
       </c>
@@ -1922,14 +1924,16 @@
       <c r="Q101" s="2"/>
       <c r="R101" s="2"/>
     </row>
-    <row r="102" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B102" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C102" s="10"/>
+      <c r="C102" s="10">
+        <v>1</v>
+      </c>
       <c r="D102" s="5"/>
       <c r="E102" s="5"/>
       <c r="F102" s="5"/>
@@ -1946,7 +1950,7 @@
       <c r="Q102" s="4"/>
       <c r="R102" s="4"/>
     </row>
-    <row r="105" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A105" s="7" t="s">
         <v>0</v>
       </c>
@@ -1954,13 +1958,13 @@
         <v>38</v>
       </c>
     </row>
-    <row r="106" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A106" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B106" s="8"/>
     </row>
-    <row r="107" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A107" s="7" t="s">
         <v>12</v>
       </c>
@@ -1968,7 +1972,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="108" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>6</v>
       </c>
@@ -1998,7 +2002,7 @@
       <c r="Q108" s="1"/>
       <c r="R108" s="1"/>
     </row>
-    <row r="109" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="109" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>24</v>
       </c>
@@ -2020,7 +2024,7 @@
       <c r="Q109" s="2"/>
       <c r="R109" s="2"/>
     </row>
-    <row r="110" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
         <v>7</v>
       </c>
@@ -2044,7 +2048,7 @@
       <c r="Q110" s="4"/>
       <c r="R110" s="4"/>
     </row>
-    <row r="112" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="112" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
check-in: 20200623 zhongshu_wangge.xlsx update
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -152,10 +152,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>0.848/0.883</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>德国30（513030）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -192,18 +188,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>0.938/0.977</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.266/0.277</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.293/1.329</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>2.867/2.919</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -229,6 +213,22 @@
   </si>
   <si>
     <t>0.970/0.983</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.287/0.312</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.977/1.041</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.048/1.069</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.364/1.394</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -637,8 +637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R112"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -747,7 +747,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C8" s="10">
         <v>1</v>
@@ -849,7 +849,7 @@
         <v>7</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="5"/>
@@ -947,7 +947,7 @@
         <v>7</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C23" s="10"/>
       <c r="D23" s="5"/>
@@ -971,7 +971,7 @@
         <v>0</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.15">
@@ -1045,7 +1045,7 @@
         <v>7</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="C31" s="10"/>
       <c r="D31" s="5"/>
@@ -1069,7 +1069,7 @@
         <v>0</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.15">
@@ -1143,7 +1143,7 @@
         <v>7</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C39" s="10"/>
       <c r="D39" s="5"/>
@@ -1167,7 +1167,7 @@
         <v>0</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.15">
@@ -1241,7 +1241,7 @@
         <v>7</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C47" s="10"/>
       <c r="D47" s="5"/>
@@ -1265,7 +1265,7 @@
         <v>0</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.15">
@@ -1339,7 +1339,7 @@
         <v>7</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="C54" s="10"/>
       <c r="D54" s="5"/>
@@ -1439,7 +1439,7 @@
         <v>7</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C62" s="10">
         <v>1</v>
@@ -1539,7 +1539,7 @@
         <v>23</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C70" s="10"/>
       <c r="D70" s="5"/>
@@ -1633,7 +1633,7 @@
         <v>7</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C78" s="10"/>
       <c r="D78" s="5"/>
@@ -1731,7 +1731,7 @@
         <v>7</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C86" s="10">
         <v>1</v>
@@ -1831,7 +1831,7 @@
         <v>7</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C94" s="10"/>
       <c r="D94" s="5"/>
@@ -1855,7 +1855,7 @@
         <v>0</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="98" spans="1:18" x14ac:dyDescent="0.15">
@@ -1929,7 +1929,7 @@
         <v>7</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C102" s="10">
         <v>1</v>
@@ -1955,7 +1955,7 @@
         <v>0</v>
       </c>
       <c r="B105" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="106" spans="1:18" x14ac:dyDescent="0.15">
@@ -2029,7 +2029,7 @@
         <v>7</v>
       </c>
       <c r="B110" s="5" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C110" s="10"/>
       <c r="D110" s="5"/>

</xml_diff>

<commit_message>
check-in: 20200702 zhongshu_wangge.xlsx update
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -204,10 +204,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>18.89/19.48</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>32.66/33.65</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -220,15 +216,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>0.977/1.041</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1.048/1.069</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>1.364/1.394</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.019/1.041</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>18.81/19.40</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -637,8 +637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C113" sqref="C113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1045,7 +1045,7 @@
         <v>7</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C31" s="10"/>
       <c r="D31" s="5"/>
@@ -1241,7 +1241,7 @@
         <v>7</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C47" s="10"/>
       <c r="D47" s="5"/>
@@ -1339,7 +1339,7 @@
         <v>7</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C54" s="10"/>
       <c r="D54" s="5"/>
@@ -1439,7 +1439,7 @@
         <v>7</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="C62" s="10">
         <v>1</v>
@@ -1539,7 +1539,7 @@
         <v>23</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C70" s="10"/>
       <c r="D70" s="5"/>
@@ -1831,7 +1831,7 @@
         <v>7</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C94" s="10"/>
       <c r="D94" s="5"/>
@@ -2029,7 +2029,7 @@
         <v>7</v>
       </c>
       <c r="B110" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C110" s="10"/>
       <c r="D110" s="5"/>

</xml_diff>

<commit_message>
check-in: 20200805 zhongshu_wangge.xlsx update
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="48">
   <si>
     <t>交易品种：</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -168,10 +168,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>3.49/3.63</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>恒生ETF（159920）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -180,39 +176,27 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>3.650/3.835</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4.09/4.23</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2.867/2.919</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.811/0.819</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3.59/3.616</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.813/0.831</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>32.66/33.65</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.970/0.983</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.287/0.312</t>
+    <t>0.274/0.280</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.018/1.030</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.3/3.38</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.118/1.161</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.485/4.586</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.390/1.413</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -220,15 +204,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1.364/1.394</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.019/1.041</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>18.81/19.40</t>
+    <t>1.079/1.112</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -637,8 +613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C113" sqref="C113"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -747,11 +723,9 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" s="10">
-        <v>1</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="C8" s="10"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
@@ -849,7 +823,7 @@
         <v>7</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="5"/>
@@ -947,7 +921,7 @@
         <v>7</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C23" s="10"/>
       <c r="D23" s="5"/>
@@ -971,7 +945,7 @@
         <v>0</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.15">
@@ -1045,7 +1019,7 @@
         <v>7</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C31" s="10"/>
       <c r="D31" s="5"/>
@@ -1069,7 +1043,7 @@
         <v>0</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.15">
@@ -1142,9 +1116,7 @@
       <c r="A39" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B39" s="5" t="s">
-        <v>41</v>
-      </c>
+      <c r="B39" s="5"/>
       <c r="C39" s="10"/>
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
@@ -1241,7 +1213,7 @@
         <v>7</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C47" s="10"/>
       <c r="D47" s="5"/>
@@ -1339,7 +1311,7 @@
         <v>7</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C54" s="10"/>
       <c r="D54" s="5"/>
@@ -1438,12 +1410,8 @@
       <c r="A62" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B62" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C62" s="10">
-        <v>1</v>
-      </c>
+      <c r="B62" s="5"/>
+      <c r="C62" s="10"/>
       <c r="D62" s="5"/>
       <c r="E62" s="5"/>
       <c r="F62" s="5"/>
@@ -1538,9 +1506,7 @@
       <c r="A70" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B70" s="5" t="s">
-        <v>47</v>
-      </c>
+      <c r="B70" s="5"/>
       <c r="C70" s="10"/>
       <c r="D70" s="5"/>
       <c r="E70" s="10"/>
@@ -1632,9 +1598,7 @@
       <c r="A78" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B78" s="5" t="s">
-        <v>38</v>
-      </c>
+      <c r="B78" s="5"/>
       <c r="C78" s="10"/>
       <c r="D78" s="5"/>
       <c r="E78" s="5"/>
@@ -1730,12 +1694,8 @@
       <c r="A86" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B86" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C86" s="10">
-        <v>1</v>
-      </c>
+      <c r="B86" s="5"/>
+      <c r="C86" s="10"/>
       <c r="D86" s="5"/>
       <c r="E86" s="5"/>
       <c r="F86" s="5"/>
@@ -1831,7 +1791,7 @@
         <v>7</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C94" s="10"/>
       <c r="D94" s="5"/>
@@ -1928,12 +1888,8 @@
       <c r="A102" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B102" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C102" s="10">
-        <v>1</v>
-      </c>
+      <c r="B102" s="5"/>
+      <c r="C102" s="10"/>
       <c r="D102" s="5"/>
       <c r="E102" s="5"/>
       <c r="F102" s="5"/>
@@ -2029,7 +1985,7 @@
         <v>7</v>
       </c>
       <c r="B110" s="5" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="C110" s="10"/>
       <c r="D110" s="5"/>

</xml_diff>

<commit_message>
check-in: 20200810 update the zhongshu_wangge.xlsx
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="51">
   <si>
     <t>交易品种：</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -180,31 +180,43 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1.018/1.030</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3.3/3.38</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.118/1.161</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4.485/4.586</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.390/1.413</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1.048/1.069</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>1.079/1.112</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.3/3.363</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.118/1.155</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.476/4.558</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.390/1.404</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.961/3.980</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.31/4.55</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.36/4.47</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.000/1.008</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -614,7 +626,7 @@
   <dimension ref="A1:R112"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+      <selection activeCell="C105" sqref="C105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -723,7 +735,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="5"/>
@@ -823,7 +835,7 @@
         <v>7</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="5"/>
@@ -921,7 +933,7 @@
         <v>7</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C23" s="10"/>
       <c r="D23" s="5"/>
@@ -1019,7 +1031,7 @@
         <v>7</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C31" s="10"/>
       <c r="D31" s="5"/>
@@ -1116,7 +1128,9 @@
       <c r="A39" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B39" s="5"/>
+      <c r="B39" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="C39" s="10"/>
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
@@ -1213,7 +1227,7 @@
         <v>7</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C47" s="10"/>
       <c r="D47" s="5"/>
@@ -1311,7 +1325,7 @@
         <v>7</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C54" s="10"/>
       <c r="D54" s="5"/>
@@ -1598,7 +1612,9 @@
       <c r="A78" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B78" s="5"/>
+      <c r="B78" s="5" t="s">
+        <v>48</v>
+      </c>
       <c r="C78" s="10"/>
       <c r="D78" s="5"/>
       <c r="E78" s="5"/>
@@ -1694,7 +1710,9 @@
       <c r="A86" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B86" s="5"/>
+      <c r="B86" s="5" t="s">
+        <v>49</v>
+      </c>
       <c r="C86" s="10"/>
       <c r="D86" s="5"/>
       <c r="E86" s="5"/>
@@ -1791,7 +1809,7 @@
         <v>7</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="C94" s="10"/>
       <c r="D94" s="5"/>

</xml_diff>

<commit_message>
check-in: update the zhongshu_wangge.xlsx 20201014
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="37">
   <si>
     <t>交易品种：</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -48,18 +48,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">1D </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>止盈目标：</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>市盈率到达平均数</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>中枢0执行情况</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -76,10 +68,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>止盈目标：</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>中枢1执行情况</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -88,30 +76,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>交易品种：</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>沃格光电（603773）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>洛阳钼业（603993）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>紫金银行（601860）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>有友食品（603697）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>30F</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1D</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -120,14 +84,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1D</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1D</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>50ETF（510050）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -160,10 +116,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>白银基金（161226）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>华宝油气（162411）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -188,18 +140,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>3.3/3.363</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1.118/1.155</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>4.476/4.558</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1.390/1.404</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -208,15 +152,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>4.31/4.55</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4.36/4.47</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1.000/1.008</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.391/3.489</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.297/4.459</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -296,7 +240,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -308,7 +252,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="176" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="176" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
@@ -623,10 +566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R112"/>
+  <dimension ref="A1:R72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C105" sqref="C105"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D72" sqref="D72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -659,12 +602,12 @@
         <v>0</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="B4" s="8">
         <v>5700</v>
@@ -672,10 +615,10 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.15">
@@ -686,13 +629,13 @@
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -710,10 +653,10 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="B7" s="3"/>
-      <c r="C7" s="11"/>
+      <c r="C7" s="10"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -735,9 +678,9 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" s="10"/>
+        <v>35</v>
+      </c>
+      <c r="C8" s="9"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
@@ -759,23 +702,23 @@
         <v>0</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A12" s="7" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A13" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.15">
@@ -786,13 +729,13 @@
         <v>5</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
@@ -810,10 +753,10 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B15" s="3"/>
-      <c r="C15" s="11"/>
+      <c r="C15" s="10"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
@@ -835,9 +778,9 @@
         <v>7</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" s="10"/>
+        <v>31</v>
+      </c>
+      <c r="C16" s="9"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
@@ -859,21 +802,21 @@
         <v>0</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A19" s="7" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="B19" s="8"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A20" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.15">
@@ -884,13 +827,13 @@
         <v>5</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
@@ -908,10 +851,10 @@
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A22" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B22" s="3"/>
-      <c r="C22" s="11"/>
+      <c r="C22" s="10"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
@@ -933,9 +876,9 @@
         <v>7</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C23" s="10"/>
+        <v>36</v>
+      </c>
+      <c r="C23" s="9"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
@@ -957,21 +900,21 @@
         <v>0</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A27" s="7" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B27" s="8"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A28" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.15">
@@ -982,13 +925,13 @@
         <v>5</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
@@ -1006,10 +949,10 @@
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A30" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B30" s="3"/>
-      <c r="C30" s="11"/>
+      <c r="C30" s="10"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
@@ -1031,9 +974,9 @@
         <v>7</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C31" s="10"/>
+        <v>32</v>
+      </c>
+      <c r="C31" s="9"/>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
@@ -1055,21 +998,21 @@
         <v>0</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A35" s="7" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B35" s="8"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A36" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.15">
@@ -1080,13 +1023,13 @@
         <v>5</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
@@ -1104,10 +1047,10 @@
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A38" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B38" s="3"/>
-      <c r="C38" s="11"/>
+      <c r="C38" s="10"/>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
@@ -1129,9 +1072,9 @@
         <v>7</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C39" s="10"/>
+        <v>33</v>
+      </c>
+      <c r="C39" s="9"/>
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
@@ -1153,21 +1096,21 @@
         <v>0</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A43" s="7" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="B43" s="8"/>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A44" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.15">
@@ -1178,13 +1121,13 @@
         <v>5</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
@@ -1202,10 +1145,10 @@
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A46" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B46" s="3"/>
-      <c r="C46" s="11"/>
+      <c r="C46" s="10"/>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
@@ -1227,9 +1170,9 @@
         <v>7</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C47" s="10"/>
+        <v>29</v>
+      </c>
+      <c r="C47" s="9"/>
       <c r="D47" s="5"/>
       <c r="E47" s="5"/>
       <c r="F47" s="5"/>
@@ -1251,21 +1194,21 @@
         <v>0</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A50" s="7" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="B50" s="8"/>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A51" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.15">
@@ -1276,13 +1219,13 @@
         <v>5</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
@@ -1300,10 +1243,10 @@
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A53" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B53" s="3"/>
-      <c r="C53" s="11"/>
+      <c r="C53" s="10"/>
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
@@ -1325,9 +1268,9 @@
         <v>7</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C54" s="10"/>
+        <v>30</v>
+      </c>
+      <c r="C54" s="9"/>
       <c r="D54" s="5"/>
       <c r="E54" s="5"/>
       <c r="F54" s="5"/>
@@ -1346,7 +1289,7 @@
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A57" s="7" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="B57" s="8" t="s">
         <v>22</v>
@@ -1354,18 +1297,16 @@
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A58" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B58" s="8">
-        <v>2</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="B58" s="8"/>
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A59" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.15">
@@ -1376,13 +1317,13 @@
         <v>5</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
@@ -1400,10 +1341,10 @@
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A61" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B61" s="3"/>
-      <c r="C61" s="9"/>
+      <c r="C61" s="10"/>
       <c r="D61" s="3"/>
       <c r="E61" s="3"/>
       <c r="F61" s="3"/>
@@ -1424,8 +1365,10 @@
       <c r="A62" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B62" s="5"/>
-      <c r="C62" s="10"/>
+      <c r="B62" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C62" s="9"/>
       <c r="D62" s="5"/>
       <c r="E62" s="5"/>
       <c r="F62" s="5"/>
@@ -1447,21 +1390,21 @@
         <v>0</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="66" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A66" s="7" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="B66" s="8"/>
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A67" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="68" spans="1:18" x14ac:dyDescent="0.15">
@@ -1472,13 +1415,13 @@
         <v>5</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F68" s="1"/>
       <c r="G68" s="1"/>
@@ -1496,10 +1439,10 @@
     </row>
     <row r="69" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A69" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B69" s="3"/>
-      <c r="C69" s="3"/>
+      <c r="C69" s="10"/>
       <c r="D69" s="3"/>
       <c r="E69" s="3"/>
       <c r="F69" s="3"/>
@@ -1518,12 +1461,14 @@
     </row>
     <row r="70" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A70" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B70" s="5"/>
-      <c r="C70" s="10"/>
+        <v>7</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C70" s="9"/>
       <c r="D70" s="5"/>
-      <c r="E70" s="10"/>
+      <c r="E70" s="5"/>
       <c r="F70" s="5"/>
       <c r="G70" s="5"/>
       <c r="H70" s="5"/>
@@ -1538,491 +1483,7 @@
       <c r="Q70" s="4"/>
       <c r="R70" s="4"/>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A73" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B73" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A74" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B74" s="8"/>
-    </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A75" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B75" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A76" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D76" s="1"/>
-      <c r="E76" s="1"/>
-      <c r="F76" s="1"/>
-      <c r="G76" s="1"/>
-      <c r="H76" s="1"/>
-      <c r="I76" s="1"/>
-      <c r="J76" s="1"/>
-      <c r="K76" s="1"/>
-      <c r="L76" s="1"/>
-      <c r="M76" s="1"/>
-      <c r="N76" s="1"/>
-      <c r="O76" s="1"/>
-      <c r="P76" s="1"/>
-      <c r="Q76" s="1"/>
-      <c r="R76" s="1"/>
-    </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A77" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B77" s="3"/>
-      <c r="C77" s="3"/>
-      <c r="D77" s="3"/>
-      <c r="E77" s="3"/>
-      <c r="F77" s="3"/>
-      <c r="G77" s="3"/>
-      <c r="H77" s="3"/>
-      <c r="I77" s="2"/>
-      <c r="J77" s="2"/>
-      <c r="K77" s="2"/>
-      <c r="L77" s="2"/>
-      <c r="M77" s="2"/>
-      <c r="N77" s="2"/>
-      <c r="O77" s="2"/>
-      <c r="P77" s="2"/>
-      <c r="Q77" s="2"/>
-      <c r="R77" s="2"/>
-    </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A78" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B78" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C78" s="10"/>
-      <c r="D78" s="5"/>
-      <c r="E78" s="5"/>
-      <c r="F78" s="5"/>
-      <c r="G78" s="5"/>
-      <c r="H78" s="5"/>
-      <c r="I78" s="4"/>
-      <c r="J78" s="4"/>
-      <c r="K78" s="4"/>
-      <c r="L78" s="4"/>
-      <c r="M78" s="4"/>
-      <c r="N78" s="4"/>
-      <c r="O78" s="4"/>
-      <c r="P78" s="4"/>
-      <c r="Q78" s="4"/>
-      <c r="R78" s="4"/>
-    </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A81" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B81" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A82" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B82" s="8"/>
-    </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A83" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B83" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A84" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E84" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F84" s="1"/>
-      <c r="G84" s="1"/>
-      <c r="H84" s="1"/>
-      <c r="I84" s="1"/>
-      <c r="J84" s="1"/>
-      <c r="K84" s="1"/>
-      <c r="L84" s="1"/>
-      <c r="M84" s="1"/>
-      <c r="N84" s="1"/>
-      <c r="O84" s="1"/>
-      <c r="P84" s="1"/>
-      <c r="Q84" s="1"/>
-      <c r="R84" s="1"/>
-    </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A85" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B85" s="3"/>
-      <c r="C85" s="11"/>
-      <c r="D85" s="3"/>
-      <c r="E85" s="3"/>
-      <c r="F85" s="3"/>
-      <c r="G85" s="3"/>
-      <c r="H85" s="3"/>
-      <c r="I85" s="2"/>
-      <c r="J85" s="2"/>
-      <c r="K85" s="2"/>
-      <c r="L85" s="2"/>
-      <c r="M85" s="2"/>
-      <c r="N85" s="2"/>
-      <c r="O85" s="2"/>
-      <c r="P85" s="2"/>
-      <c r="Q85" s="2"/>
-      <c r="R85" s="2"/>
-    </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A86" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B86" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C86" s="10"/>
-      <c r="D86" s="5"/>
-      <c r="E86" s="5"/>
-      <c r="F86" s="5"/>
-      <c r="G86" s="5"/>
-      <c r="H86" s="5"/>
-      <c r="I86" s="4"/>
-      <c r="J86" s="4"/>
-      <c r="K86" s="4"/>
-      <c r="L86" s="4"/>
-      <c r="M86" s="4"/>
-      <c r="N86" s="4"/>
-      <c r="O86" s="4"/>
-      <c r="P86" s="4"/>
-      <c r="Q86" s="4"/>
-      <c r="R86" s="4"/>
-    </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A89" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B89" s="8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A90" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B90" s="8"/>
-    </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A91" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B91" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A92" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D92" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E92" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F92" s="1"/>
-      <c r="G92" s="1"/>
-      <c r="H92" s="1"/>
-      <c r="I92" s="1"/>
-      <c r="J92" s="1"/>
-      <c r="K92" s="1"/>
-      <c r="L92" s="1"/>
-      <c r="M92" s="1"/>
-      <c r="N92" s="1"/>
-      <c r="O92" s="1"/>
-      <c r="P92" s="1"/>
-      <c r="Q92" s="1"/>
-      <c r="R92" s="1"/>
-    </row>
-    <row r="93" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A93" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B93" s="3"/>
-      <c r="C93" s="11"/>
-      <c r="D93" s="3"/>
-      <c r="E93" s="3"/>
-      <c r="F93" s="3"/>
-      <c r="G93" s="3"/>
-      <c r="H93" s="3"/>
-      <c r="I93" s="2"/>
-      <c r="J93" s="2"/>
-      <c r="K93" s="2"/>
-      <c r="L93" s="2"/>
-      <c r="M93" s="2"/>
-      <c r="N93" s="2"/>
-      <c r="O93" s="2"/>
-      <c r="P93" s="2"/>
-      <c r="Q93" s="2"/>
-      <c r="R93" s="2"/>
-    </row>
-    <row r="94" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A94" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B94" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C94" s="10"/>
-      <c r="D94" s="5"/>
-      <c r="E94" s="5"/>
-      <c r="F94" s="5"/>
-      <c r="G94" s="5"/>
-      <c r="H94" s="5"/>
-      <c r="I94" s="4"/>
-      <c r="J94" s="4"/>
-      <c r="K94" s="4"/>
-      <c r="L94" s="4"/>
-      <c r="M94" s="4"/>
-      <c r="N94" s="4"/>
-      <c r="O94" s="4"/>
-      <c r="P94" s="4"/>
-      <c r="Q94" s="4"/>
-      <c r="R94" s="4"/>
-    </row>
-    <row r="97" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A97" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B97" s="8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A98" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B98" s="8"/>
-    </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A99" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B99" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="100" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A100" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C100" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D100" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E100" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F100" s="1"/>
-      <c r="G100" s="1"/>
-      <c r="H100" s="1"/>
-      <c r="I100" s="1"/>
-      <c r="J100" s="1"/>
-      <c r="K100" s="1"/>
-      <c r="L100" s="1"/>
-      <c r="M100" s="1"/>
-      <c r="N100" s="1"/>
-      <c r="O100" s="1"/>
-      <c r="P100" s="1"/>
-      <c r="Q100" s="1"/>
-      <c r="R100" s="1"/>
-    </row>
-    <row r="101" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A101" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B101" s="3"/>
-      <c r="C101" s="11"/>
-      <c r="D101" s="3"/>
-      <c r="E101" s="3"/>
-      <c r="F101" s="3"/>
-      <c r="G101" s="3"/>
-      <c r="H101" s="3"/>
-      <c r="I101" s="2"/>
-      <c r="J101" s="2"/>
-      <c r="K101" s="2"/>
-      <c r="L101" s="2"/>
-      <c r="M101" s="2"/>
-      <c r="N101" s="2"/>
-      <c r="O101" s="2"/>
-      <c r="P101" s="2"/>
-      <c r="Q101" s="2"/>
-      <c r="R101" s="2"/>
-    </row>
-    <row r="102" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A102" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B102" s="5"/>
-      <c r="C102" s="10"/>
-      <c r="D102" s="5"/>
-      <c r="E102" s="5"/>
-      <c r="F102" s="5"/>
-      <c r="G102" s="5"/>
-      <c r="H102" s="5"/>
-      <c r="I102" s="4"/>
-      <c r="J102" s="4"/>
-      <c r="K102" s="4"/>
-      <c r="L102" s="4"/>
-      <c r="M102" s="4"/>
-      <c r="N102" s="4"/>
-      <c r="O102" s="4"/>
-      <c r="P102" s="4"/>
-      <c r="Q102" s="4"/>
-      <c r="R102" s="4"/>
-    </row>
-    <row r="105" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A105" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B105" s="8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="106" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A106" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B106" s="8"/>
-    </row>
-    <row r="107" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A107" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B107" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="108" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A108" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B108" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C108" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D108" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E108" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F108" s="1"/>
-      <c r="G108" s="1"/>
-      <c r="H108" s="1"/>
-      <c r="I108" s="1"/>
-      <c r="J108" s="1"/>
-      <c r="K108" s="1"/>
-      <c r="L108" s="1"/>
-      <c r="M108" s="1"/>
-      <c r="N108" s="1"/>
-      <c r="O108" s="1"/>
-      <c r="P108" s="1"/>
-      <c r="Q108" s="1"/>
-      <c r="R108" s="1"/>
-    </row>
-    <row r="109" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A109" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B109" s="3"/>
-      <c r="C109" s="11"/>
-      <c r="D109" s="3"/>
-      <c r="E109" s="3"/>
-      <c r="F109" s="3"/>
-      <c r="G109" s="3"/>
-      <c r="H109" s="3"/>
-      <c r="I109" s="2"/>
-      <c r="J109" s="2"/>
-      <c r="K109" s="2"/>
-      <c r="L109" s="2"/>
-      <c r="M109" s="2"/>
-      <c r="N109" s="2"/>
-      <c r="O109" s="2"/>
-      <c r="P109" s="2"/>
-      <c r="Q109" s="2"/>
-      <c r="R109" s="2"/>
-    </row>
-    <row r="110" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A110" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B110" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C110" s="10"/>
-      <c r="D110" s="5"/>
-      <c r="E110" s="5"/>
-      <c r="F110" s="5"/>
-      <c r="G110" s="5"/>
-      <c r="H110" s="5"/>
-      <c r="I110" s="4"/>
-      <c r="J110" s="4"/>
-      <c r="K110" s="4"/>
-      <c r="L110" s="4"/>
-      <c r="M110" s="4"/>
-      <c r="N110" s="4"/>
-      <c r="O110" s="4"/>
-      <c r="P110" s="4"/>
-      <c r="Q110" s="4"/>
-      <c r="R110" s="4"/>
-    </row>
-    <row r="112" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="72" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
check-in: fine-tune Excel_Analyser.py for debug
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30690" windowHeight="11850"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30696" windowHeight="11856"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
   <si>
     <t>交易品种：</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -100,10 +100,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>沪深300（510300）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>创业板50（159949）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -121,13 +117,25 @@
   </si>
   <si>
     <t>1.096/1.105</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>300ETF（510300）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pending</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pending</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0_);\(0\)"/>
   </numFmts>
@@ -249,7 +257,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -538,21 +546,21 @@
   <dimension ref="A1:R27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.75" customWidth="1"/>
-    <col min="2" max="2" width="25.125" customWidth="1"/>
-    <col min="3" max="3" width="23.125" customWidth="1"/>
-    <col min="4" max="4" width="21.5" customWidth="1"/>
+    <col min="1" max="1" width="17.77734375" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="21.75" customWidth="1"/>
-    <col min="7" max="8" width="19.5" customWidth="1"/>
+    <col min="6" max="6" width="21.77734375" customWidth="1"/>
+    <col min="7" max="8" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="25.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="25.8" x14ac:dyDescent="0.4">
       <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
@@ -566,23 +574,23 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
@@ -590,7 +598,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -620,12 +628,12 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="3"/>
@@ -644,14 +652,16 @@
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="9"/>
+        <v>24</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>27</v>
+      </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
@@ -668,12 +678,12 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
     </row>
-    <row r="9" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9" s="13">
         <v>1</v>
@@ -684,15 +694,15 @@
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>16</v>
       </c>
@@ -700,7 +710,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>9</v>
       </c>
@@ -708,7 +718,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
@@ -738,7 +748,7 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -762,14 +772,16 @@
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="9"/>
+      <c r="C17" s="9" t="s">
+        <v>28</v>
+      </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
@@ -786,7 +798,7 @@
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
     </row>
-    <row r="18" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>17</v>
       </c>
@@ -802,7 +814,7 @@
       <c r="G18" s="12"/>
       <c r="H18" s="12"/>
     </row>
-    <row r="27" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="27" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
check-in: update the zhongshu_wangge.xlsx 20201026
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30696" windowHeight="11856"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30690" windowHeight="11850"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
   <si>
     <t>交易品种：</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -129,13 +129,21 @@
   </si>
   <si>
     <t>pending</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.732/4.776</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.047/1.064</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0_);\(0\)"/>
   </numFmts>
@@ -257,7 +265,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -546,21 +554,21 @@
   <dimension ref="A1:R27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" customWidth="1"/>
-    <col min="2" max="2" width="25.109375" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" customWidth="1"/>
+    <col min="1" max="1" width="17.75" customWidth="1"/>
+    <col min="2" max="2" width="25.125" customWidth="1"/>
+    <col min="3" max="3" width="23.125" customWidth="1"/>
+    <col min="4" max="4" width="21.5" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="21.77734375" customWidth="1"/>
-    <col min="7" max="8" width="19.44140625" customWidth="1"/>
+    <col min="6" max="6" width="21.75" customWidth="1"/>
+    <col min="7" max="8" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="25.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:18" ht="25.5" x14ac:dyDescent="0.3">
       <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
@@ -574,7 +582,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
@@ -582,7 +590,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
         <v>16</v>
       </c>
@@ -590,7 +598,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
@@ -598,7 +606,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -628,7 +636,7 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
@@ -652,7 +660,7 @@
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
@@ -678,7 +686,7 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
     </row>
-    <row r="9" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A9" s="11" t="s">
         <v>17</v>
       </c>
@@ -688,13 +696,15 @@
       <c r="C9" s="13">
         <v>1</v>
       </c>
-      <c r="D9" s="12"/>
+      <c r="D9" s="12" t="s">
+        <v>30</v>
+      </c>
       <c r="E9" s="12"/>
       <c r="F9" s="12"/>
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A12" s="7" t="s">
         <v>0</v>
       </c>
@@ -702,7 +712,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A13" s="7" t="s">
         <v>16</v>
       </c>
@@ -710,7 +720,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A14" s="7" t="s">
         <v>9</v>
       </c>
@@ -718,7 +728,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
@@ -748,7 +758,7 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -772,7 +782,7 @@
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A17" s="4" t="s">
         <v>7</v>
       </c>
@@ -798,7 +808,7 @@
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
     </row>
-    <row r="18" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A18" s="11" t="s">
         <v>17</v>
       </c>
@@ -808,13 +818,15 @@
       <c r="C18" s="13">
         <v>1</v>
       </c>
-      <c r="D18" s="12"/>
+      <c r="D18" s="12" t="s">
+        <v>29</v>
+      </c>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
       <c r="G18" s="12"/>
       <c r="H18" s="12"/>
     </row>
-    <row r="27" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
check-in: update the zhongshu_wangge.xlsx 20201102
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
   <si>
     <t>交易品种：</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -96,10 +96,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>4.813/4.829</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>创业板50（159949）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -116,10 +112,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1.096/1.105</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>300ETF（510300）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -132,11 +124,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>4.732/4.776</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.047/1.064</t>
+    <t>1.09/1.107</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.761/4.804</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -554,7 +546,7 @@
   <dimension ref="A1:R27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -587,7 +579,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.15">
@@ -595,7 +587,7 @@
         <v>16</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.15">
@@ -641,7 +633,7 @@
         <v>15</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="3"/>
@@ -665,10 +657,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
@@ -691,14 +683,10 @@
         <v>17</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="13">
-        <v>1</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>30</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="C9" s="13"/>
+      <c r="D9" s="12"/>
       <c r="E9" s="12"/>
       <c r="F9" s="12"/>
       <c r="G9" s="12"/>
@@ -709,7 +697,7 @@
         <v>0</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.15">
@@ -790,7 +778,7 @@
         <v>19</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
@@ -813,14 +801,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" s="13">
-        <v>1</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>29</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="C18" s="13"/>
+      <c r="D18" s="12"/>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
       <c r="G18" s="12"/>

</xml_diff>

<commit_message>
check-in: update the zhongshu_wangge.xlsx 20201104
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
   <si>
     <t>交易品种：</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -129,6 +129,14 @@
   </si>
   <si>
     <t>4.761/4.804</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.121/1.128</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.830/4.863</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -546,7 +554,7 @@
   <dimension ref="A1:R27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -686,7 +694,9 @@
         <v>27</v>
       </c>
       <c r="C9" s="13"/>
-      <c r="D9" s="12"/>
+      <c r="D9" s="12" t="s">
+        <v>29</v>
+      </c>
       <c r="E9" s="12"/>
       <c r="F9" s="12"/>
       <c r="G9" s="12"/>
@@ -804,7 +814,9 @@
         <v>28</v>
       </c>
       <c r="C18" s="13"/>
-      <c r="D18" s="12"/>
+      <c r="D18" s="12" t="s">
+        <v>30</v>
+      </c>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
       <c r="G18" s="12"/>

</xml_diff>

<commit_message>
check-in: update the zhongshu_wangge.xlsx 20201105
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
   <si>
     <t>交易品种：</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -116,27 +116,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>pending</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>pending</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1.09/1.107</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>4.761/4.804</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1.121/1.128</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>4.830/4.863</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.900/4.953</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -554,7 +546,7 @@
   <dimension ref="A1:R27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -667,9 +659,7 @@
       <c r="B8" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="9" t="s">
-        <v>25</v>
-      </c>
+      <c r="C8" s="9"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
@@ -691,11 +681,11 @@
         <v>17</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C9" s="13"/>
       <c r="D9" s="12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E9" s="12"/>
       <c r="F9" s="12"/>
@@ -787,9 +777,7 @@
       <c r="B17" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="9" t="s">
-        <v>26</v>
-      </c>
+      <c r="C17" s="9"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
@@ -815,7 +803,7 @@
       </c>
       <c r="C18" s="13"/>
       <c r="D18" s="12" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>

</xml_diff>

<commit_message>
check-in: update the zhongshu_wangge.xlsx 20201110
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
   <si>
     <t>交易品种：</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -108,27 +108,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1.089/1.113</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>300ETF（510300）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1.09/1.107</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.121/1.128</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4.830/4.863</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4.900/4.953</t>
+    <t>1.139/1.161</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.114/1.150</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.005/5.029</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -546,7 +538,7 @@
   <dimension ref="A1:R27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -657,7 +649,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="5"/>
@@ -681,12 +673,10 @@
         <v>17</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" s="13"/>
-      <c r="D9" s="12" t="s">
-        <v>26</v>
-      </c>
+      <c r="D9" s="12"/>
       <c r="E9" s="12"/>
       <c r="F9" s="12"/>
       <c r="G9" s="12"/>
@@ -697,7 +687,7 @@
         <v>0</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.15">
@@ -799,12 +789,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C18" s="13"/>
-      <c r="D18" s="12" t="s">
-        <v>27</v>
-      </c>
+      <c r="D18" s="12"/>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
       <c r="G18" s="12"/>

</xml_diff>

<commit_message>
check-in: update zhongshu_wangge.xlsx for 5F operation 20201111
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30690" windowHeight="11850"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30696" windowHeight="11856"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -127,7 +127,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0_);\(0\)"/>
   </numFmts>
@@ -249,7 +249,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -538,21 +538,21 @@
   <dimension ref="A1:R27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.75" customWidth="1"/>
-    <col min="2" max="2" width="25.125" customWidth="1"/>
-    <col min="3" max="3" width="23.125" customWidth="1"/>
-    <col min="4" max="4" width="21.5" customWidth="1"/>
+    <col min="1" max="1" width="17.77734375" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="21.75" customWidth="1"/>
-    <col min="7" max="8" width="19.5" customWidth="1"/>
+    <col min="6" max="6" width="21.77734375" customWidth="1"/>
+    <col min="7" max="8" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="25.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="25.8" x14ac:dyDescent="0.4">
       <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
@@ -566,7 +566,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
@@ -574,7 +574,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>16</v>
       </c>
@@ -582,7 +582,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
@@ -590,7 +590,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -620,7 +620,7 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
@@ -644,7 +644,7 @@
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
@@ -668,21 +668,23 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
     </row>
-    <row r="9" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="13"/>
+      <c r="C9" s="13">
+        <v>1</v>
+      </c>
       <c r="D9" s="12"/>
       <c r="E9" s="12"/>
       <c r="F9" s="12"/>
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>0</v>
       </c>
@@ -690,7 +692,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>16</v>
       </c>
@@ -698,7 +700,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>9</v>
       </c>
@@ -706,7 +708,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
@@ -736,7 +738,7 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -760,7 +762,7 @@
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>7</v>
       </c>
@@ -784,7 +786,7 @@
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
     </row>
-    <row r="18" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>17</v>
       </c>
@@ -798,7 +800,7 @@
       <c r="G18" s="12"/>
       <c r="H18" s="12"/>
     </row>
-    <row r="27" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="27" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
check-in: update the zhongshu_wangge.xlsx 20201112
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30696" windowHeight="11856"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30690" windowHeight="11850"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
   <si>
     <t>交易品种：</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -121,13 +121,17 @@
   </si>
   <si>
     <t>5.005/5.029</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.107/1.12</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0_);\(0\)"/>
   </numFmts>
@@ -249,7 +253,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -538,21 +542,21 @@
   <dimension ref="A1:R27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" customWidth="1"/>
-    <col min="2" max="2" width="25.109375" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" customWidth="1"/>
+    <col min="1" max="1" width="17.75" customWidth="1"/>
+    <col min="2" max="2" width="25.125" customWidth="1"/>
+    <col min="3" max="3" width="23.125" customWidth="1"/>
+    <col min="4" max="4" width="21.5" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="21.77734375" customWidth="1"/>
-    <col min="7" max="8" width="19.44140625" customWidth="1"/>
+    <col min="6" max="6" width="21.75" customWidth="1"/>
+    <col min="7" max="8" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="25.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:18" ht="25.5" x14ac:dyDescent="0.3">
       <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
@@ -566,7 +570,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
@@ -574,7 +578,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
         <v>16</v>
       </c>
@@ -582,7 +586,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
@@ -590,7 +594,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -620,7 +624,7 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
@@ -644,7 +648,7 @@
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
@@ -668,7 +672,7 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
     </row>
-    <row r="9" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A9" s="11" t="s">
         <v>17</v>
       </c>
@@ -678,13 +682,15 @@
       <c r="C9" s="13">
         <v>1</v>
       </c>
-      <c r="D9" s="12"/>
+      <c r="D9" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="E9" s="12"/>
       <c r="F9" s="12"/>
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A12" s="7" t="s">
         <v>0</v>
       </c>
@@ -692,7 +698,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A13" s="7" t="s">
         <v>16</v>
       </c>
@@ -700,7 +706,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A14" s="7" t="s">
         <v>9</v>
       </c>
@@ -708,7 +714,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
@@ -738,7 +744,7 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -762,7 +768,7 @@
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A17" s="4" t="s">
         <v>7</v>
       </c>
@@ -786,7 +792,7 @@
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
     </row>
-    <row r="18" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A18" s="11" t="s">
         <v>17</v>
       </c>
@@ -800,7 +806,7 @@
       <c r="G18" s="12"/>
       <c r="H18" s="12"/>
     </row>
-    <row r="27" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
check-in:update the zhongshu_wangge.xlsx 20201113
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30690" windowHeight="11850"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30696" windowHeight="11856"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -131,7 +131,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0_);\(0\)"/>
   </numFmts>
@@ -253,7 +253,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -542,21 +542,21 @@
   <dimension ref="A1:R27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.75" customWidth="1"/>
-    <col min="2" max="2" width="25.125" customWidth="1"/>
-    <col min="3" max="3" width="23.125" customWidth="1"/>
-    <col min="4" max="4" width="21.5" customWidth="1"/>
+    <col min="1" max="1" width="17.77734375" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="21.75" customWidth="1"/>
-    <col min="7" max="8" width="19.5" customWidth="1"/>
+    <col min="6" max="6" width="21.77734375" customWidth="1"/>
+    <col min="7" max="8" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="25.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="25.8" x14ac:dyDescent="0.4">
       <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
@@ -570,7 +570,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
@@ -578,7 +578,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>16</v>
       </c>
@@ -586,7 +586,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
@@ -594,7 +594,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -624,7 +624,7 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
@@ -648,14 +648,16 @@
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="9"/>
+      <c r="C8" s="9">
+        <v>1</v>
+      </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
@@ -672,7 +674,7 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
     </row>
-    <row r="9" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>17</v>
       </c>
@@ -690,7 +692,7 @@
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>0</v>
       </c>
@@ -698,7 +700,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>16</v>
       </c>
@@ -706,7 +708,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>9</v>
       </c>
@@ -714,7 +716,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
@@ -744,7 +746,7 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -768,7 +770,7 @@
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>7</v>
       </c>
@@ -792,21 +794,23 @@
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
     </row>
-    <row r="18" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="13"/>
+      <c r="C18" s="13">
+        <v>1</v>
+      </c>
       <c r="D18" s="12"/>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
       <c r="G18" s="12"/>
       <c r="H18" s="12"/>
     </row>
-    <row r="27" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="27" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
check-in: update the zhongshu_wangge.xlsx 20201115
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30696" windowHeight="11856"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30690" windowHeight="11850"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
   <si>
     <t>交易品种：</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -125,13 +125,17 @@
   </si>
   <si>
     <t>1.107/1.12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.887/4.933</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0_);\(0\)"/>
   </numFmts>
@@ -253,7 +257,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -542,21 +546,21 @@
   <dimension ref="A1:R27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" customWidth="1"/>
-    <col min="2" max="2" width="25.109375" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" customWidth="1"/>
+    <col min="1" max="1" width="17.75" customWidth="1"/>
+    <col min="2" max="2" width="25.125" customWidth="1"/>
+    <col min="3" max="3" width="23.125" customWidth="1"/>
+    <col min="4" max="4" width="21.5" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="21.77734375" customWidth="1"/>
-    <col min="7" max="8" width="19.44140625" customWidth="1"/>
+    <col min="6" max="6" width="21.75" customWidth="1"/>
+    <col min="7" max="8" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="25.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:18" ht="25.5" x14ac:dyDescent="0.3">
       <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
@@ -570,7 +574,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
@@ -578,7 +582,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
         <v>16</v>
       </c>
@@ -586,7 +590,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
@@ -594,7 +598,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -624,7 +628,7 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
@@ -648,7 +652,7 @@
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
@@ -674,7 +678,7 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
     </row>
-    <row r="9" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A9" s="11" t="s">
         <v>17</v>
       </c>
@@ -692,7 +696,7 @@
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A12" s="7" t="s">
         <v>0</v>
       </c>
@@ -700,7 +704,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A13" s="7" t="s">
         <v>16</v>
       </c>
@@ -708,7 +712,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A14" s="7" t="s">
         <v>9</v>
       </c>
@@ -716,7 +720,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
@@ -746,7 +750,7 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -770,7 +774,7 @@
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A17" s="4" t="s">
         <v>7</v>
       </c>
@@ -794,7 +798,7 @@
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
     </row>
-    <row r="18" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A18" s="11" t="s">
         <v>17</v>
       </c>
@@ -804,13 +808,15 @@
       <c r="C18" s="13">
         <v>1</v>
       </c>
-      <c r="D18" s="12"/>
+      <c r="D18" s="12" t="s">
+        <v>28</v>
+      </c>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
       <c r="G18" s="12"/>
       <c r="H18" s="12"/>
     </row>
-    <row r="27" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
check-in: update zhongshu_wangge.xlsx 20201117
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30690" windowHeight="11850"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30696" windowHeight="11856"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -135,7 +135,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0_);\(0\)"/>
   </numFmts>
@@ -257,7 +257,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -546,21 +546,21 @@
   <dimension ref="A1:R27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.75" customWidth="1"/>
-    <col min="2" max="2" width="25.125" customWidth="1"/>
-    <col min="3" max="3" width="23.125" customWidth="1"/>
-    <col min="4" max="4" width="21.5" customWidth="1"/>
+    <col min="1" max="1" width="17.77734375" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="21.75" customWidth="1"/>
-    <col min="7" max="8" width="19.5" customWidth="1"/>
+    <col min="6" max="6" width="21.77734375" customWidth="1"/>
+    <col min="7" max="8" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="25.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="25.8" x14ac:dyDescent="0.4">
       <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
@@ -574,7 +574,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
@@ -582,7 +582,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>16</v>
       </c>
@@ -590,7 +590,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
@@ -598,7 +598,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -628,7 +628,7 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
@@ -652,7 +652,7 @@
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
@@ -678,7 +678,7 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
     </row>
-    <row r="9" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>17</v>
       </c>
@@ -691,12 +691,14 @@
       <c r="D9" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="12"/>
+      <c r="E9" s="13">
+        <v>1</v>
+      </c>
       <c r="F9" s="12"/>
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>0</v>
       </c>
@@ -704,7 +706,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>16</v>
       </c>
@@ -712,7 +714,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>9</v>
       </c>
@@ -720,7 +722,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
@@ -750,7 +752,7 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -774,7 +776,7 @@
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>7</v>
       </c>
@@ -798,7 +800,7 @@
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
     </row>
-    <row r="18" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>17</v>
       </c>
@@ -811,12 +813,12 @@
       <c r="D18" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E18" s="12"/>
+      <c r="E18" s="13"/>
       <c r="F18" s="12"/>
       <c r="G18" s="12"/>
       <c r="H18" s="12"/>
     </row>
-    <row r="27" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="27" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
check-in: update the zhongshu_wangge.xlsx 20201117
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="31">
   <si>
     <t>交易品种：</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -129,6 +129,14 @@
   </si>
   <si>
     <t>4.887/4.933</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>科创50（588000）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.452/1.464</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -546,7 +554,7 @@
   <dimension ref="A1:R27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -818,7 +826,120 @@
       <c r="G18" s="12"/>
       <c r="H18" s="12"/>
     </row>
-    <row r="27" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" s="3"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="2"/>
+      <c r="R25" s="2"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="5"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
+      <c r="M26" s="4"/>
+      <c r="N26" s="4"/>
+      <c r="O26" s="4"/>
+      <c r="P26" s="4"/>
+      <c r="Q26" s="4"/>
+      <c r="R26" s="4"/>
+    </row>
+    <row r="27" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="13">
+        <v>1</v>
+      </c>
+      <c r="D27" s="12"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
check-in: update the zhongshu_wangge.xlsx 20201118
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30696" windowHeight="11856"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30690" windowHeight="11850"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="34">
   <si>
     <t>交易品种：</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -137,13 +137,25 @@
   </si>
   <si>
     <t>1.452/1.464</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.076/1.1000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.430/1.445</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.943/4.960</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0_);\(0\)"/>
   </numFmts>
@@ -265,7 +277,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -553,22 +565,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" customWidth="1"/>
-    <col min="2" max="2" width="25.109375" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" customWidth="1"/>
+    <col min="1" max="1" width="17.75" customWidth="1"/>
+    <col min="2" max="2" width="25.125" customWidth="1"/>
+    <col min="3" max="3" width="23.125" customWidth="1"/>
+    <col min="4" max="4" width="21.5" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="21.77734375" customWidth="1"/>
-    <col min="7" max="8" width="19.44140625" customWidth="1"/>
+    <col min="6" max="6" width="21.75" customWidth="1"/>
+    <col min="7" max="8" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="25.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:18" ht="25.5" x14ac:dyDescent="0.3">
       <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
@@ -582,7 +594,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
@@ -590,7 +602,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
         <v>16</v>
       </c>
@@ -598,7 +610,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
@@ -606,7 +618,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -636,7 +648,7 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
@@ -660,7 +672,7 @@
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
@@ -686,7 +698,7 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
     </row>
-    <row r="9" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A9" s="11" t="s">
         <v>17</v>
       </c>
@@ -702,11 +714,13 @@
       <c r="E9" s="13">
         <v>1</v>
       </c>
-      <c r="F9" s="12"/>
+      <c r="F9" s="12" t="s">
+        <v>31</v>
+      </c>
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A12" s="7" t="s">
         <v>0</v>
       </c>
@@ -714,7 +728,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A13" s="7" t="s">
         <v>16</v>
       </c>
@@ -722,7 +736,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A14" s="7" t="s">
         <v>9</v>
       </c>
@@ -730,7 +744,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
@@ -760,7 +774,7 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -784,7 +798,7 @@
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A17" s="4" t="s">
         <v>7</v>
       </c>
@@ -808,7 +822,7 @@
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
     </row>
-    <row r="18" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A18" s="11" t="s">
         <v>17</v>
       </c>
@@ -822,11 +836,13 @@
         <v>28</v>
       </c>
       <c r="E18" s="13"/>
-      <c r="F18" s="12"/>
+      <c r="F18" s="12" t="s">
+        <v>33</v>
+      </c>
       <c r="G18" s="12"/>
       <c r="H18" s="12"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A21" s="7" t="s">
         <v>0</v>
       </c>
@@ -834,7 +850,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A22" s="7" t="s">
         <v>16</v>
       </c>
@@ -842,7 +858,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A23" s="7" t="s">
         <v>9</v>
       </c>
@@ -850,7 +866,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
         <v>6</v>
       </c>
@@ -880,7 +896,7 @@
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A25" s="2" t="s">
         <v>14</v>
       </c>
@@ -902,7 +918,7 @@
       <c r="Q25" s="2"/>
       <c r="R25" s="2"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A26" s="4" t="s">
         <v>7</v>
       </c>
@@ -924,7 +940,7 @@
       <c r="Q26" s="4"/>
       <c r="R26" s="4"/>
     </row>
-    <row r="27" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A27" s="11" t="s">
         <v>17</v>
       </c>
@@ -934,7 +950,9 @@
       <c r="C27" s="13">
         <v>1</v>
       </c>
-      <c r="D27" s="12"/>
+      <c r="D27" s="12" t="s">
+        <v>32</v>
+      </c>
       <c r="E27" s="13"/>
       <c r="F27" s="12"/>
       <c r="G27" s="12"/>

</xml_diff>

<commit_message>
check-in: update the zhongshu_wangge.xlsx 20201119
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30690" windowHeight="11850"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30696" windowHeight="11856"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -155,7 +155,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0_);\(0\)"/>
   </numFmts>
@@ -277,7 +277,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -565,22 +565,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.75" customWidth="1"/>
-    <col min="2" max="2" width="25.125" customWidth="1"/>
-    <col min="3" max="3" width="23.125" customWidth="1"/>
-    <col min="4" max="4" width="21.5" customWidth="1"/>
+    <col min="1" max="1" width="17.77734375" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="21.75" customWidth="1"/>
-    <col min="7" max="8" width="19.5" customWidth="1"/>
+    <col min="6" max="6" width="21.77734375" customWidth="1"/>
+    <col min="7" max="8" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="25.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="25.8" x14ac:dyDescent="0.4">
       <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
@@ -594,7 +594,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
@@ -602,7 +602,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>16</v>
       </c>
@@ -610,7 +610,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
@@ -618,7 +618,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -648,7 +648,7 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
@@ -672,7 +672,7 @@
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
@@ -698,7 +698,7 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
     </row>
-    <row r="9" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>17</v>
       </c>
@@ -717,10 +717,12 @@
       <c r="F9" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="G9" s="12"/>
+      <c r="G9" s="13">
+        <v>1</v>
+      </c>
       <c r="H9" s="12"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>0</v>
       </c>
@@ -728,7 +730,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>16</v>
       </c>
@@ -736,7 +738,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>9</v>
       </c>
@@ -744,7 +746,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
@@ -774,7 +776,7 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -798,7 +800,7 @@
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>7</v>
       </c>
@@ -822,7 +824,7 @@
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
     </row>
-    <row r="18" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>17</v>
       </c>
@@ -842,7 +844,7 @@
       <c r="G18" s="12"/>
       <c r="H18" s="12"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>0</v>
       </c>
@@ -850,7 +852,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>16</v>
       </c>
@@ -858,7 +860,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>9</v>
       </c>
@@ -866,7 +868,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>6</v>
       </c>
@@ -896,7 +898,7 @@
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>14</v>
       </c>
@@ -918,7 +920,7 @@
       <c r="Q25" s="2"/>
       <c r="R25" s="2"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>7</v>
       </c>
@@ -940,7 +942,7 @@
       <c r="Q26" s="4"/>
       <c r="R26" s="4"/>
     </row>
-    <row r="27" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>17</v>
       </c>
@@ -953,7 +955,9 @@
       <c r="D27" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E27" s="13"/>
+      <c r="E27" s="13">
+        <v>1</v>
+      </c>
       <c r="F27" s="12"/>
       <c r="G27" s="12"/>
       <c r="H27" s="12"/>

</xml_diff>

<commit_message>
check-in: update the zhongshu_wangge.xlsx
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30696" windowHeight="11856"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30690" windowHeight="11850"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="35">
   <si>
     <t>交易品种：</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -149,13 +149,17 @@
   </si>
   <si>
     <t>4.943/4.960</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.412/1.444</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0_);\(0\)"/>
   </numFmts>
@@ -277,7 +281,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -565,22 +569,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" customWidth="1"/>
-    <col min="2" max="2" width="25.109375" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" customWidth="1"/>
+    <col min="1" max="1" width="17.75" customWidth="1"/>
+    <col min="2" max="2" width="25.125" customWidth="1"/>
+    <col min="3" max="3" width="23.125" customWidth="1"/>
+    <col min="4" max="4" width="21.5" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="21.77734375" customWidth="1"/>
-    <col min="7" max="8" width="19.44140625" customWidth="1"/>
+    <col min="6" max="6" width="21.75" customWidth="1"/>
+    <col min="7" max="8" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="25.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:18" ht="25.5" x14ac:dyDescent="0.3">
       <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
@@ -594,7 +598,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
@@ -602,7 +606,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
         <v>16</v>
       </c>
@@ -610,7 +614,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
@@ -618,7 +622,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -648,7 +652,7 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
@@ -672,7 +676,7 @@
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
@@ -698,7 +702,7 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
     </row>
-    <row r="9" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A9" s="11" t="s">
         <v>17</v>
       </c>
@@ -722,7 +726,7 @@
       </c>
       <c r="H9" s="12"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A12" s="7" t="s">
         <v>0</v>
       </c>
@@ -730,7 +734,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A13" s="7" t="s">
         <v>16</v>
       </c>
@@ -738,7 +742,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A14" s="7" t="s">
         <v>9</v>
       </c>
@@ -746,7 +750,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
@@ -776,7 +780,7 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -800,7 +804,7 @@
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A17" s="4" t="s">
         <v>7</v>
       </c>
@@ -824,7 +828,7 @@
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
     </row>
-    <row r="18" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A18" s="11" t="s">
         <v>17</v>
       </c>
@@ -844,7 +848,7 @@
       <c r="G18" s="12"/>
       <c r="H18" s="12"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A21" s="7" t="s">
         <v>0</v>
       </c>
@@ -852,7 +856,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A22" s="7" t="s">
         <v>16</v>
       </c>
@@ -860,7 +864,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A23" s="7" t="s">
         <v>9</v>
       </c>
@@ -868,7 +872,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
         <v>6</v>
       </c>
@@ -898,7 +902,7 @@
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A25" s="2" t="s">
         <v>14</v>
       </c>
@@ -920,11 +924,13 @@
       <c r="Q25" s="2"/>
       <c r="R25" s="2"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A26" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B26" s="5"/>
+      <c r="B26" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="C26" s="9"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
@@ -942,7 +948,7 @@
       <c r="Q26" s="4"/>
       <c r="R26" s="4"/>
     </row>
-    <row r="27" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A27" s="11" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
check-in: zhongshu_wangge.xlsx 20201123 update
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="33">
   <si>
     <t>交易品种：</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -120,18 +120,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>5.005/5.029</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1.107/1.12</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>4.887/4.933</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>科创50（588000）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -148,11 +140,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>4.943/4.960</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.412/1.444</t>
+    <t>4.988/5.012</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.416/1.444</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -569,8 +561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -713,17 +705,15 @@
         <v>1</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E9" s="13">
         <v>1</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="G9" s="13">
-        <v>1</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="G9" s="13"/>
       <c r="H9" s="12"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.15">
@@ -833,18 +823,12 @@
         <v>17</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" s="13">
-        <v>1</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>28</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="C18" s="13"/>
+      <c r="D18" s="12"/>
       <c r="E18" s="13"/>
-      <c r="F18" s="12" t="s">
-        <v>33</v>
-      </c>
+      <c r="F18" s="12"/>
       <c r="G18" s="12"/>
       <c r="H18" s="12"/>
     </row>
@@ -853,7 +837,7 @@
         <v>0</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.15">
@@ -929,7 +913,7 @@
         <v>7</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C26" s="9"/>
       <c r="D26" s="5"/>
@@ -953,13 +937,13 @@
         <v>17</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C27" s="13">
         <v>1</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E27" s="13">
         <v>1</v>

</xml_diff>

<commit_message>
check-in: zhongshu_wangge.xlsx update 20201124
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="34">
   <si>
     <t>交易品种：</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -140,11 +140,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>4.988/5.012</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1.416/1.444</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.416/1.424</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.034/5.051</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -561,8 +565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -823,7 +827,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C18" s="13"/>
       <c r="D18" s="12"/>
@@ -913,7 +917,7 @@
         <v>7</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C26" s="9"/>
       <c r="D26" s="5"/>
@@ -948,7 +952,9 @@
       <c r="E27" s="13">
         <v>1</v>
       </c>
-      <c r="F27" s="12"/>
+      <c r="F27" s="12" t="s">
+        <v>32</v>
+      </c>
       <c r="G27" s="12"/>
       <c r="H27" s="12"/>
     </row>

</xml_diff>

<commit_message>
check-in: update the zhongshu_wangge.xlsx 20201125
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30690" windowHeight="11850"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30696" windowHeight="11856"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -155,7 +155,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0_);\(0\)"/>
   </numFmts>
@@ -277,7 +277,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -565,22 +565,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.75" customWidth="1"/>
-    <col min="2" max="2" width="25.125" customWidth="1"/>
-    <col min="3" max="3" width="23.125" customWidth="1"/>
-    <col min="4" max="4" width="21.5" customWidth="1"/>
+    <col min="1" max="1" width="17.77734375" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="21.75" customWidth="1"/>
-    <col min="7" max="8" width="19.5" customWidth="1"/>
+    <col min="6" max="6" width="21.77734375" customWidth="1"/>
+    <col min="7" max="8" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="25.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="25.8" x14ac:dyDescent="0.4">
       <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
@@ -594,7 +594,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
@@ -602,7 +602,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>16</v>
       </c>
@@ -610,7 +610,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
@@ -618,7 +618,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -648,7 +648,7 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
@@ -672,7 +672,7 @@
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
@@ -698,7 +698,7 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
     </row>
-    <row r="9" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>17</v>
       </c>
@@ -720,7 +720,7 @@
       <c r="G9" s="13"/>
       <c r="H9" s="12"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>0</v>
       </c>
@@ -728,7 +728,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>16</v>
       </c>
@@ -736,7 +736,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>9</v>
       </c>
@@ -744,7 +744,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
@@ -774,7 +774,7 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -798,7 +798,7 @@
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>7</v>
       </c>
@@ -822,7 +822,7 @@
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
     </row>
-    <row r="18" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>17</v>
       </c>
@@ -836,7 +836,7 @@
       <c r="G18" s="12"/>
       <c r="H18" s="12"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>0</v>
       </c>
@@ -844,7 +844,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>16</v>
       </c>
@@ -852,7 +852,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>9</v>
       </c>
@@ -860,7 +860,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>6</v>
       </c>
@@ -890,7 +890,7 @@
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>14</v>
       </c>
@@ -912,14 +912,16 @@
       <c r="Q25" s="2"/>
       <c r="R25" s="2"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C26" s="9"/>
+      <c r="C26" s="9">
+        <v>1</v>
+      </c>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
@@ -936,7 +938,7 @@
       <c r="Q26" s="4"/>
       <c r="R26" s="4"/>
     </row>
-    <row r="27" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>17</v>
       </c>
@@ -955,7 +957,9 @@
       <c r="F27" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="G27" s="12"/>
+      <c r="G27" s="13">
+        <v>1</v>
+      </c>
       <c r="H27" s="12"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
check-in： update the zhongshu_wangge.xlsx
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -565,8 +565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -829,7 +829,9 @@
       <c r="B18" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="13"/>
+      <c r="C18" s="13">
+        <v>1</v>
+      </c>
       <c r="D18" s="12"/>
       <c r="E18" s="13"/>
       <c r="F18" s="12"/>

</xml_diff>

<commit_message>
check-in: update zhongshu_wangge.xlsx 20201126
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30696" windowHeight="11856"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30690" windowHeight="11850"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="37">
   <si>
     <t>交易品种：</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -149,13 +149,25 @@
   </si>
   <si>
     <t>5.034/5.051</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.887/5.105</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.934/4.975</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.061/1.112</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0_);\(0\)"/>
   </numFmts>
@@ -277,7 +289,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -565,22 +577,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" customWidth="1"/>
-    <col min="2" max="2" width="25.109375" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" customWidth="1"/>
+    <col min="1" max="1" width="17.75" customWidth="1"/>
+    <col min="2" max="2" width="25.125" customWidth="1"/>
+    <col min="3" max="3" width="23.125" customWidth="1"/>
+    <col min="4" max="4" width="21.5" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="21.77734375" customWidth="1"/>
-    <col min="7" max="8" width="19.44140625" customWidth="1"/>
+    <col min="6" max="6" width="21.75" customWidth="1"/>
+    <col min="7" max="8" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="25.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:18" ht="25.5" x14ac:dyDescent="0.3">
       <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
@@ -594,7 +606,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
@@ -602,7 +614,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
         <v>16</v>
       </c>
@@ -610,7 +622,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
@@ -618,7 +630,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -648,7 +660,7 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
@@ -672,7 +684,7 @@
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
@@ -682,7 +694,9 @@
       <c r="C8" s="9">
         <v>1</v>
       </c>
-      <c r="D8" s="5"/>
+      <c r="D8" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
@@ -698,7 +712,7 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
     </row>
-    <row r="9" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A9" s="11" t="s">
         <v>17</v>
       </c>
@@ -722,7 +736,7 @@
       </c>
       <c r="H9" s="12"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A12" s="7" t="s">
         <v>0</v>
       </c>
@@ -730,7 +744,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A13" s="7" t="s">
         <v>16</v>
       </c>
@@ -738,7 +752,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A14" s="7" t="s">
         <v>9</v>
       </c>
@@ -746,7 +760,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
@@ -776,7 +790,7 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -784,7 +798,9 @@
         <v>18</v>
       </c>
       <c r="C16" s="10"/>
-      <c r="D16" s="3"/>
+      <c r="D16" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
@@ -800,7 +816,7 @@
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A17" s="4" t="s">
         <v>7</v>
       </c>
@@ -808,7 +824,9 @@
         <v>19</v>
       </c>
       <c r="C17" s="9"/>
-      <c r="D17" s="5"/>
+      <c r="D17" s="5" t="s">
+        <v>35</v>
+      </c>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
@@ -824,7 +842,7 @@
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
     </row>
-    <row r="18" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A18" s="11" t="s">
         <v>17</v>
       </c>
@@ -840,7 +858,7 @@
       <c r="G18" s="12"/>
       <c r="H18" s="12"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A21" s="7" t="s">
         <v>0</v>
       </c>
@@ -848,7 +866,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A22" s="7" t="s">
         <v>16</v>
       </c>
@@ -856,7 +874,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A23" s="7" t="s">
         <v>9</v>
       </c>
@@ -864,7 +882,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
         <v>6</v>
       </c>
@@ -894,7 +912,7 @@
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A25" s="2" t="s">
         <v>14</v>
       </c>
@@ -916,7 +934,7 @@
       <c r="Q25" s="2"/>
       <c r="R25" s="2"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A26" s="4" t="s">
         <v>7</v>
       </c>
@@ -942,7 +960,7 @@
       <c r="Q26" s="4"/>
       <c r="R26" s="4"/>
     </row>
-    <row r="27" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A27" s="11" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
check-in: update the zhongshu_wangge.xlsx 20201127
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30690" windowHeight="11850"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30696" windowHeight="11856"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="38">
   <si>
     <t>交易品种：</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -161,13 +161,17 @@
   </si>
   <si>
     <t>1.061/1.112</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.384/1.400</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0_);\(0\)"/>
   </numFmts>
@@ -289,7 +293,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -578,21 +582,21 @@
   <dimension ref="A1:R27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.75" customWidth="1"/>
-    <col min="2" max="2" width="25.125" customWidth="1"/>
-    <col min="3" max="3" width="23.125" customWidth="1"/>
-    <col min="4" max="4" width="21.5" customWidth="1"/>
+    <col min="1" max="1" width="17.77734375" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="21.75" customWidth="1"/>
-    <col min="7" max="8" width="19.5" customWidth="1"/>
+    <col min="6" max="6" width="21.77734375" customWidth="1"/>
+    <col min="7" max="8" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="25.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="25.8" x14ac:dyDescent="0.4">
       <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
@@ -606,7 +610,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
@@ -614,7 +618,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>16</v>
       </c>
@@ -622,7 +626,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
@@ -630,7 +634,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -660,7 +664,7 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
@@ -684,7 +688,7 @@
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
@@ -697,7 +701,9 @@
       <c r="D8" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="5"/>
+      <c r="E8" s="9">
+        <v>1</v>
+      </c>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
@@ -712,7 +718,7 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
     </row>
-    <row r="9" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>17</v>
       </c>
@@ -736,7 +742,7 @@
       </c>
       <c r="H9" s="12"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>0</v>
       </c>
@@ -744,7 +750,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>16</v>
       </c>
@@ -752,7 +758,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>9</v>
       </c>
@@ -760,7 +766,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
@@ -790,7 +796,7 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -816,7 +822,7 @@
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>7</v>
       </c>
@@ -842,23 +848,21 @@
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
     </row>
-    <row r="18" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="13">
-        <v>1</v>
-      </c>
+      <c r="C18" s="13"/>
       <c r="D18" s="12"/>
       <c r="E18" s="13"/>
       <c r="F18" s="12"/>
       <c r="G18" s="12"/>
       <c r="H18" s="12"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>0</v>
       </c>
@@ -866,7 +870,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>16</v>
       </c>
@@ -874,7 +878,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>9</v>
       </c>
@@ -882,7 +886,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>6</v>
       </c>
@@ -912,7 +916,7 @@
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>14</v>
       </c>
@@ -934,7 +938,7 @@
       <c r="Q25" s="2"/>
       <c r="R25" s="2"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>7</v>
       </c>
@@ -944,8 +948,12 @@
       <c r="C26" s="9">
         <v>1</v>
       </c>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
+      <c r="D26" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E26" s="9">
+        <v>1</v>
+      </c>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
@@ -960,7 +968,7 @@
       <c r="Q26" s="4"/>
       <c r="R26" s="4"/>
     </row>
-    <row r="27" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
check-in: update the zhongshu_wangge.xlsx 20201201
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -582,7 +582,7 @@
   <dimension ref="A1:R27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -731,15 +731,11 @@
       <c r="D9" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="13">
-        <v>1</v>
-      </c>
+      <c r="E9" s="13"/>
       <c r="F9" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="G9" s="13">
-        <v>1</v>
-      </c>
+      <c r="G9" s="13"/>
       <c r="H9" s="12"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
@@ -951,9 +947,7 @@
       <c r="D26" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E26" s="9">
-        <v>1</v>
-      </c>
+      <c r="E26" s="9"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>

</xml_diff>

<commit_message>
check-in: update the zhongshu_wangge.xlsx 20201202
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30696" windowHeight="11856"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30690" windowHeight="11850"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="33">
   <si>
     <t>交易品种：</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -60,10 +60,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>无</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>中枢1执行情况</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -92,18 +88,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>4.824/4.914</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>创业板50（159949）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>无</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1.022/1.104</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -120,10 +108,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1.107/1.12</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>科创50（588000）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -132,10 +116,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1.076/1.1000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1.430/1.445</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -144,34 +124,34 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1.416/1.424</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5.034/5.051</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>4.887/5.105</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>4.934/4.975</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1.061/1.112</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>1.384/1.400</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.097/1.103</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.026/5.074</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.120/5.154</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0_);\(0\)"/>
   </numFmts>
@@ -293,7 +273,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -581,22 +561,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" customWidth="1"/>
-    <col min="2" max="2" width="25.109375" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" customWidth="1"/>
+    <col min="1" max="1" width="17.75" customWidth="1"/>
+    <col min="2" max="2" width="25.125" customWidth="1"/>
+    <col min="3" max="3" width="23.125" customWidth="1"/>
+    <col min="4" max="4" width="21.5" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="21.77734375" customWidth="1"/>
-    <col min="7" max="8" width="19.44140625" customWidth="1"/>
+    <col min="6" max="6" width="21.75" customWidth="1"/>
+    <col min="7" max="8" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="25.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:18" ht="25.5" x14ac:dyDescent="0.3">
       <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
@@ -610,23 +590,23 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="B4" s="8">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
@@ -634,7 +614,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -645,10 +625,10 @@
         <v>8</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -664,12 +644,12 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="3"/>
@@ -688,18 +668,18 @@
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C8" s="9">
         <v>1</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E8" s="9">
         <v>1</v>
@@ -718,43 +698,41 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
     </row>
-    <row r="9" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A9" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C9" s="13">
         <v>1</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="E9" s="13"/>
-      <c r="F9" s="12" t="s">
-        <v>29</v>
-      </c>
+      <c r="F9" s="12"/>
       <c r="G9" s="13"/>
       <c r="H9" s="12"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A12" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A13" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="B13" s="8">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A14" s="7" t="s">
         <v>9</v>
       </c>
@@ -762,7 +740,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
@@ -773,10 +751,10 @@
         <v>8</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -792,16 +770,16 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="3" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
@@ -818,17 +796,15 @@
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A17" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="C17" s="9"/>
-      <c r="D17" s="5" t="s">
-        <v>35</v>
-      </c>
+      <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
@@ -844,12 +820,12 @@
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
     </row>
-    <row r="18" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A18" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C18" s="13"/>
       <c r="D18" s="12"/>
@@ -858,23 +834,23 @@
       <c r="G18" s="12"/>
       <c r="H18" s="12"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A21" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A22" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="B22" s="8">
+        <v>6100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A23" s="7" t="s">
         <v>9</v>
       </c>
@@ -882,7 +858,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
         <v>6</v>
       </c>
@@ -893,10 +869,10 @@
         <v>8</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
@@ -912,9 +888,9 @@
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A25" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="10"/>
@@ -934,18 +910,18 @@
       <c r="Q25" s="2"/>
       <c r="R25" s="2"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A26" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C26" s="9">
         <v>1</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="E26" s="9"/>
       <c r="F26" s="5"/>
@@ -962,28 +938,24 @@
       <c r="Q26" s="4"/>
       <c r="R26" s="4"/>
     </row>
-    <row r="27" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A27" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C27" s="13">
         <v>1</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E27" s="13">
         <v>1</v>
       </c>
-      <c r="F27" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="G27" s="13">
-        <v>1</v>
-      </c>
+      <c r="F27" s="12"/>
+      <c r="G27" s="13"/>
       <c r="H27" s="12"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
check-in: update the zhongshu_wangge.xlsx 20201203
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30690" windowHeight="11850"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30696" windowHeight="11856"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -151,7 +151,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0_);\(0\)"/>
   </numFmts>
@@ -273,7 +273,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -561,22 +561,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.75" customWidth="1"/>
-    <col min="2" max="2" width="25.125" customWidth="1"/>
-    <col min="3" max="3" width="23.125" customWidth="1"/>
-    <col min="4" max="4" width="21.5" customWidth="1"/>
+    <col min="1" max="1" width="17.77734375" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="21.75" customWidth="1"/>
-    <col min="7" max="8" width="19.5" customWidth="1"/>
+    <col min="6" max="6" width="21.77734375" customWidth="1"/>
+    <col min="7" max="8" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="25.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="25.8" x14ac:dyDescent="0.4">
       <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
@@ -590,7 +590,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
@@ -598,7 +598,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>15</v>
       </c>
@@ -606,7 +606,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
@@ -614,7 +614,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -644,7 +644,7 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
@@ -668,7 +668,7 @@
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
@@ -698,7 +698,7 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
     </row>
-    <row r="9" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>16</v>
       </c>
@@ -711,12 +711,14 @@
       <c r="D9" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="13"/>
+      <c r="E9" s="13">
+        <v>1</v>
+      </c>
       <c r="F9" s="12"/>
       <c r="G9" s="13"/>
       <c r="H9" s="12"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>0</v>
       </c>
@@ -724,7 +726,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>15</v>
       </c>
@@ -732,7 +734,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>9</v>
       </c>
@@ -740,7 +742,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
@@ -770,7 +772,7 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
@@ -796,7 +798,7 @@
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>7</v>
       </c>
@@ -820,21 +822,23 @@
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
     </row>
-    <row r="18" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>16</v>
       </c>
       <c r="B18" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="13"/>
+      <c r="C18" s="13">
+        <v>1</v>
+      </c>
       <c r="D18" s="12"/>
       <c r="E18" s="13"/>
       <c r="F18" s="12"/>
       <c r="G18" s="12"/>
       <c r="H18" s="12"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>0</v>
       </c>
@@ -842,7 +846,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>15</v>
       </c>
@@ -850,7 +854,7 @@
         <v>6100</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>9</v>
       </c>
@@ -858,7 +862,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>6</v>
       </c>
@@ -888,7 +892,7 @@
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>13</v>
       </c>
@@ -910,7 +914,7 @@
       <c r="Q25" s="2"/>
       <c r="R25" s="2"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>7</v>
       </c>
@@ -938,7 +942,7 @@
       <c r="Q26" s="4"/>
       <c r="R26" s="4"/>
     </row>
-    <row r="27" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
check-in: update the zhongshu_wangge.xlsx 20201204
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30690" windowHeight="11850"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30696" windowHeight="11856"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -155,7 +155,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0_);\(0\)"/>
   </numFmts>
@@ -277,7 +277,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -565,22 +565,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.75" customWidth="1"/>
-    <col min="2" max="2" width="25.125" customWidth="1"/>
-    <col min="3" max="3" width="23.125" customWidth="1"/>
-    <col min="4" max="4" width="21.5" customWidth="1"/>
+    <col min="1" max="1" width="17.77734375" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="21.75" customWidth="1"/>
-    <col min="7" max="8" width="19.5" customWidth="1"/>
+    <col min="6" max="6" width="21.77734375" customWidth="1"/>
+    <col min="7" max="8" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="25.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="25.8" x14ac:dyDescent="0.4">
       <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
@@ -594,7 +594,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
@@ -602,7 +602,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>15</v>
       </c>
@@ -610,7 +610,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
@@ -618,7 +618,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -648,7 +648,7 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
@@ -672,7 +672,7 @@
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
@@ -700,7 +700,7 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
     </row>
-    <row r="9" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>16</v>
       </c>
@@ -718,7 +718,7 @@
       <c r="G9" s="13"/>
       <c r="H9" s="12"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>0</v>
       </c>
@@ -726,7 +726,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>15</v>
       </c>
@@ -734,7 +734,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>9</v>
       </c>
@@ -742,7 +742,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
@@ -772,7 +772,7 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
@@ -798,7 +798,7 @@
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>7</v>
       </c>
@@ -822,7 +822,7 @@
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
     </row>
-    <row r="18" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>16</v>
       </c>
@@ -838,7 +838,7 @@
       <c r="G18" s="12"/>
       <c r="H18" s="12"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>0</v>
       </c>
@@ -846,7 +846,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>15</v>
       </c>
@@ -854,7 +854,7 @@
         <v>6100</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>9</v>
       </c>
@@ -862,7 +862,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>6</v>
       </c>
@@ -892,7 +892,7 @@
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>13</v>
       </c>
@@ -914,7 +914,7 @@
       <c r="Q25" s="2"/>
       <c r="R25" s="2"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>7</v>
       </c>
@@ -942,7 +942,7 @@
       <c r="Q26" s="4"/>
       <c r="R26" s="4"/>
     </row>
-    <row r="27" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>16</v>
       </c>
@@ -961,7 +961,9 @@
       <c r="F27" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="G27" s="13"/>
+      <c r="G27" s="13">
+        <v>1</v>
+      </c>
       <c r="H27" s="12"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
check-in: update the zhongshu_wangge.xlsx 20201206
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -124,10 +124,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>4.887/5.105</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1.061/1.112</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -149,6 +145,10 @@
   </si>
   <si>
     <t>1.408/1.420</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.887/5.074</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -566,7 +566,7 @@
   <dimension ref="A1:R27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -683,7 +683,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="5"/>
@@ -711,7 +711,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E9" s="13"/>
       <c r="F9" s="12"/>
@@ -781,7 +781,7 @@
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="3" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
@@ -803,7 +803,7 @@
         <v>7</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C17" s="9"/>
       <c r="D17" s="5"/>
@@ -827,7 +827,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C18" s="13">
         <v>1</v>
@@ -925,7 +925,7 @@
         <v>1</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E26" s="9"/>
       <c r="F26" s="5"/>
@@ -959,7 +959,7 @@
         <v>1</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G27" s="13"/>
       <c r="H27" s="12"/>

</xml_diff>

<commit_message>
check-in: update the zhongshu_wangge.xlsx 20201207
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="36">
   <si>
     <t>交易品种：</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -149,6 +149,14 @@
   </si>
   <si>
     <t>4.887/5.074</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.080/5.147</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.095/5.121</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -566,7 +574,7 @@
   <dimension ref="A1:R27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -806,7 +814,9 @@
         <v>29</v>
       </c>
       <c r="C17" s="9"/>
-      <c r="D17" s="5"/>
+      <c r="D17" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
@@ -832,7 +842,9 @@
       <c r="C18" s="13">
         <v>1</v>
       </c>
-      <c r="D18" s="12"/>
+      <c r="D18" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="E18" s="13"/>
       <c r="F18" s="12"/>
       <c r="G18" s="12"/>

</xml_diff>

<commit_message>
check-in: update the zhongshu_wangge.xlsx 20201208
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="36">
   <si>
     <t>交易品种：</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -149,6 +149,14 @@
   </si>
   <si>
     <t>1.408/1.420</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pending</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pending</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -679,8 +687,8 @@
       <c r="B8" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="9">
-        <v>1</v>
+      <c r="C8" s="9" t="s">
+        <v>34</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>28</v>
@@ -707,8 +715,8 @@
       <c r="B9" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="13">
-        <v>1</v>
+      <c r="C9" s="13" t="s">
+        <v>35</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
check-in: update the zhongshu_wangge.xlsx 20201209
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30690" windowHeight="11850"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30696" windowHeight="11856"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -163,7 +163,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0_);\(0\)"/>
   </numFmts>
@@ -285,7 +285,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -573,22 +573,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.75" customWidth="1"/>
-    <col min="2" max="2" width="25.125" customWidth="1"/>
-    <col min="3" max="3" width="23.125" customWidth="1"/>
-    <col min="4" max="4" width="21.5" customWidth="1"/>
+    <col min="1" max="1" width="17.77734375" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="21.75" customWidth="1"/>
-    <col min="7" max="8" width="19.5" customWidth="1"/>
+    <col min="6" max="6" width="21.77734375" customWidth="1"/>
+    <col min="7" max="8" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="25.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="25.8" x14ac:dyDescent="0.4">
       <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
@@ -602,7 +602,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
@@ -610,7 +610,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>15</v>
       </c>
@@ -618,7 +618,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
@@ -626,7 +626,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -656,7 +656,7 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
@@ -680,14 +680,16 @@
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="9"/>
+      <c r="C8" s="9">
+        <v>1</v>
+      </c>
       <c r="D8" s="5" t="s">
         <v>28</v>
       </c>
@@ -706,14 +708,16 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
     </row>
-    <row r="9" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="13"/>
+      <c r="C9" s="13">
+        <v>1</v>
+      </c>
       <c r="D9" s="12" t="s">
         <v>32</v>
       </c>
@@ -722,7 +726,7 @@
       <c r="G9" s="13"/>
       <c r="H9" s="12"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>0</v>
       </c>
@@ -730,7 +734,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>15</v>
       </c>
@@ -738,7 +742,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>9</v>
       </c>
@@ -746,7 +750,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
@@ -776,7 +780,7 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
@@ -802,7 +806,7 @@
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>7</v>
       </c>
@@ -813,7 +817,9 @@
       <c r="D17" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E17" s="5"/>
+      <c r="E17" s="9">
+        <v>1</v>
+      </c>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
@@ -828,7 +834,7 @@
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
     </row>
-    <row r="18" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>16</v>
       </c>
@@ -844,7 +850,7 @@
       <c r="G18" s="12"/>
       <c r="H18" s="12"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>0</v>
       </c>
@@ -852,7 +858,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>15</v>
       </c>
@@ -860,7 +866,7 @@
         <v>6100</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>9</v>
       </c>
@@ -868,7 +874,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>6</v>
       </c>
@@ -898,7 +904,7 @@
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>13</v>
       </c>
@@ -922,7 +928,7 @@
       <c r="Q25" s="2"/>
       <c r="R25" s="2"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>7</v>
       </c>
@@ -950,7 +956,7 @@
       <c r="Q26" s="4"/>
       <c r="R26" s="4"/>
     </row>
-    <row r="27" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
check-in: update the zhongshu_wangge.xlsx 20201210
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -574,7 +574,7 @@
   <dimension ref="A1:R27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -813,7 +813,9 @@
       <c r="B17" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="9"/>
+      <c r="C17" s="9">
+        <v>1</v>
+      </c>
       <c r="D17" s="5" t="s">
         <v>34</v>
       </c>
@@ -911,7 +913,9 @@
       <c r="B25" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C25" s="10"/>
+      <c r="C25" s="10">
+        <v>1</v>
+      </c>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
@@ -941,7 +945,9 @@
       <c r="D26" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E26" s="9"/>
+      <c r="E26" s="9">
+        <v>1</v>
+      </c>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>

</xml_diff>

<commit_message>
check-in: update the zhongshu_wangge.xlsx 20201213
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30696" windowHeight="11856"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30690" windowHeight="11850"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="37">
   <si>
     <t>交易品种：</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -157,13 +157,17 @@
   </si>
   <si>
     <t>1.384/1.422</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.995/5.032</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0_);\(0\)"/>
   </numFmts>
@@ -285,7 +289,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -573,22 +577,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" customWidth="1"/>
-    <col min="2" max="2" width="25.109375" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" customWidth="1"/>
+    <col min="1" max="1" width="17.75" customWidth="1"/>
+    <col min="2" max="2" width="25.125" customWidth="1"/>
+    <col min="3" max="3" width="23.125" customWidth="1"/>
+    <col min="4" max="4" width="21.5" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="21.77734375" customWidth="1"/>
-    <col min="7" max="8" width="19.44140625" customWidth="1"/>
+    <col min="6" max="6" width="21.75" customWidth="1"/>
+    <col min="7" max="8" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="25.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:18" ht="25.5" x14ac:dyDescent="0.3">
       <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
@@ -602,7 +606,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
@@ -610,7 +614,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
         <v>15</v>
       </c>
@@ -618,7 +622,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
@@ -626,7 +630,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -656,7 +660,7 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
@@ -680,7 +684,7 @@
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
@@ -708,7 +712,7 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
     </row>
-    <row r="9" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A9" s="11" t="s">
         <v>16</v>
       </c>
@@ -721,12 +725,14 @@
       <c r="D9" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="13"/>
+      <c r="E9" s="13">
+        <v>1</v>
+      </c>
       <c r="F9" s="12"/>
       <c r="G9" s="13"/>
       <c r="H9" s="12"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A12" s="7" t="s">
         <v>0</v>
       </c>
@@ -734,7 +740,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A13" s="7" t="s">
         <v>15</v>
       </c>
@@ -742,7 +748,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A14" s="7" t="s">
         <v>9</v>
       </c>
@@ -750,7 +756,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
@@ -780,7 +786,7 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
@@ -806,7 +812,7 @@
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A17" s="4" t="s">
         <v>7</v>
       </c>
@@ -836,7 +842,7 @@
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
     </row>
-    <row r="18" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A18" s="11" t="s">
         <v>16</v>
       </c>
@@ -846,13 +852,15 @@
       <c r="C18" s="13">
         <v>1</v>
       </c>
-      <c r="D18" s="12"/>
+      <c r="D18" s="12" t="s">
+        <v>36</v>
+      </c>
       <c r="E18" s="13"/>
       <c r="F18" s="12"/>
       <c r="G18" s="12"/>
       <c r="H18" s="12"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A21" s="7" t="s">
         <v>0</v>
       </c>
@@ -860,7 +868,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A22" s="7" t="s">
         <v>15</v>
       </c>
@@ -868,7 +876,7 @@
         <v>6100</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A23" s="7" t="s">
         <v>9</v>
       </c>
@@ -876,7 +884,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
         <v>6</v>
       </c>
@@ -906,7 +914,7 @@
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A25" s="2" t="s">
         <v>13</v>
       </c>
@@ -932,7 +940,7 @@
       <c r="Q25" s="2"/>
       <c r="R25" s="2"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A26" s="4" t="s">
         <v>7</v>
       </c>
@@ -962,7 +970,7 @@
       <c r="Q26" s="4"/>
       <c r="R26" s="4"/>
     </row>
-    <row r="27" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A27" s="11" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
check-in: update the zhongshu_wangge.xlsx 20201217
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30690" windowHeight="11850"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30696" windowHeight="11856"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -167,7 +167,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0_);\(0\)"/>
   </numFmts>
@@ -289,7 +289,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -577,22 +577,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.75" customWidth="1"/>
-    <col min="2" max="2" width="25.125" customWidth="1"/>
-    <col min="3" max="3" width="23.125" customWidth="1"/>
-    <col min="4" max="4" width="21.5" customWidth="1"/>
+    <col min="1" max="1" width="17.77734375" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="21.75" customWidth="1"/>
-    <col min="7" max="8" width="19.5" customWidth="1"/>
+    <col min="6" max="6" width="21.77734375" customWidth="1"/>
+    <col min="7" max="8" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="25.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="25.8" x14ac:dyDescent="0.4">
       <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
@@ -606,7 +606,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
@@ -614,7 +614,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>15</v>
       </c>
@@ -622,7 +622,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
@@ -630,7 +630,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -660,7 +660,7 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
@@ -684,16 +684,14 @@
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="9">
-        <v>1</v>
-      </c>
+      <c r="C8" s="9"/>
       <c r="D8" s="5" t="s">
         <v>28</v>
       </c>
@@ -712,7 +710,7 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
     </row>
-    <row r="9" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>16</v>
       </c>
@@ -725,14 +723,12 @@
       <c r="D9" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="13">
-        <v>1</v>
-      </c>
+      <c r="E9" s="13"/>
       <c r="F9" s="12"/>
       <c r="G9" s="13"/>
       <c r="H9" s="12"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>0</v>
       </c>
@@ -740,7 +736,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>15</v>
       </c>
@@ -748,7 +744,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>9</v>
       </c>
@@ -756,7 +752,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
@@ -786,7 +782,7 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
@@ -812,7 +808,7 @@
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>7</v>
       </c>
@@ -825,9 +821,7 @@
       <c r="D17" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E17" s="9">
-        <v>1</v>
-      </c>
+      <c r="E17" s="9"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
@@ -842,7 +836,7 @@
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
     </row>
-    <row r="18" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>16</v>
       </c>
@@ -860,7 +854,7 @@
       <c r="G18" s="12"/>
       <c r="H18" s="12"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>0</v>
       </c>
@@ -868,7 +862,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>15</v>
       </c>
@@ -876,7 +870,7 @@
         <v>6100</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>9</v>
       </c>
@@ -884,7 +878,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>6</v>
       </c>
@@ -914,7 +908,7 @@
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>13</v>
       </c>
@@ -940,7 +934,7 @@
       <c r="Q25" s="2"/>
       <c r="R25" s="2"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>7</v>
       </c>
@@ -953,9 +947,7 @@
       <c r="D26" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E26" s="9">
-        <v>1</v>
-      </c>
+      <c r="E26" s="9"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
@@ -970,7 +962,7 @@
       <c r="Q26" s="4"/>
       <c r="R26" s="4"/>
     </row>
-    <row r="27" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
check-in: update the zhongshu_wangge.xlsx 20201223
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30696" windowHeight="11856"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30690" windowHeight="11850"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="42">
   <si>
     <t>交易品种：</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -84,59 +84,67 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>创业板50（159949）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.022/1.104</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>300ETF（510300）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.114/1.150</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>科创50（588000）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.452/1.464</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.430/1.445</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.061/1.112</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.384/1.400</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.026/5.074</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.408/1.420</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.080/5.147</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.384/1.422</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.150/1.165</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>4.622/4.863</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>创业板50（159949）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.022/1.104</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>300ETF（510300）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.139/1.161</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.114/1.150</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>科创50（588000）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.452/1.464</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.430/1.445</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.416/1.444</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4.887/5.105</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.061/1.112</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.384/1.400</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5.026/5.074</t>
+    <t>4.918/5.074</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -144,30 +152,42 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1.106/1.117</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.408/1.420</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5.080/5.147</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.384/1.422</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4.995/5.032</t>
+    <t>5.043/5.071</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.412/1.444</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>证券ETF（512880）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.163/1.279</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.163/1.201</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.203/1.236</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.156/1.166</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.172/1.181</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0_);\(0\)"/>
   </numFmts>
@@ -289,7 +309,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -575,24 +595,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R27"/>
+  <dimension ref="A1:R36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" customWidth="1"/>
-    <col min="2" max="2" width="25.109375" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" customWidth="1"/>
+    <col min="1" max="1" width="17.75" customWidth="1"/>
+    <col min="2" max="2" width="25.125" customWidth="1"/>
+    <col min="3" max="3" width="23.125" customWidth="1"/>
+    <col min="4" max="4" width="21.5" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="21.77734375" customWidth="1"/>
-    <col min="7" max="8" width="19.44140625" customWidth="1"/>
+    <col min="6" max="6" width="21.75" customWidth="1"/>
+    <col min="7" max="8" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="25.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:18" ht="25.5" x14ac:dyDescent="0.3">
       <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
@@ -606,15 +626,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
         <v>15</v>
       </c>
@@ -622,7 +642,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
@@ -630,7 +650,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -660,12 +680,12 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="3"/>
@@ -684,16 +704,16 @@
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="5"/>
@@ -710,33 +730,29 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
     </row>
-    <row r="9" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A9" s="11" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="13">
-        <v>1</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>32</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="C9" s="13"/>
+      <c r="D9" s="12"/>
       <c r="E9" s="13"/>
       <c r="F9" s="12"/>
       <c r="G9" s="13"/>
       <c r="H9" s="12"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A12" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A13" s="7" t="s">
         <v>15</v>
       </c>
@@ -744,7 +760,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A14" s="7" t="s">
         <v>9</v>
       </c>
@@ -752,7 +768,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
@@ -782,16 +798,16 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="3" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
@@ -808,16 +824,16 @@
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A17" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C17" s="9"/>
       <c r="D17" s="5" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E17" s="9">
         <v>1</v>
@@ -836,33 +852,33 @@
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
     </row>
-    <row r="18" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A18" s="11" t="s">
         <v>16</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C18" s="13">
         <v>1</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E18" s="13"/>
       <c r="F18" s="12"/>
       <c r="G18" s="12"/>
       <c r="H18" s="12"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A21" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A22" s="7" t="s">
         <v>15</v>
       </c>
@@ -870,7 +886,7 @@
         <v>6100</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A23" s="7" t="s">
         <v>9</v>
       </c>
@@ -878,7 +894,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
         <v>6</v>
       </c>
@@ -908,16 +924,14 @@
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A25" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C25" s="10">
-        <v>1</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="C25" s="10"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
@@ -934,18 +948,18 @@
       <c r="Q25" s="2"/>
       <c r="R25" s="2"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A26" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="C26" s="9">
         <v>1</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E26" s="9"/>
       <c r="F26" s="5"/>
@@ -962,29 +976,157 @@
       <c r="Q26" s="4"/>
       <c r="R26" s="4"/>
     </row>
-    <row r="27" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A27" s="11" t="s">
         <v>16</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C27" s="13">
         <v>1</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E27" s="13">
         <v>1</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="G27" s="13">
         <v>1</v>
       </c>
       <c r="H27" s="12"/>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A30" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A31" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B31" s="8">
+        <v>7800</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A32" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A33" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
+      <c r="O33" s="1"/>
+      <c r="P33" s="1"/>
+      <c r="Q33" s="1"/>
+      <c r="R33" s="1"/>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A34" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C34" s="10"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
+      <c r="O34" s="2"/>
+      <c r="P34" s="2"/>
+      <c r="Q34" s="2"/>
+      <c r="R34" s="2"/>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A35" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C35" s="9">
+        <v>1</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E35" s="9">
+        <v>1</v>
+      </c>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="4"/>
+      <c r="L35" s="4"/>
+      <c r="M35" s="4"/>
+      <c r="N35" s="4"/>
+      <c r="O35" s="4"/>
+      <c r="P35" s="4"/>
+      <c r="Q35" s="4"/>
+      <c r="R35" s="4"/>
+    </row>
+    <row r="36" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C36" s="13">
+        <v>1</v>
+      </c>
+      <c r="D36" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E36" s="13">
+        <v>1</v>
+      </c>
+      <c r="F36" s="12"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="12"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
check-in: update the zhongshu_wangge.xlsx for 2021, come on
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="40">
   <si>
     <t>交易品种：</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -96,31 +96,67 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>科创50（588000）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.026/5.074</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.384/1.422</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.622/4.863</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.918/5.074</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.412/1.444</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>证券ETF（512880）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.163/1.279</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.163/1.201</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.203/1.236</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.156/1.166</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.172/1.181</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.169/1.201</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>1.114/1.150</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>科创50（588000）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.452/1.464</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.430/1.445</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.061/1.112</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.384/1.400</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5.026/5.074</t>
+    <t>1.221/1.250</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.176/1.199</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -128,59 +164,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>5.080/5.147</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.384/1.422</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.150/1.165</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4.622/4.863</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4.918/5.074</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5.120/5.154</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5.043/5.071</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.412/1.444</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>证券ETF（512880）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.163/1.279</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.163/1.201</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.203/1.236</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.156/1.166</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.172/1.181</t>
+    <t>5.080/5.121</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.112/5.152</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.043/5.097</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -597,8 +589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38:E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -709,11 +701,11 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="5" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="5"/>
@@ -735,10 +727,12 @@
         <v>16</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C9" s="13"/>
-      <c r="D9" s="12"/>
+      <c r="D9" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="E9" s="13"/>
       <c r="F9" s="12"/>
       <c r="G9" s="13"/>
@@ -803,11 +797,11 @@
         <v>13</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
@@ -829,15 +823,13 @@
         <v>7</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C17" s="9"/>
       <c r="D17" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E17" s="9">
-        <v>1</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="E17" s="9"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
@@ -857,13 +849,11 @@
         <v>16</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" s="13">
-        <v>1</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="C18" s="13"/>
       <c r="D18" s="12" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E18" s="13"/>
       <c r="F18" s="12"/>
@@ -875,7 +865,7 @@
         <v>0</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.15">
@@ -929,7 +919,7 @@
         <v>13</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C25" s="10"/>
       <c r="D25" s="3"/>
@@ -953,14 +943,10 @@
         <v>7</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C26" s="9">
-        <v>1</v>
-      </c>
-      <c r="D26" s="5" t="s">
         <v>25</v>
       </c>
+      <c r="C26" s="9"/>
+      <c r="D26" s="5"/>
       <c r="E26" s="9"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
@@ -981,23 +967,13 @@
         <v>16</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C27" s="13">
-        <v>1</v>
-      </c>
-      <c r="D27" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E27" s="13">
-        <v>1</v>
-      </c>
-      <c r="F27" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="G27" s="13">
-        <v>1</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="C27" s="13"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="13"/>
       <c r="H27" s="12"/>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.15">
@@ -1005,7 +981,7 @@
         <v>0</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.15">
@@ -1059,7 +1035,7 @@
         <v>13</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="C34" s="10"/>
       <c r="D34" s="3"/>
@@ -1083,17 +1059,13 @@
         <v>7</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C35" s="9">
-        <v>1</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="C35" s="9"/>
       <c r="D35" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E35" s="9">
-        <v>1</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="E35" s="9"/>
       <c r="F35" s="5"/>
       <c r="G35" s="5"/>
       <c r="H35" s="5"/>
@@ -1113,17 +1085,13 @@
         <v>16</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="C36" s="13">
-        <v>1</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="C36" s="13"/>
       <c r="D36" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="E36" s="13">
-        <v>1</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="E36" s="13"/>
       <c r="F36" s="12"/>
       <c r="G36" s="13"/>
       <c r="H36" s="12"/>

</xml_diff>

<commit_message>
check-in: update the zhongshu_wangge.xlsx 20210105
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="49">
   <si>
     <t>交易品种：</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -136,10 +136,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1.156/1.166</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1.172/1.181</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -156,10 +152,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1.176/1.199</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1.408/1.420</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -172,7 +164,51 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>5.043/5.097</t>
+    <t>生物医药ETF（512290）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.832/1.942</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.890/1.944</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.910/1.923</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.055/1.128</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>银行ETF（512800）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.104/1.125</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.095/1.109</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.287/1.300</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.305/5.366</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.452/1.469</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.206/1.232</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -587,10 +623,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R36"/>
+  <dimension ref="A1:R54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38:E39"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -701,11 +737,11 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="5"/>
@@ -727,11 +763,11 @@
         <v>16</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C9" s="13"/>
       <c r="D9" s="12" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="E9" s="13"/>
       <c r="F9" s="12"/>
@@ -827,7 +863,7 @@
       </c>
       <c r="C17" s="9"/>
       <c r="D17" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E17" s="9"/>
       <c r="F17" s="5"/>
@@ -849,11 +885,11 @@
         <v>16</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C18" s="13"/>
       <c r="D18" s="12" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="E18" s="13"/>
       <c r="F18" s="12"/>
@@ -967,10 +1003,12 @@
         <v>16</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C27" s="13"/>
-      <c r="D27" s="12"/>
+      <c r="D27" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="E27" s="13"/>
       <c r="F27" s="12"/>
       <c r="G27" s="13"/>
@@ -1085,16 +1123,248 @@
         <v>16</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="C36" s="13"/>
       <c r="D36" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E36" s="13"/>
       <c r="F36" s="12"/>
       <c r="G36" s="13"/>
       <c r="H36" s="12"/>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A39" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A40" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B40" s="8">
+        <v>4600</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A41" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A42" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+      <c r="K42" s="1"/>
+      <c r="L42" s="1"/>
+      <c r="M42" s="1"/>
+      <c r="N42" s="1"/>
+      <c r="O42" s="1"/>
+      <c r="P42" s="1"/>
+      <c r="Q42" s="1"/>
+      <c r="R42" s="1"/>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A43" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C43" s="10"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+      <c r="L43" s="2"/>
+      <c r="M43" s="2"/>
+      <c r="N43" s="2"/>
+      <c r="O43" s="2"/>
+      <c r="P43" s="2"/>
+      <c r="Q43" s="2"/>
+      <c r="R43" s="2"/>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A44" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C44" s="9"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="9"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="5"/>
+      <c r="H44" s="5"/>
+      <c r="I44" s="4"/>
+      <c r="J44" s="4"/>
+      <c r="K44" s="4"/>
+      <c r="L44" s="4"/>
+      <c r="M44" s="4"/>
+      <c r="N44" s="4"/>
+      <c r="O44" s="4"/>
+      <c r="P44" s="4"/>
+      <c r="Q44" s="4"/>
+      <c r="R44" s="4"/>
+    </row>
+    <row r="45" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A45" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B45" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C45" s="13"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="12"/>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A48" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A49" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B49" s="8">
+        <v>7800</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A50" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A51" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
+      <c r="J51" s="1"/>
+      <c r="K51" s="1"/>
+      <c r="L51" s="1"/>
+      <c r="M51" s="1"/>
+      <c r="N51" s="1"/>
+      <c r="O51" s="1"/>
+      <c r="P51" s="1"/>
+      <c r="Q51" s="1"/>
+      <c r="R51" s="1"/>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A52" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C52" s="10"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3"/>
+      <c r="H52" s="3"/>
+      <c r="I52" s="2"/>
+      <c r="J52" s="2"/>
+      <c r="K52" s="2"/>
+      <c r="L52" s="2"/>
+      <c r="M52" s="2"/>
+      <c r="N52" s="2"/>
+      <c r="O52" s="2"/>
+      <c r="P52" s="2"/>
+      <c r="Q52" s="2"/>
+      <c r="R52" s="2"/>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A53" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C53" s="9"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="9"/>
+      <c r="F53" s="5"/>
+      <c r="G53" s="5"/>
+      <c r="H53" s="5"/>
+      <c r="I53" s="4"/>
+      <c r="J53" s="4"/>
+      <c r="K53" s="4"/>
+      <c r="L53" s="4"/>
+      <c r="M53" s="4"/>
+      <c r="N53" s="4"/>
+      <c r="O53" s="4"/>
+      <c r="P53" s="4"/>
+      <c r="Q53" s="4"/>
+      <c r="R53" s="4"/>
+    </row>
+    <row r="54" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A54" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B54" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C54" s="13"/>
+      <c r="D54" s="12"/>
+      <c r="E54" s="13"/>
+      <c r="F54" s="12"/>
+      <c r="G54" s="13"/>
+      <c r="H54" s="12"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
check-in: update the zhongshu_wangge.xlsx 20210203
</commit_message>
<xml_diff>
--- a/zhongshu_wangge.xlsx
+++ b/zhongshu_wangge.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30690" windowHeight="11850"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30696" windowHeight="11856"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -212,10 +212,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1.195/1.124</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>pending</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -253,13 +249,17 @@
   </si>
   <si>
     <t>pending</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.195/1.254</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0_);\(0\)"/>
   </numFmts>
@@ -381,7 +381,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -669,22 +669,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.75" customWidth="1"/>
-    <col min="2" max="2" width="25.125" customWidth="1"/>
-    <col min="3" max="3" width="23.125" customWidth="1"/>
-    <col min="4" max="4" width="21.5" customWidth="1"/>
+    <col min="1" max="1" width="17.77734375" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="21.75" customWidth="1"/>
-    <col min="7" max="8" width="19.5" customWidth="1"/>
+    <col min="6" max="6" width="21.77734375" customWidth="1"/>
+    <col min="7" max="8" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="25.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="25.8" x14ac:dyDescent="0.4">
       <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
@@ -698,7 +698,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
@@ -706,7 +706,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>15</v>
       </c>
@@ -714,7 +714,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
@@ -722,7 +722,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -752,7 +752,7 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
@@ -760,7 +760,7 @@
         <v>18</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
@@ -778,7 +778,7 @@
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
@@ -792,7 +792,7 @@
         <v>40</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
@@ -808,7 +808,7 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
     </row>
-    <row r="9" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>16</v>
       </c>
@@ -816,7 +816,7 @@
         <v>29</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="13"/>
@@ -824,7 +824,7 @@
       <c r="G9" s="13"/>
       <c r="H9" s="12"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>0</v>
       </c>
@@ -832,7 +832,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>15</v>
       </c>
@@ -840,7 +840,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>9</v>
       </c>
@@ -848,7 +848,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
@@ -878,7 +878,7 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
@@ -886,13 +886,13 @@
         <v>23</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>24</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
@@ -908,7 +908,7 @@
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>7</v>
       </c>
@@ -916,13 +916,13 @@
         <v>21</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>24</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
@@ -938,7 +938,7 @@
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
     </row>
-    <row r="18" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>16</v>
       </c>
@@ -946,7 +946,7 @@
         <v>31</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="13"/>
@@ -954,7 +954,7 @@
       <c r="G18" s="12"/>
       <c r="H18" s="12"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>0</v>
       </c>
@@ -962,7 +962,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>15</v>
       </c>
@@ -970,7 +970,7 @@
         <v>6100</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>9</v>
       </c>
@@ -978,7 +978,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>6</v>
       </c>
@@ -1008,7 +1008,7 @@
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>13</v>
       </c>
@@ -1016,7 +1016,7 @@
         <v>22</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
@@ -1034,7 +1034,7 @@
       <c r="Q25" s="2"/>
       <c r="R25" s="2"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>7</v>
       </c>
@@ -1042,7 +1042,7 @@
         <v>25</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>42</v>
@@ -1064,7 +1064,7 @@
       <c r="Q26" s="4"/>
       <c r="R26" s="4"/>
     </row>
-    <row r="27" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>16</v>
       </c>
@@ -1072,7 +1072,7 @@
         <v>30</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D27" s="12"/>
       <c r="E27" s="13"/>
@@ -1080,7 +1080,7 @@
       <c r="G27" s="13"/>
       <c r="H27" s="12"/>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>0</v>
       </c>
@@ -1088,7 +1088,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>15</v>
       </c>
@@ -1096,7 +1096,7 @@
         <v>7800</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>9</v>
       </c>
@@ -1104,7 +1104,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>6</v>
       </c>
@@ -1134,7 +1134,7 @@
       <c r="Q33" s="1"/>
       <c r="R33" s="1"/>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>13</v>
       </c>
@@ -1160,7 +1160,7 @@
       <c r="Q34" s="2"/>
       <c r="R34" s="2"/>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>7</v>
       </c>
@@ -1190,7 +1190,7 @@
       <c r="Q35" s="4"/>
       <c r="R35" s="4"/>
     </row>
-    <row r="36" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
         <v>16</v>
       </c>
@@ -1206,7 +1206,7 @@
       <c r="G36" s="13"/>
       <c r="H36" s="12"/>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>0</v>
       </c>
@@ -1214,7 +1214,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>15</v>
       </c>
@@ -1222,7 +1222,7 @@
         <v>4600</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>9</v>
       </c>
@@ -1230,7 +1230,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>6</v>
       </c>
@@ -1260,7 +1260,7 @@
       <c r="Q42" s="1"/>
       <c r="R42" s="1"/>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>13</v>
       </c>
@@ -1284,7 +1284,7 @@
       <c r="Q43" s="2"/>
       <c r="R43" s="2"/>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>7</v>
       </c>
@@ -1312,7 +1312,7 @@
       <c r="Q44" s="4"/>
       <c r="R44" s="4"/>
     </row>
-    <row r="45" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
         <v>16</v>
       </c>
@@ -1328,7 +1328,7 @@
       <c r="G45" s="13"/>
       <c r="H45" s="12"/>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
         <v>0</v>
       </c>
@@ -1336,7 +1336,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>15</v>
       </c>
@@ -1344,7 +1344,7 @@
         <v>7800</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
         <v>9</v>
       </c>
@@ -1352,7 +1352,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>6</v>
       </c>
@@ -1382,7 +1382,7 @@
       <c r="Q51" s="1"/>
       <c r="R51" s="1"/>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>13</v>
       </c>
@@ -1390,7 +1390,7 @@
         <v>35</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D52" s="3"/>
       <c r="E52" s="3"/>
@@ -1408,7 +1408,7 @@
       <c r="Q52" s="2"/>
       <c r="R52" s="2"/>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>7</v>
       </c>
@@ -1416,7 +1416,7 @@
         <v>37</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D53" s="5"/>
       <c r="E53" s="9"/>
@@ -1434,7 +1434,7 @@
       <c r="Q53" s="4"/>
       <c r="R53" s="4"/>
     </row>
-    <row r="54" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="11" t="s">
         <v>16</v>
       </c>
@@ -1442,7 +1442,7 @@
         <v>41</v>
       </c>
       <c r="C54" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D54" s="12"/>
       <c r="E54" s="13"/>
@@ -1450,7 +1450,7 @@
       <c r="G54" s="13"/>
       <c r="H54" s="12"/>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
         <v>0</v>
       </c>
@@ -1458,7 +1458,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
         <v>15</v>
       </c>
@@ -1466,7 +1466,7 @@
         <v>7800</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>9</v>
       </c>
@@ -1474,7 +1474,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>6</v>
       </c>
@@ -1504,12 +1504,12 @@
       <c r="Q60" s="1"/>
       <c r="R60" s="1"/>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="C61" s="10">
         <v>1</v>
@@ -1530,18 +1530,18 @@
       <c r="Q61" s="2"/>
       <c r="R61" s="2"/>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C62" s="9">
         <v>1</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E62" s="9">
         <v>1</v>
@@ -1560,7 +1560,7 @@
       <c r="Q62" s="4"/>
       <c r="R62" s="4"/>
     </row>
-    <row r="63" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="11" t="s">
         <v>16</v>
       </c>
@@ -1568,7 +1568,7 @@
         <v>41</v>
       </c>
       <c r="C63" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D63" s="12"/>
       <c r="E63" s="13"/>

</xml_diff>